<commit_message>
Calculated model parameters at more load points: 0.5, 1, 2, 3, 4, 5, 6 kW Added plot of engine life and battery life vs. load.
</commit_message>
<xml_diff>
--- a/Control and Data Systems/BMs Hygen System Design Calcs.xlsx
+++ b/Control and Data Systems/BMs Hygen System Design Calcs.xlsx
@@ -32,7 +32,7 @@
     <definedName name="Nominal_Energy">'Beckett Battery Modules'!$C$7</definedName>
     <definedName name="Nominal_Energy_Module">'Beckett Battery Modules'!$H$9</definedName>
     <definedName name="Nominal_Voltage">'Beckett Battery Modules'!$C$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Hygen Use Models'!$B$1:$G$87</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Hygen Use Models'!$B$1:$G$106</definedName>
     <definedName name="Stack_height">'Hygen Use Models'!$D$15</definedName>
     <definedName name="Voltage_at_0">'Beckett Battery Modules'!$B$11:$C$11</definedName>
     <definedName name="Voltage_at_100">'Beckett Battery Modules'!$B$14:$C$14</definedName>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="165">
   <si>
     <t>Boston Swing 5300</t>
   </si>
@@ -437,6 +437,108 @@
   </si>
   <si>
     <t>Bill Marty's analysis:</t>
+  </si>
+  <si>
+    <t>Battery C-rate w/ 0.5kW Tower Load</t>
+  </si>
+  <si>
+    <t>Battery C-rate w/ 1kW Tower Load</t>
+  </si>
+  <si>
+    <t>Battery C-rate w/ 3kW Tower Load</t>
+  </si>
+  <si>
+    <t>Battery C-rate w/ 5kW Tower Load</t>
+  </si>
+  <si>
+    <t>Engine on time to charge battery w/ 0.5kW Tower Load, h</t>
+  </si>
+  <si>
+    <t>Engine on time to charge battery w/ 1kW Tower Load, h</t>
+  </si>
+  <si>
+    <t>Engine on time to charge battery w/ 3kW Tower Load, h</t>
+  </si>
+  <si>
+    <t>Engine on time to charge battery w/ 5kW Tower Load, h</t>
+  </si>
+  <si>
+    <t>Tower run time on battery w/ 0.5kW Tower Load, h</t>
+  </si>
+  <si>
+    <t>Tower run time on battery w/ 1kW Tower Load, h</t>
+  </si>
+  <si>
+    <t>Tower run time on battery w/ 3kW Tower Load, h</t>
+  </si>
+  <si>
+    <t>Tower run time on battery w/ 5kW Tower Load, h</t>
+  </si>
+  <si>
+    <t>Cycle time w/ 0.5kW Tower Load, h</t>
+  </si>
+  <si>
+    <t>Cycle time w/ 1kW Tower Load, h</t>
+  </si>
+  <si>
+    <t>Cycle time w/ 3kW Tower Load, h</t>
+  </si>
+  <si>
+    <t>Cycle time w/ 5kW Tower Load, h</t>
+  </si>
+  <si>
+    <t>Engine duty cycle w/ 0.5kW Tower Load, %</t>
+  </si>
+  <si>
+    <t>Engine duty cycle w/ 1kW Tower Load, %</t>
+  </si>
+  <si>
+    <t>Engine duty cycle w/ 3kW Tower Load, %</t>
+  </si>
+  <si>
+    <t>Engine duty cycle w/ 5kW Tower Load, %</t>
+  </si>
+  <si>
+    <t>Engine life in years w/ 0.5kW Tower Load, y</t>
+  </si>
+  <si>
+    <t>Engine life in years w/ 1kW Tower Load, y</t>
+  </si>
+  <si>
+    <t>Engine life in years w/ 3kW Tower Load, y</t>
+  </si>
+  <si>
+    <t>Engine life in years w/ 5kW Tower Load, y</t>
+  </si>
+  <si>
+    <t>Battery life in years w/ 0.5kW Tower Load, y</t>
+  </si>
+  <si>
+    <t>Battery life in years w/ 1kW Tower Load, y</t>
+  </si>
+  <si>
+    <t>Battery life in years w/ 3kW Tower Load, y</t>
+  </si>
+  <si>
+    <t>Battery life in years w/ 5kW Tower Load, y</t>
+  </si>
+  <si>
+    <t>Engine maintenance interval w/ 0.5kW T.L., d</t>
+  </si>
+  <si>
+    <t>Engine maintenance interval w/ 1kW T.L., d</t>
+  </si>
+  <si>
+    <t>Engine maintenance interval w/ 3kW T.L., d</t>
+  </si>
+  <si>
+    <t>Engine maintenance interval w/ 5kW T.L., d</t>
+  </si>
+  <si>
+    <t>SFC, l/kWh</t>
+  </si>
+  <si>
+    <t>Fuel Tank Capacity, l</t>
   </si>
 </sst>
 </file>
@@ -470,7 +572,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,6 +597,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -509,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -544,9 +658,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -558,6 +669,18 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,6 +690,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF99"/>
       <color rgb="FFFF9999"/>
     </mruColors>
   </colors>
@@ -576,6 +700,261 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Engine Life in Years</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$D$102:$D$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$G$102:$G$108</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>23.440642431601713</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.675259932455509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7925686828824041</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8316715996913686</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8512230580958526</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.262953933138542</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8707745165003349</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Battery Life in Years</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$D$111:$D$117</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$G$111:$G$117</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10.159991169312509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5182233585799088</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.34253022359679</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.837825302119557</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9471866006451912</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.8705216300526137</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.2663659785740737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="80529664"/>
+        <c:axId val="80456320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="80529664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Customer Load, W </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80456320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="80456320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Years</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80529664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -622,6 +1001,36 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1299,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G87"/>
+  <dimension ref="B1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H108" sqref="H108:H109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,7 +1772,7 @@
         <v>125</v>
       </c>
       <c r="G16">
-        <v>250</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1382,6 +1791,12 @@
         <f>D17*Batt_bank_energy__kWh</f>
         <v>5.5</v>
       </c>
+      <c r="F18" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G18">
+        <v>0.38</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
@@ -1390,6 +1805,12 @@
       <c r="D19">
         <v>3000</v>
       </c>
+      <c r="F19" t="s">
+        <v>164</v>
+      </c>
+      <c r="G19">
+        <v>1000</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
@@ -1400,408 +1821,349 @@
         <v>7500</v>
       </c>
     </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+      <c r="D21" s="19"/>
+    </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="F23" s="1" t="s">
+    <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E27" s="4">
         <v>10.3</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F27" s="4">
         <v>15.3</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G27" s="4">
         <v>15.3</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-      <c r="C25" t="s">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E28" s="5">
         <v>0.7</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F28" s="5">
         <v>0.7</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G28" s="5">
         <v>0.59</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="6">
-        <f>E24*E25</f>
+      <c r="E29" s="6">
+        <f>E27*E28</f>
         <v>7.21</v>
       </c>
-      <c r="F26" s="6">
-        <f t="shared" ref="F26:G26" si="0">F24*F25</f>
+      <c r="F29" s="6">
+        <f t="shared" ref="F29:G29" si="0">F27*F28</f>
         <v>10.709999999999999</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G29" s="6">
         <f t="shared" si="0"/>
         <v>9.0269999999999992</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-      <c r="C27" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E30" s="5">
         <v>0.88</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F30" s="5">
         <v>0.88</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G30" s="5">
         <v>0.88</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C31" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="6">
-        <f>E27*E26</f>
+      <c r="E31" s="6">
+        <f>E30*E29</f>
         <v>6.3448000000000002</v>
       </c>
-      <c r="F28" s="6">
-        <f t="shared" ref="F28:G28" si="1">F27*F26</f>
+      <c r="F31" s="6">
+        <f t="shared" ref="F31:G31" si="1">F30*F29</f>
         <v>9.4247999999999994</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G31" s="6">
         <f t="shared" si="1"/>
         <v>7.9437599999999993</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
-      <c r="C29" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="F29" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="G29" s="5">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="9">
-        <f>E29*E28</f>
-        <v>6.0275600000000003</v>
-      </c>
-      <c r="F30" s="6">
-        <f t="shared" ref="F30:G30" si="2">F29*F28</f>
-        <v>8.9535599999999995</v>
-      </c>
-      <c r="G30" s="6">
-        <f t="shared" si="2"/>
-        <v>7.5465719999999994</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="F31" s="9">
-        <f>F30</f>
-        <v>8.9535599999999995</v>
-      </c>
-      <c r="G31" s="10">
-        <v>7.5</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E32" s="5">
-        <v>0.99</v>
+        <v>0.94</v>
       </c>
       <c r="F32" s="5">
-        <v>0.99</v>
+        <v>0.94</v>
       </c>
       <c r="G32" s="5">
-        <v>0.99</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="6">
-        <f>E32*E30</f>
-        <v>5.9672844000000005</v>
+        <v>60</v>
+      </c>
+      <c r="E33" s="9">
+        <f>E32*E31</f>
+        <v>5.9641120000000001</v>
       </c>
       <c r="F33" s="6">
-        <f>F32*F31</f>
-        <v>8.8640243999999999</v>
+        <f t="shared" ref="F33:G33" si="2">F32*F31</f>
+        <v>8.8593119999999992</v>
       </c>
       <c r="G33" s="6">
-        <f>G32*G31</f>
-        <v>7.4249999999999998</v>
+        <f t="shared" si="2"/>
+        <v>7.4671343999999991</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
+      <c r="B34" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="C34" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="F34" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="G34" s="5">
-        <v>0.95</v>
+        <v>61</v>
+      </c>
+      <c r="E34" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="F34" s="9">
+        <f>F33</f>
+        <v>8.8593119999999992</v>
+      </c>
+      <c r="G34" s="10">
+        <v>7.5</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
-        <v>67</v>
-      </c>
+      <c r="B35" s="4"/>
       <c r="C35" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="6">
-        <f>E34*E33</f>
-        <v>5.6689201800000006</v>
-      </c>
-      <c r="F35" s="6">
-        <f t="shared" ref="F35:G35" si="3">F34*F33</f>
-        <v>8.4208231799999993</v>
-      </c>
-      <c r="G35" s="6">
-        <f t="shared" si="3"/>
-        <v>7.0537499999999991</v>
+        <v>62</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0.99</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.99</v>
+      </c>
+      <c r="G35" s="5">
+        <v>0.99</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
-      </c>
-      <c r="E36" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="F36" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="G36" s="4">
-        <v>0.5</v>
+        <v>64</v>
+      </c>
+      <c r="E36" s="6">
+        <f>E35*E33</f>
+        <v>5.9044708799999999</v>
+      </c>
+      <c r="F36" s="6">
+        <f>F35*F34</f>
+        <v>8.7707188799999987</v>
+      </c>
+      <c r="G36" s="6">
+        <f>G35*G34</f>
+        <v>7.4249999999999998</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
       <c r="C37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="G37" s="5">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="6">
+        <f>E37*E36</f>
+        <v>5.6092473359999993</v>
+      </c>
+      <c r="F38" s="6">
+        <f t="shared" ref="F38:G38" si="3">F37*F36</f>
+        <v>8.3321829359999988</v>
+      </c>
+      <c r="G38" s="6">
+        <f t="shared" si="3"/>
+        <v>7.0537499999999991</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G39" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" t="s">
         <v>75</v>
       </c>
-      <c r="E37" s="5">
-        <f>E34</f>
+      <c r="E40" s="5">
+        <f>E37</f>
         <v>0.95</v>
       </c>
-      <c r="F37" s="5">
-        <f t="shared" ref="F37:G37" si="4">F34</f>
+      <c r="F40" s="5">
+        <f t="shared" ref="F40:G40" si="4">F37</f>
         <v>0.95</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G40" s="5">
         <f t="shared" si="4"/>
         <v>0.95</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C41" t="s">
         <v>70</v>
       </c>
-      <c r="E38" s="7">
-        <f>E36/E37</f>
+      <c r="E41" s="7">
+        <f>E39/E40</f>
         <v>0.52631578947368418</v>
       </c>
-      <c r="F38" s="7">
-        <f t="shared" ref="F38:G38" si="5">F36/F37</f>
+      <c r="F41" s="7">
+        <f t="shared" ref="F41:G41" si="5">F39/F40</f>
         <v>0.52631578947368418</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G41" s="7">
         <f t="shared" si="5"/>
         <v>0.52631578947368418</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C42" t="s">
         <v>72</v>
       </c>
-      <c r="E39" s="8">
-        <f>E35-E38</f>
-        <v>5.1426043905263166</v>
-      </c>
-      <c r="F39" s="8">
-        <f t="shared" ref="F39:G39" si="6">F35-F38</f>
-        <v>7.8945073905263152</v>
-      </c>
-      <c r="G39" s="8">
+      <c r="E42" s="8">
+        <f>E38-E41</f>
+        <v>5.0829315465263152</v>
+      </c>
+      <c r="F42" s="8">
+        <f t="shared" ref="F42:G42" si="6">F38-F41</f>
+        <v>7.8058671465263147</v>
+      </c>
+      <c r="G42" s="8">
         <f t="shared" si="6"/>
         <v>6.527434210526315</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="4"/>
-      <c r="C41" t="s">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" t="s">
         <v>130</v>
       </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
-      <c r="C42" s="1" t="s">
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="4">
-        <v>0</v>
-      </c>
-      <c r="E43" s="11">
-        <f>E$33-($D43+E$38)/E$34</f>
-        <v>5.4132677795013855</v>
-      </c>
-      <c r="F43" s="11">
-        <f t="shared" ref="F43:G46" si="7">F$33-($D43+F$38)/F$34</f>
-        <v>8.3100077795013849</v>
-      </c>
-      <c r="G43" s="11">
-        <f t="shared" si="7"/>
-        <v>6.8709833795013848</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" t="s">
-        <v>88</v>
-      </c>
-      <c r="D44" s="4">
-        <v>2</v>
-      </c>
-      <c r="E44" s="11">
-        <f t="shared" ref="E44:E46" si="8">E$33-($D44+E$38)/E$34</f>
-        <v>3.3080046216066488</v>
-      </c>
-      <c r="F44" s="11">
-        <f t="shared" si="7"/>
-        <v>6.2047446216066486</v>
-      </c>
-      <c r="G44" s="11">
-        <f t="shared" si="7"/>
-        <v>4.7657202216066477</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C45" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="4">
-        <v>4</v>
-      </c>
-      <c r="E45" s="11">
-        <f t="shared" si="8"/>
-        <v>1.202741463711912</v>
-      </c>
-      <c r="F45" s="11">
-        <f t="shared" si="7"/>
-        <v>4.0994814637119115</v>
-      </c>
-      <c r="G45" s="11">
-        <f t="shared" si="7"/>
-        <v>2.6604570637119114</v>
-      </c>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
@@ -1811,609 +2173,1363 @@
         <v>88</v>
       </c>
       <c r="D46" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E46" s="11">
-        <f t="shared" si="8"/>
-        <v>-0.90252169418282513</v>
+        <f>E$36-($D46+E$41)/E$37</f>
+        <v>5.3504542595013849</v>
       </c>
       <c r="F46" s="11">
-        <f t="shared" si="7"/>
-        <v>1.9942183058171743</v>
+        <f t="shared" ref="F46:G53" si="7">F$36-($D46+F$41)/F$37</f>
+        <v>8.2167022595013837</v>
       </c>
       <c r="G46" s="11">
         <f t="shared" si="7"/>
+        <v>6.8709833795013848</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="C47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E47" s="11">
+        <f t="shared" ref="E47:E48" si="8">E$36-($D47+E$41)/E$37</f>
+        <v>4.8241384700277008</v>
+      </c>
+      <c r="F47" s="11">
+        <f t="shared" si="7"/>
+        <v>7.6903864700276996</v>
+      </c>
+      <c r="G47" s="11">
+        <f t="shared" si="7"/>
+        <v>6.3446675900277008</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="4">
+        <v>1</v>
+      </c>
+      <c r="E48" s="11">
+        <f t="shared" si="8"/>
+        <v>4.2978226805540167</v>
+      </c>
+      <c r="F48" s="11">
+        <f t="shared" si="7"/>
+        <v>7.1640706805540155</v>
+      </c>
+      <c r="G48" s="11">
+        <f t="shared" si="7"/>
+        <v>5.8183518005540167</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="4">
+        <v>2</v>
+      </c>
+      <c r="E49" s="11">
+        <f t="shared" ref="E49:E53" si="9">E$36-($D49+E$41)/E$37</f>
+        <v>3.2451911016066481</v>
+      </c>
+      <c r="F49" s="11">
+        <f t="shared" si="7"/>
+        <v>6.1114391016066474</v>
+      </c>
+      <c r="G49" s="11">
+        <f t="shared" si="7"/>
+        <v>4.7657202216066477</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" s="4">
+        <v>3</v>
+      </c>
+      <c r="E50" s="11">
+        <f t="shared" si="9"/>
+        <v>2.1925595226592796</v>
+      </c>
+      <c r="F50" s="11">
+        <f t="shared" si="7"/>
+        <v>5.0588075226592784</v>
+      </c>
+      <c r="G50" s="11">
+        <f t="shared" si="7"/>
+        <v>3.7130886426592795</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="4"/>
+      <c r="C51" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="4">
+        <v>4</v>
+      </c>
+      <c r="E51" s="11">
+        <f t="shared" si="9"/>
+        <v>1.1399279437119114</v>
+      </c>
+      <c r="F51" s="11">
+        <f t="shared" si="7"/>
+        <v>4.0061759437119102</v>
+      </c>
+      <c r="G51" s="11">
+        <f t="shared" si="7"/>
+        <v>2.6604570637119114</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" s="4">
+        <v>5</v>
+      </c>
+      <c r="E52" s="11">
+        <f t="shared" si="9"/>
+        <v>8.7296364764542389E-2</v>
+      </c>
+      <c r="F52" s="11">
+        <f t="shared" si="7"/>
+        <v>2.9535443647645412</v>
+      </c>
+      <c r="G52" s="11">
+        <f t="shared" si="7"/>
+        <v>1.6078254847645423</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="C53" t="s">
+        <v>88</v>
+      </c>
+      <c r="D53" s="4">
+        <v>6</v>
+      </c>
+      <c r="E53" s="22">
+        <f t="shared" si="9"/>
+        <v>-0.96533521418282575</v>
+      </c>
+      <c r="F53" s="11">
+        <f t="shared" si="7"/>
+        <v>1.900912785817173</v>
+      </c>
+      <c r="G53" s="11">
+        <f t="shared" si="7"/>
         <v>0.5551939058171742</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="18" t="s">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C55" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="19">
-        <f t="shared" ref="E48:G51" si="9">E43/Batt_bank_energy__kWh</f>
-        <v>0.49211525268194412</v>
-      </c>
-      <c r="F48" s="19">
-        <f t="shared" si="9"/>
-        <v>0.75545525268194413</v>
-      </c>
-      <c r="G48" s="19">
-        <f t="shared" si="9"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="18">
+        <f>E46/Batt_bank_energy__kWh</f>
+        <v>0.48640493268194407</v>
+      </c>
+      <c r="F55" s="21">
+        <f>F46/Batt_bank_energy__kWh</f>
+        <v>0.74697293268194398</v>
+      </c>
+      <c r="G55" s="21">
+        <f>G46/Batt_bank_energy__kWh</f>
         <v>0.62463485268194407</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="18" t="s">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C56" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" s="17"/>
+      <c r="E56" s="18">
+        <f>E47/Batt_bank_energy__kWh</f>
+        <v>0.43855804272979099</v>
+      </c>
+      <c r="F56" s="21">
+        <f>F47/Batt_bank_energy__kWh</f>
+        <v>0.69912604272979084</v>
+      </c>
+      <c r="G56" s="21">
+        <f>G47/Batt_bank_energy__kWh</f>
+        <v>0.57678796272979094</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C57" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D57" s="17"/>
+      <c r="E57" s="18">
+        <f>E48/Batt_bank_energy__kWh</f>
+        <v>0.3907111527776379</v>
+      </c>
+      <c r="F57" s="21">
+        <f>F48/Batt_bank_energy__kWh</f>
+        <v>0.65127915277763782</v>
+      </c>
+      <c r="G57" s="21">
+        <f>G48/Batt_bank_energy__kWh</f>
+        <v>0.52894107277763791</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C58" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="18"/>
-      <c r="E49" s="19">
-        <f t="shared" si="9"/>
-        <v>0.30072769287333173</v>
-      </c>
-      <c r="F49" s="19">
-        <f t="shared" si="9"/>
-        <v>0.56406769287333169</v>
-      </c>
-      <c r="G49" s="19">
-        <f t="shared" si="9"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="18">
+        <f>E49/Batt_bank_energy__kWh</f>
+        <v>0.29501737287333163</v>
+      </c>
+      <c r="F58" s="21">
+        <f>F49/Batt_bank_energy__kWh</f>
+        <v>0.55558537287333154</v>
+      </c>
+      <c r="G58" s="18">
+        <f>G49/Batt_bank_energy__kWh</f>
         <v>0.43324729287333158</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C50" s="18" t="s">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C59" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D59" s="17"/>
+      <c r="E59" s="18">
+        <f>E50/Batt_bank_energy__kWh</f>
+        <v>0.19932359296902541</v>
+      </c>
+      <c r="F59" s="18">
+        <f>F50/Batt_bank_energy__kWh</f>
+        <v>0.45989159296902532</v>
+      </c>
+      <c r="G59" s="18">
+        <f>G50/Batt_bank_energy__kWh</f>
+        <v>0.33755351296902542</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C60" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D50" s="18"/>
-      <c r="E50" s="19">
-        <f t="shared" si="9"/>
-        <v>0.10934013306471928</v>
-      </c>
-      <c r="F50" s="19">
-        <f t="shared" si="9"/>
-        <v>0.3726801330647192</v>
-      </c>
-      <c r="G50" s="19">
-        <f t="shared" si="9"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="18">
+        <f>E51/Batt_bank_energy__kWh</f>
+        <v>0.10362981306471922</v>
+      </c>
+      <c r="F60" s="18">
+        <f>F51/Batt_bank_energy__kWh</f>
+        <v>0.3641978130647191</v>
+      </c>
+      <c r="G60" s="18">
+        <f>G51/Batt_bank_energy__kWh</f>
         <v>0.24185973306471922</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="18" t="s">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C61" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D61" s="17"/>
+      <c r="E61" s="18">
+        <f>E52/Batt_bank_energy__kWh</f>
+        <v>7.9360331604129437E-3</v>
+      </c>
+      <c r="F61" s="18">
+        <f>F52/Batt_bank_energy__kWh</f>
+        <v>0.26850403316041282</v>
+      </c>
+      <c r="G61" s="18">
+        <f>G52/Batt_bank_energy__kWh</f>
+        <v>0.14616595316041295</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C62" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D51" s="18"/>
-      <c r="E51" s="19">
-        <f t="shared" si="9"/>
-        <v>-8.204742674389319E-2</v>
-      </c>
-      <c r="F51" s="19">
-        <f t="shared" si="9"/>
-        <v>0.18129257325610676</v>
-      </c>
-      <c r="G51" s="19">
-        <f t="shared" si="9"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="21">
+        <f>E53/Batt_bank_energy__kWh</f>
+        <v>-8.775774674389325E-2</v>
+      </c>
+      <c r="F62" s="18">
+        <f>F53/Batt_bank_energy__kWh</f>
+        <v>0.17281025325610663</v>
+      </c>
+      <c r="G62" s="18">
+        <f>G53/Batt_bank_energy__kWh</f>
         <v>5.0472173256106749E-2</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>101</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C64" t="s">
         <v>93</v>
       </c>
-      <c r="E53" s="13">
-        <f t="shared" ref="E53:G56" si="10">1/E48*Depth_of_Discharge</f>
-        <v>1.0160221559382387</v>
-      </c>
-      <c r="F53" s="13">
+      <c r="E64" s="13">
+        <f>1/E55*Depth_of_Discharge</f>
+        <v>1.0279501016634336</v>
+      </c>
+      <c r="F64" s="13">
+        <f>1/F55*Depth_of_Discharge</f>
+        <v>0.66936829719490865</v>
+      </c>
+      <c r="G64" s="13">
+        <f>1/G55*Depth_of_Discharge</f>
+        <v>0.80046766179183004</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>135</v>
+      </c>
+      <c r="E65" s="13">
+        <f>1/E56*Depth_of_Discharge</f>
+        <v>1.1400999440980844</v>
+      </c>
+      <c r="F65" s="13">
+        <f>1/F56*Depth_of_Discharge</f>
+        <v>0.71517862222341477</v>
+      </c>
+      <c r="G65" s="13">
+        <f>1/G56*Depth_of_Discharge</f>
+        <v>0.86686968575701018</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>136</v>
+      </c>
+      <c r="E66" s="13">
+        <f>1/E57*Depth_of_Discharge</f>
+        <v>1.2797177568272813</v>
+      </c>
+      <c r="F66" s="13">
+        <f>1/F57*Depth_of_Discharge</f>
+        <v>0.76771995213965016</v>
+      </c>
+      <c r="G66" s="13">
+        <f>1/G57*Depth_of_Discharge</f>
+        <v>0.94528488282133372</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>94</v>
+      </c>
+      <c r="E67" s="13">
+        <f>1/E58*Depth_of_Discharge</f>
+        <v>1.6948154446981654</v>
+      </c>
+      <c r="F67" s="13">
+        <f>1/F58*Depth_of_Discharge</f>
+        <v>0.89995169853759904</v>
+      </c>
+      <c r="G67" s="13">
+        <f>1/G58*Depth_of_Discharge</f>
+        <v>1.1540753011610505</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>137</v>
+      </c>
+      <c r="E68" s="13">
+        <f>1/E59*Depth_of_Discharge</f>
+        <v>2.5084837803305065</v>
+      </c>
+      <c r="F68" s="13">
+        <f>1/F59*Depth_of_Discharge</f>
+        <v>1.0872127424031344</v>
+      </c>
+      <c r="G68" s="13">
+        <f>1/G59*Depth_of_Discharge</f>
+        <v>1.4812466195423095</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>95</v>
+      </c>
+      <c r="E69" s="13">
+        <f>1/E60*Depth_of_Discharge</f>
+        <v>4.8248663701413648</v>
+      </c>
+      <c r="F69" s="13">
+        <f>1/F60*Depth_of_Discharge</f>
+        <v>1.3728802921481256</v>
+      </c>
+      <c r="G69" s="13">
+        <f>1/G60*Depth_of_Discharge</f>
+        <v>2.0673139495535828</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>138</v>
+      </c>
+      <c r="E70" s="13">
+        <f>1/E61*Depth_of_Discharge</f>
+        <v>63.00376899811026</v>
+      </c>
+      <c r="F70" s="13">
+        <f>1/F61*Depth_of_Discharge</f>
+        <v>1.8621694211247999</v>
+      </c>
+      <c r="G70" s="13">
+        <f>1/G61*Depth_of_Discharge</f>
+        <v>3.4207692639014526</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>96</v>
+      </c>
+      <c r="E71" s="13">
+        <f>1/E62*Depth_of_Discharge</f>
+        <v>-5.697502711175674</v>
+      </c>
+      <c r="F71" s="13">
+        <f>1/F62*Depth_of_Discharge</f>
+        <v>2.8933468389690669</v>
+      </c>
+      <c r="G71" s="13">
+        <f>1/G62*Depth_of_Discharge</f>
+        <v>9.9064487963078509</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>102</v>
+      </c>
+      <c r="C73" t="s">
+        <v>97</v>
+      </c>
+      <c r="D73" s="4">
+        <v>0</v>
+      </c>
+      <c r="E73" s="13" t="e">
+        <f t="shared" ref="E73:G80" si="10">Cycle_energy__kWh/$D73</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F73" s="13" t="e">
         <f t="shared" si="10"/>
-        <v>0.66185256932816128</v>
-      </c>
-      <c r="G53" s="13">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G73" s="13" t="e">
         <f t="shared" si="10"/>
-        <v>0.80046766179183004</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>94</v>
-      </c>
-      <c r="E54" s="13">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>139</v>
+      </c>
+      <c r="D74" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E74" s="13">
         <f t="shared" si="10"/>
-        <v>1.6626337109918339</v>
-      </c>
-      <c r="F54" s="13">
+        <v>11</v>
+      </c>
+      <c r="F74" s="13">
         <f t="shared" si="10"/>
-        <v>0.8864184322506149</v>
-      </c>
-      <c r="G54" s="13">
+        <v>11</v>
+      </c>
+      <c r="G74" s="13">
         <f t="shared" si="10"/>
-        <v>1.1540753011610505</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>95</v>
-      </c>
-      <c r="E55" s="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>140</v>
+      </c>
+      <c r="D75" s="4">
+        <v>1</v>
+      </c>
+      <c r="E75" s="13">
         <f t="shared" si="10"/>
-        <v>4.5728863317190775</v>
-      </c>
-      <c r="F55" s="13">
+        <v>5.5</v>
+      </c>
+      <c r="F75" s="13">
         <f t="shared" si="10"/>
-        <v>1.3416330940108647</v>
-      </c>
-      <c r="G55" s="13">
+        <v>5.5</v>
+      </c>
+      <c r="G75" s="13">
         <f t="shared" si="10"/>
-        <v>2.0673139495535828</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
-        <v>96</v>
-      </c>
-      <c r="E56" s="13">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>98</v>
+      </c>
+      <c r="D76" s="4">
+        <v>2</v>
+      </c>
+      <c r="E76" s="13">
         <f t="shared" si="10"/>
-        <v>-6.0940363377967257</v>
-      </c>
-      <c r="F56" s="13">
+        <v>2.75</v>
+      </c>
+      <c r="F76" s="13">
         <f t="shared" si="10"/>
-        <v>2.7579728778721924</v>
-      </c>
-      <c r="G56" s="13">
+        <v>2.75</v>
+      </c>
+      <c r="G76" s="13">
         <f t="shared" si="10"/>
-        <v>9.9064487963078509</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>102</v>
-      </c>
-      <c r="C58" t="s">
-        <v>97</v>
-      </c>
-      <c r="D58" s="4">
-        <v>0</v>
-      </c>
-      <c r="E58" s="13" t="e">
-        <f t="shared" ref="E58:G61" si="11">Cycle_energy__kWh/$D58</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>141</v>
+      </c>
+      <c r="D77" s="4">
+        <v>3</v>
+      </c>
+      <c r="E77" s="13">
+        <f t="shared" si="10"/>
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="F77" s="13">
+        <f t="shared" si="10"/>
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="G77" s="13">
+        <f t="shared" si="10"/>
+        <v>1.8333333333333333</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>99</v>
+      </c>
+      <c r="D78" s="4">
+        <v>4</v>
+      </c>
+      <c r="E78" s="13">
+        <f t="shared" si="10"/>
+        <v>1.375</v>
+      </c>
+      <c r="F78" s="13">
+        <f t="shared" si="10"/>
+        <v>1.375</v>
+      </c>
+      <c r="G78" s="13">
+        <f t="shared" si="10"/>
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>142</v>
+      </c>
+      <c r="D79" s="4">
+        <v>5</v>
+      </c>
+      <c r="E79" s="13">
+        <f t="shared" si="10"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F79" s="13">
+        <f t="shared" si="10"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G79" s="13">
+        <f t="shared" si="10"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>100</v>
+      </c>
+      <c r="D80" s="4">
+        <v>6</v>
+      </c>
+      <c r="E80" s="13">
+        <f t="shared" si="10"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F80" s="13">
+        <f t="shared" si="10"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="G80" s="13">
+        <f t="shared" si="10"/>
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>103</v>
+      </c>
+      <c r="C82" t="s">
+        <v>104</v>
+      </c>
+      <c r="E82" s="7" t="e">
+        <f>E64+E73</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F58" s="13" t="e">
+      <c r="F82" s="7" t="e">
+        <f t="shared" ref="F82:G82" si="11">F64+F73</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G82" s="7" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G58" s="13" t="e">
-        <f t="shared" si="11"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>143</v>
+      </c>
+      <c r="E83" s="7">
+        <f t="shared" ref="E83:G83" si="12">E65+E74</f>
+        <v>12.140099944098084</v>
+      </c>
+      <c r="F83" s="7">
+        <f t="shared" si="12"/>
+        <v>11.715178622223414</v>
+      </c>
+      <c r="G83" s="7">
+        <f t="shared" si="12"/>
+        <v>11.86686968575701</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>144</v>
+      </c>
+      <c r="E84" s="7">
+        <f t="shared" ref="E84:G84" si="13">E66+E75</f>
+        <v>6.7797177568272815</v>
+      </c>
+      <c r="F84" s="7">
+        <f t="shared" si="13"/>
+        <v>6.2677199521396503</v>
+      </c>
+      <c r="G84" s="7">
+        <f t="shared" si="13"/>
+        <v>6.4452848828213334</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>105</v>
+      </c>
+      <c r="E85" s="7">
+        <f t="shared" ref="E85:G85" si="14">E67+E76</f>
+        <v>4.4448154446981656</v>
+      </c>
+      <c r="F85" s="7">
+        <f t="shared" si="14"/>
+        <v>3.649951698537599</v>
+      </c>
+      <c r="G85" s="7">
+        <f t="shared" si="14"/>
+        <v>3.9040753011610505</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>145</v>
+      </c>
+      <c r="E86" s="7">
+        <f t="shared" ref="E86:G86" si="15">E68+E77</f>
+        <v>4.3418171136638399</v>
+      </c>
+      <c r="F86" s="7">
+        <f t="shared" si="15"/>
+        <v>2.9205460757364676</v>
+      </c>
+      <c r="G86" s="7">
+        <f t="shared" si="15"/>
+        <v>3.3145799528756426</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>106</v>
+      </c>
+      <c r="E87" s="7">
+        <f t="shared" ref="E87:G87" si="16">E69+E78</f>
+        <v>6.1998663701413648</v>
+      </c>
+      <c r="F87" s="7">
+        <f t="shared" si="16"/>
+        <v>2.7478802921481256</v>
+      </c>
+      <c r="G87" s="7">
+        <f t="shared" si="16"/>
+        <v>3.4423139495535828</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>146</v>
+      </c>
+      <c r="E88" s="7">
+        <f t="shared" ref="E88:G88" si="17">E70+E79</f>
+        <v>64.103768998110255</v>
+      </c>
+      <c r="F88" s="7">
+        <f t="shared" si="17"/>
+        <v>2.9621694211248002</v>
+      </c>
+      <c r="G88" s="7">
+        <f t="shared" si="17"/>
+        <v>4.5207692639014532</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>107</v>
+      </c>
+      <c r="E89" s="7">
+        <f t="shared" ref="E89:G89" si="18">E71+E80</f>
+        <v>-4.780836044509007</v>
+      </c>
+      <c r="F89" s="7">
+        <f t="shared" si="18"/>
+        <v>3.8100135056357334</v>
+      </c>
+      <c r="G89" s="7">
+        <f t="shared" si="18"/>
+        <v>10.823115462974517</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>108</v>
+      </c>
+      <c r="E91" s="7" t="e">
+        <f>E64/E82</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
-        <v>98</v>
-      </c>
-      <c r="D59" s="4">
-        <v>2</v>
-      </c>
-      <c r="E59" s="13">
-        <f t="shared" si="11"/>
-        <v>2.75</v>
-      </c>
-      <c r="F59" s="13">
-        <f t="shared" si="11"/>
-        <v>2.75</v>
-      </c>
-      <c r="G59" s="13">
-        <f t="shared" si="11"/>
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
-        <v>99</v>
-      </c>
-      <c r="D60" s="4">
-        <v>4</v>
-      </c>
-      <c r="E60" s="13">
-        <f t="shared" si="11"/>
-        <v>1.375</v>
-      </c>
-      <c r="F60" s="13">
-        <f t="shared" si="11"/>
-        <v>1.375</v>
-      </c>
-      <c r="G60" s="13">
-        <f t="shared" si="11"/>
-        <v>1.375</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>100</v>
-      </c>
-      <c r="D61" s="4">
-        <v>6</v>
-      </c>
-      <c r="E61" s="13">
-        <f t="shared" si="11"/>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="F61" s="13">
-        <f t="shared" si="11"/>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="G61" s="13">
-        <f t="shared" si="11"/>
-        <v>0.91666666666666663</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>103</v>
-      </c>
-      <c r="C63" t="s">
-        <v>104</v>
-      </c>
-      <c r="E63" s="7" t="e">
-        <f>E53+E58</f>
+      <c r="F91" s="7" t="e">
+        <f>F64/F82</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F63" s="7" t="e">
-        <f t="shared" ref="F63:G63" si="12">F53+F58</f>
+      <c r="G91" s="7" t="e">
+        <f>G64/G82</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G63" s="7" t="e">
-        <f t="shared" si="12"/>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>147</v>
+      </c>
+      <c r="E92" s="7">
+        <f t="shared" ref="E92:G92" si="19">E65/E83</f>
+        <v>9.3911907591201049E-2</v>
+      </c>
+      <c r="F92" s="7">
+        <f t="shared" si="19"/>
+        <v>6.1047180353420986E-2</v>
+      </c>
+      <c r="G92" s="7">
+        <f t="shared" si="19"/>
+        <v>7.3049566457905446E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>148</v>
+      </c>
+      <c r="E93" s="7">
+        <f t="shared" ref="E93:G93" si="20">E66/E84</f>
+        <v>0.18875678940153306</v>
+      </c>
+      <c r="F93" s="7">
+        <f t="shared" si="20"/>
+        <v>0.12248791554216919</v>
+      </c>
+      <c r="G93" s="7">
+        <f t="shared" si="20"/>
+        <v>0.14666301024812861</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>109</v>
+      </c>
+      <c r="E94" s="7">
+        <f t="shared" ref="E94:G94" si="21">E67/E85</f>
+        <v>0.38130164588042986</v>
+      </c>
+      <c r="F94" s="7">
+        <f t="shared" si="21"/>
+        <v>0.2465653720563416</v>
+      </c>
+      <c r="G94" s="7">
+        <f t="shared" si="21"/>
+        <v>0.29560784875687074</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>149</v>
+      </c>
+      <c r="E95" s="7">
+        <f t="shared" ref="E95:G95" si="22">E68/E86</f>
+        <v>0.57774975653309446</v>
+      </c>
+      <c r="F95" s="7">
+        <f t="shared" si="22"/>
+        <v>0.37226351312706968</v>
+      </c>
+      <c r="G95" s="7">
+        <f t="shared" si="22"/>
+        <v>0.44688818510991685</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>110</v>
+      </c>
+      <c r="D96" s="20"/>
+      <c r="E96" s="7">
+        <f t="shared" ref="E96:G96" si="23">E69/E87</f>
+        <v>0.77822102640437263</v>
+      </c>
+      <c r="F96" s="7">
+        <f t="shared" si="23"/>
+        <v>0.49961430127470774</v>
+      </c>
+      <c r="G96" s="7">
+        <f t="shared" si="23"/>
+        <v>0.60055938530001973</v>
+      </c>
+    </row>
+    <row r="97" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>150</v>
+      </c>
+      <c r="D97" s="20"/>
+      <c r="E97" s="7">
+        <f t="shared" ref="E97:G97" si="24">E70/E88</f>
+        <v>0.98284032253965559</v>
+      </c>
+      <c r="F97" s="7">
+        <f t="shared" si="24"/>
+        <v>0.62865054505143514</v>
+      </c>
+      <c r="G97" s="7">
+        <f t="shared" si="24"/>
+        <v>0.756678579288806</v>
+      </c>
+    </row>
+    <row r="98" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>111</v>
+      </c>
+      <c r="D98" s="20"/>
+      <c r="E98" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F98" s="7">
+        <f t="shared" ref="F98:G98" si="25">F71/F89</f>
+        <v>0.759405927220273</v>
+      </c>
+      <c r="G98" s="7">
+        <f t="shared" si="25"/>
+        <v>0.9153047318212072</v>
+      </c>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D99" s="20"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7"/>
+      <c r="G99" s="7"/>
+    </row>
+    <row r="100" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D100" s="20"/>
+    </row>
+    <row r="101" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C101" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D101" s="14">
+        <v>0</v>
+      </c>
+      <c r="E101" s="15" t="e">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E91</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
-        <v>105</v>
-      </c>
-      <c r="E64" s="7">
-        <f t="shared" ref="E64:G64" si="13">E54+E59</f>
-        <v>4.4126337109918339</v>
-      </c>
-      <c r="F64" s="7">
-        <f t="shared" si="13"/>
-        <v>3.6364184322506148</v>
-      </c>
-      <c r="G64" s="7">
-        <f t="shared" si="13"/>
-        <v>3.9040753011610505</v>
-      </c>
-    </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
-        <v>106</v>
-      </c>
-      <c r="E65" s="7">
-        <f t="shared" ref="E65:G65" si="14">E55+E60</f>
-        <v>5.9478863317190775</v>
-      </c>
-      <c r="F65" s="7">
-        <f t="shared" si="14"/>
-        <v>2.7166330940108647</v>
-      </c>
-      <c r="G65" s="7">
-        <f t="shared" si="14"/>
-        <v>3.4423139495535828</v>
-      </c>
-    </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
-        <v>107</v>
-      </c>
-      <c r="E66" s="7">
-        <f t="shared" ref="E66:G66" si="15">E56+E61</f>
-        <v>-5.1773696711300587</v>
-      </c>
-      <c r="F66" s="7">
-        <f t="shared" si="15"/>
-        <v>3.6746395445388589</v>
-      </c>
-      <c r="G66" s="7">
-        <f t="shared" si="15"/>
-        <v>10.823115462974517</v>
-      </c>
-    </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
-        <v>108</v>
-      </c>
-      <c r="E68" s="7" t="e">
-        <f>E53/E63</f>
+      <c r="F101" s="15" t="e">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F91</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F68" s="7" t="e">
-        <f t="shared" ref="F68:G68" si="16">F53/F63</f>
+      <c r="G101" s="15" t="e">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G91</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G68" s="7" t="e">
-        <f t="shared" si="16"/>
+    </row>
+    <row r="102" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C102" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D102" s="23">
+        <v>500</v>
+      </c>
+      <c r="E102" s="24">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E92</f>
+        <v>18.233350924752401</v>
+      </c>
+      <c r="F102" s="24">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F92</f>
+        <v>28.049268732971569</v>
+      </c>
+      <c r="G102" s="24">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G92</f>
+        <v>23.440642431601713</v>
+      </c>
+    </row>
+    <row r="103" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C103" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="D103" s="23">
+        <v>1000</v>
+      </c>
+      <c r="E103" s="24">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E93</f>
+        <v>9.0716141790308509</v>
+      </c>
+      <c r="F103" s="24">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F93</f>
+        <v>13.979573083140437</v>
+      </c>
+      <c r="G103" s="24">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G93</f>
+        <v>11.675259932455509</v>
+      </c>
+    </row>
+    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C104" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D104" s="14">
+        <v>2000</v>
+      </c>
+      <c r="E104" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E94</f>
+        <v>4.4907458061700751</v>
+      </c>
+      <c r="F104" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F94</f>
+        <v>6.9447252582248682</v>
+      </c>
+      <c r="G104" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G94</f>
+        <v>5.7925686828824041</v>
+      </c>
+    </row>
+    <row r="105" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C105" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D105" s="14">
+        <v>3000</v>
+      </c>
+      <c r="E105" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E95</f>
+        <v>2.9637896818831506</v>
+      </c>
+      <c r="F105" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F95</f>
+        <v>4.5997759832530125</v>
+      </c>
+      <c r="G105" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G95</f>
+        <v>3.8316715996913686</v>
+      </c>
+    </row>
+    <row r="106" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C106" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D106" s="14">
+        <v>4000</v>
+      </c>
+      <c r="E106" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E96</f>
+        <v>2.2003116197396881</v>
+      </c>
+      <c r="F106" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F96</f>
+        <v>3.4273013457670847</v>
+      </c>
+      <c r="G106" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G96</f>
+        <v>2.8512230580958526</v>
+      </c>
+    </row>
+    <row r="107" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C107" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D107" s="14">
+        <v>5000</v>
+      </c>
+      <c r="E107" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E97</f>
+        <v>1.7422247824536103</v>
+      </c>
+      <c r="F107" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F97</f>
+        <v>2.7238165632755282</v>
+      </c>
+      <c r="G107" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G97</f>
+        <v>2.262953933138542</v>
+      </c>
+    </row>
+    <row r="108" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C108" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D108" s="14">
+        <v>6000</v>
+      </c>
+      <c r="E108" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F108" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F98</f>
+        <v>2.2548267082811564</v>
+      </c>
+      <c r="G108" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G98</f>
+        <v>1.8707745165003349</v>
+      </c>
+    </row>
+    <row r="109" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C109" s="14"/>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14"/>
+      <c r="F109" s="14"/>
+      <c r="G109" s="14"/>
+    </row>
+    <row r="110" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C110" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D110" s="14">
+        <v>0</v>
+      </c>
+      <c r="E110" s="16" t="e">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E82)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>109</v>
-      </c>
-      <c r="E69" s="7">
-        <f t="shared" ref="E69:G69" si="17">E54/E64</f>
-        <v>0.37678942325310782</v>
-      </c>
-      <c r="F69" s="7">
-        <f t="shared" si="17"/>
-        <v>0.24376139566040037</v>
-      </c>
-      <c r="G69" s="7">
-        <f t="shared" si="17"/>
-        <v>0.29560784875687074</v>
-      </c>
-    </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>110</v>
-      </c>
-      <c r="E70" s="7">
-        <f t="shared" ref="E70:G70" si="18">E55/E65</f>
-        <v>0.76882544095246808</v>
-      </c>
-      <c r="F70" s="7">
-        <f t="shared" si="18"/>
-        <v>0.49385877576499077</v>
-      </c>
-      <c r="G70" s="7">
-        <f t="shared" si="18"/>
-        <v>0.60055938530001973</v>
-      </c>
-    </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>111</v>
-      </c>
-      <c r="E71" s="7" t="s">
+      <c r="F110" s="16" t="e">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F82)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G110" s="16" t="e">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G82)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="111" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C111" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="D111" s="23">
+        <v>500</v>
+      </c>
+      <c r="E111" s="24">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E83)</f>
+        <v>10.393921185015483</v>
+      </c>
+      <c r="F111" s="24">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F83)</f>
+        <v>10.030118683410457</v>
+      </c>
+      <c r="G111" s="24">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G83)</f>
+        <v>10.159991169312509</v>
+      </c>
+    </row>
+    <row r="112" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C112" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="D112" s="23">
+        <v>1000</v>
+      </c>
+      <c r="E112" s="24">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E84)</f>
+        <v>5.8045528739959602</v>
+      </c>
+      <c r="F112" s="24">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F84)</f>
+        <v>5.3661985891606596</v>
+      </c>
+      <c r="G112" s="24">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G84)</f>
+        <v>5.5182233585799088</v>
+      </c>
+    </row>
+    <row r="113" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C113" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D113" s="14">
+        <v>2000</v>
+      </c>
+      <c r="E113" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E85)</f>
+        <v>3.8054926752552789</v>
+      </c>
+      <c r="F113" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F85)</f>
+        <v>3.1249586460082184</v>
+      </c>
+      <c r="G113" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G85)</f>
+        <v>3.34253022359679</v>
+      </c>
+    </row>
+    <row r="114" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C114" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D114" s="14">
+        <v>3000</v>
+      </c>
+      <c r="E114" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E86)</f>
+        <v>3.717309172657397</v>
+      </c>
+      <c r="F114" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F86)</f>
+        <v>2.5004675305962909</v>
+      </c>
+      <c r="G114" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G86)</f>
+        <v>2.837825302119557</v>
+      </c>
+    </row>
+    <row r="115" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C115" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D115" s="14">
+        <v>4000</v>
+      </c>
+      <c r="E115" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E87)</f>
+        <v>5.3081047689566478</v>
+      </c>
+      <c r="F115" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F87)</f>
+        <v>2.3526372364281896</v>
+      </c>
+      <c r="G115" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G87)</f>
+        <v>2.9471866006451912</v>
+      </c>
+    </row>
+    <row r="116" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C116" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D116" s="14">
+        <v>5000</v>
+      </c>
+      <c r="E116" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E88)</f>
+        <v>54.883363868245084</v>
+      </c>
+      <c r="F116" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F88)</f>
+        <v>2.5361039564424659</v>
+      </c>
+      <c r="G116" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G88)</f>
+        <v>3.8705216300526137</v>
+      </c>
+    </row>
+    <row r="117" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C117" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D117" s="14">
+        <v>6000</v>
+      </c>
+      <c r="E117" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="F71" s="7">
-        <f t="shared" ref="F71:G71" si="19">F56/F66</f>
-        <v>0.75054242584718556</v>
-      </c>
-      <c r="G71" s="7">
-        <f t="shared" si="19"/>
-        <v>0.9153047318212072</v>
-      </c>
-    </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-    </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="D74" s="15"/>
-      <c r="E74" s="16" t="e">
-        <f t="shared" ref="E74:G76" si="20">Engine_spec_d_life__h/Hours_in_a_year__h/E68</f>
+      <c r="F117" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F89)</f>
+        <v>3.2619978644141554</v>
+      </c>
+      <c r="G117" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G89)</f>
+        <v>9.2663659785740737</v>
+      </c>
+    </row>
+    <row r="119" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>126</v>
+      </c>
+      <c r="E119" s="4" t="e">
+        <f>(Engine_service_interval__h/E91)/24</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F74" s="16" t="e">
-        <f t="shared" si="20"/>
+      <c r="F119" s="4" t="e">
+        <f>(Engine_service_interval__h/F91)/24</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G74" s="16" t="e">
-        <f t="shared" si="20"/>
+      <c r="G119" s="4" t="e">
+        <f>(Engine_service_interval__h/G91)/24</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="D75" s="15"/>
-      <c r="E75" s="16">
-        <f t="shared" si="20"/>
-        <v>4.5445245048002132</v>
-      </c>
-      <c r="F75" s="16">
-        <f t="shared" si="20"/>
-        <v>7.0246101212385685</v>
-      </c>
-      <c r="G75" s="16">
-        <f t="shared" si="20"/>
-        <v>5.7925686828824041</v>
-      </c>
-    </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="D76" s="15"/>
-      <c r="E76" s="16">
-        <f t="shared" si="20"/>
-        <v>2.2272009690547567</v>
-      </c>
-      <c r="F76" s="16">
-        <f t="shared" si="20"/>
-        <v>3.4672437772739344</v>
-      </c>
-      <c r="G76" s="16">
-        <f t="shared" si="20"/>
-        <v>2.8512230580958526</v>
-      </c>
-    </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C77" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="D77" s="15"/>
-      <c r="E77" s="16" t="s">
+    <row r="120" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>159</v>
+      </c>
+      <c r="E120" s="7">
+        <f>(Engine_service_interval__h/E92)/24</f>
+        <v>443.67820583564179</v>
+      </c>
+      <c r="F120" s="7">
+        <f>(Engine_service_interval__h/F92)/24</f>
+        <v>682.53220583564155</v>
+      </c>
+      <c r="G120" s="7">
+        <f>(Engine_service_interval__h/G92)/24</f>
+        <v>570.38896583564167</v>
+      </c>
+    </row>
+    <row r="121" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>160</v>
+      </c>
+      <c r="E121" s="7">
+        <f>(Engine_service_interval__h/E93)/24</f>
+        <v>220.7426116897507</v>
+      </c>
+      <c r="F121" s="7">
+        <f>(Engine_service_interval__h/F93)/24</f>
+        <v>340.16961168975064</v>
+      </c>
+      <c r="G121" s="7">
+        <f>(Engine_service_interval__h/G93)/24</f>
+        <v>284.0979916897507</v>
+      </c>
+    </row>
+    <row r="122" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>127</v>
+      </c>
+      <c r="E122" s="7">
+        <f>(Engine_service_interval__h/E94)/24</f>
+        <v>109.27481461680516</v>
+      </c>
+      <c r="F122" s="7">
+        <f>(Engine_service_interval__h/F94)/24</f>
+        <v>168.98831461680513</v>
+      </c>
+      <c r="G122" s="7">
+        <f>(Engine_service_interval__h/G94)/24</f>
+        <v>140.95250461680516</v>
+      </c>
+    </row>
+    <row r="123" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
+        <v>161</v>
+      </c>
+      <c r="E123" s="7">
+        <f>(Engine_service_interval__h/E95)/24</f>
+        <v>72.118882259156663</v>
+      </c>
+      <c r="F123" s="7">
+        <f>(Engine_service_interval__h/F95)/24</f>
+        <v>111.92788225915665</v>
+      </c>
+      <c r="G123" s="7">
+        <f>(Engine_service_interval__h/G95)/24</f>
+        <v>93.237342259156648</v>
+      </c>
+    </row>
+    <row r="124" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>128</v>
+      </c>
+      <c r="E124" s="7">
+        <f>(Engine_service_interval__h/E96)/24</f>
+        <v>53.540916080332408</v>
+      </c>
+      <c r="F124" s="7">
+        <f>(Engine_service_interval__h/F96)/24</f>
+        <v>83.397666080332399</v>
+      </c>
+      <c r="G124" s="7">
+        <f>(Engine_service_interval__h/G96)/24</f>
+        <v>69.379761080332415</v>
+      </c>
+    </row>
+    <row r="125" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>162</v>
+      </c>
+      <c r="E125" s="7">
+        <f>(Engine_service_interval__h/E97)/24</f>
+        <v>42.394136373037853</v>
+      </c>
+      <c r="F125" s="7">
+        <f>(Engine_service_interval__h/F97)/24</f>
+        <v>66.279536373037857</v>
+      </c>
+      <c r="G125" s="7">
+        <f>(Engine_service_interval__h/G97)/24</f>
+        <v>55.065212373037859</v>
+      </c>
+    </row>
+    <row r="126" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>129</v>
+      </c>
+      <c r="E126" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="F77" s="16">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F71</f>
-        <v>2.28145499595239</v>
-      </c>
-      <c r="G77" s="16">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G71</f>
-        <v>1.8707745165003349</v>
-      </c>
-    </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C78" s="15"/>
-      <c r="D78" s="15"/>
-      <c r="E78" s="15"/>
-      <c r="F78" s="15"/>
-      <c r="G78" s="15"/>
-    </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D79" s="15"/>
-      <c r="E79" s="17" t="e">
-        <f t="shared" ref="E79:G81" si="21">Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E63)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F79" s="17" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G79" s="17" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C80" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D80" s="15"/>
-      <c r="E80" s="16">
-        <f t="shared" si="21"/>
-        <v>3.7779398210546522</v>
-      </c>
-      <c r="F80" s="16">
-        <f t="shared" si="21"/>
-        <v>3.113371945420047</v>
-      </c>
-      <c r="G80" s="16">
-        <f t="shared" si="21"/>
-        <v>3.34253022359679</v>
-      </c>
-    </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C81" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="D81" s="15"/>
-      <c r="E81" s="16">
-        <f t="shared" si="21"/>
-        <v>5.0923684346909912</v>
-      </c>
-      <c r="F81" s="16">
-        <f t="shared" si="21"/>
-        <v>2.3258844982969733</v>
-      </c>
-      <c r="G81" s="16">
-        <f t="shared" si="21"/>
-        <v>2.9471866006451912</v>
-      </c>
-    </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C82" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="D82" s="15"/>
-      <c r="E82" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F82" s="16">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F66)</f>
-        <v>3.1460955004613513</v>
-      </c>
-      <c r="G82" s="16">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G66)</f>
-        <v>9.2663659785740737</v>
-      </c>
-    </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
-        <v>126</v>
-      </c>
-      <c r="E84" s="4" t="e">
-        <f t="shared" ref="E84:G86" si="22">(Engine_service_interval__h/E68)/24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F84" s="4" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G84" s="4" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
-        <v>127</v>
-      </c>
-      <c r="E85" s="14">
-        <f t="shared" si="22"/>
-        <v>27.645857404201294</v>
-      </c>
-      <c r="F85" s="14">
-        <f t="shared" si="22"/>
-        <v>42.733044904201286</v>
-      </c>
-      <c r="G85" s="14">
-        <f t="shared" si="22"/>
-        <v>35.238126154201289</v>
-      </c>
-    </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C86" t="s">
-        <v>128</v>
-      </c>
-      <c r="E86" s="14">
-        <f t="shared" si="22"/>
-        <v>13.548805895083104</v>
-      </c>
-      <c r="F86" s="14">
-        <f t="shared" si="22"/>
-        <v>21.092399645083102</v>
-      </c>
-      <c r="G86" s="14">
-        <f t="shared" si="22"/>
-        <v>17.344940270083104</v>
-      </c>
-    </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C87" t="s">
-        <v>129</v>
-      </c>
-      <c r="E87" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="F87" s="14">
-        <f>(Engine_service_interval__h/F71)/24</f>
-        <v>13.878851225377039</v>
-      </c>
-      <c r="G87" s="14">
-        <f>(Engine_service_interval__h/G71)/24</f>
-        <v>11.380544975377036</v>
+      <c r="F126" s="7">
+        <f>(Engine_service_interval__h/F98)/24</f>
+        <v>54.867449901508138</v>
+      </c>
+      <c r="G126" s="7">
+        <f>(Engine_service_interval__h/G98)/24</f>
+        <v>45.522179901508146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes. This is the version I sent to Michael Holder on 3/31/2016.
</commit_message>
<xml_diff>
--- a/Control and Data Systems/BMs Hygen System Design Calcs.xlsx
+++ b/Control and Data Systems/BMs Hygen System Design Calcs.xlsx
@@ -18,12 +18,14 @@
     <definedName name="Beckett_module_nominal_energy__kWh">'Hygen Use Models'!$D$14</definedName>
     <definedName name="Cycle_energy__kWh">'Hygen Use Models'!$D$18</definedName>
     <definedName name="Depth_of_Discharge">'Hygen Use Models'!$D$17</definedName>
+    <definedName name="Diesel_cost____l">'Hygen Use Models'!$G$20</definedName>
     <definedName name="Engine_service_interval__h">'Hygen Use Models'!$G$16</definedName>
     <definedName name="Engine_spec_d_life__h">'Hygen Use Models'!$G$14</definedName>
     <definedName name="Format_Parallel">'Beckett Battery Modules'!$H$7</definedName>
     <definedName name="Format_Parallel_Stack">'Beckett Battery Modules'!$N$7</definedName>
     <definedName name="Format_Series">'Beckett Battery Modules'!$H$6</definedName>
     <definedName name="Format_Series_Stack">'Beckett Battery Modules'!$N$6</definedName>
+    <definedName name="Fuel_Tank_Capacity__l">'Hygen Use Models'!$G$19</definedName>
     <definedName name="Hours_in_a_year__h">'Hygen Use Models'!$G$15</definedName>
     <definedName name="Max_charge_rate">'Beckett Battery Modules'!$C$9</definedName>
     <definedName name="Max_discharge_rate">'Beckett Battery Modules'!$C$10</definedName>
@@ -32,7 +34,8 @@
     <definedName name="Nominal_Energy">'Beckett Battery Modules'!$C$7</definedName>
     <definedName name="Nominal_Energy_Module">'Beckett Battery Modules'!$H$9</definedName>
     <definedName name="Nominal_Voltage">'Beckett Battery Modules'!$C$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Hygen Use Models'!$B$1:$G$106</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Hygen Use Models'!$B$1:$P$127</definedName>
+    <definedName name="SFC__l_kWh">'Hygen Use Models'!$G$18</definedName>
     <definedName name="Stack_height">'Hygen Use Models'!$D$15</definedName>
     <definedName name="Voltage_at_0">'Beckett Battery Modules'!$B$11:$C$11</definedName>
     <definedName name="Voltage_at_100">'Beckett Battery Modules'!$B$14:$C$14</definedName>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="170">
   <si>
     <t>Boston Swing 5300</t>
   </si>
@@ -115,12 +118,6 @@
     <t>Approx</t>
   </si>
   <si>
-    <t>260V</t>
-  </si>
-  <si>
-    <t>296V</t>
-  </si>
-  <si>
     <t>10kWh</t>
   </si>
   <si>
@@ -406,9 +403,6 @@
     <t>Batt Cycles 80% DOD</t>
   </si>
   <si>
-    <t>Batt Cycles 50% DOD, guesstimated</t>
-  </si>
-  <si>
     <t>Battery life in years w/ 0kW Tower Load, y</t>
   </si>
   <si>
@@ -539,6 +533,30 @@
   </si>
   <si>
     <t>Fuel Tank Capacity, l</t>
+  </si>
+  <si>
+    <t>Diesel cost, $/l</t>
+  </si>
+  <si>
+    <t>250 liter tank refill interval, d</t>
+  </si>
+  <si>
+    <t>Fuel Cost per Month, $USD</t>
+  </si>
+  <si>
+    <t>1000 liter tank refill interval, days</t>
+  </si>
+  <si>
+    <t>Engine maintenance interval, days</t>
+  </si>
+  <si>
+    <t>These plots customized for Angus's Chilean customer.</t>
+  </si>
+  <si>
+    <t>Batt Cycles 50% DOD, estimated.</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -623,7 +641,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -681,6 +699,37 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,8 +739,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9999"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFFF9999"/>
     </mruColors>
   </colors>
   <extLst>
@@ -716,9 +765,45 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HyGen Life</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.44040243138621465"/>
+          <c:y val="9.3800045756119894E-3"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13067957104489797"/>
+          <c:y val="9.2522060512247276E-2"/>
+          <c:w val="0.82038607282198306"/>
+          <c:h val="0.7405269111309406"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -730,37 +815,37 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hygen Use Models'!$D$102:$D$108</c:f>
+              <c:f>'Hygen Use Models'!$D$103:$D$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>500</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2000</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hygen Use Models'!$G$102:$G$108</c:f>
+              <c:f>'Hygen Use Models'!$G$103:$G$109</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -798,37 +883,37 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hygen Use Models'!$D$111:$D$117</c:f>
+              <c:f>'Hygen Use Models'!$D$112:$D$118</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>500</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2000</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3000</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5000</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hygen Use Models'!$G$111:$G$117</c:f>
+              <c:f>'Hygen Use Models'!$G$112:$G$118</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -866,11 +951,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="80529664"/>
-        <c:axId val="80456320"/>
+        <c:axId val="100256000"/>
+        <c:axId val="109233280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80529664"/>
+        <c:axId val="100256000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -888,7 +973,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Customer Load, W </a:t>
+                  <a:t>Customer Load, kW </a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -900,12 +985,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80456320"/>
+        <c:crossAx val="109233280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80456320"/>
+        <c:axId val="109233280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -931,11 +1016,1027 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80529664"/>
+        <c:crossAx val="100256000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HyGen Fuel</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11244156336128087"/>
+          <c:y val="0.10059742656665657"/>
+          <c:w val="0.7850726906559361"/>
+          <c:h val="0.69191106122942914"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hygen Use Models'!$J$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fuel Cost per Month, $USD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$I$46:$I$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$J$46:$J$53</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>139.08000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>278.16000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>556.32000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>834.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1112.6400000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1390.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1668.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="99794304"/>
+        <c:axId val="99800576"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hygen Use Models'!$K$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1000 liter tank refill interval, days</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$I$46:$I$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$K$46:$K$53</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
+                  <c:v>219.29824561403507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>109.64912280701753</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54.824561403508767</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.549707602339183</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.412280701754383</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.929824561403507</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.274853801169591</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="99804672"/>
+        <c:axId val="99802496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="99794304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Customer Load, kW</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99800576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="99800576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>$USD</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99794304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="99802496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="270"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99804672"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="30"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="99804672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99802496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HyGen Fuel Use</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11244156336128087"/>
+          <c:y val="0.10059742656665657"/>
+          <c:w val="0.7850726906559361"/>
+          <c:h val="0.69191106122942914"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hygen Use Models'!$J$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fuel Cost per Month, $USD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$I$46:$I$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$J$46:$J$49</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>139.08000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>278.16000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>556.32000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="99824000"/>
+        <c:axId val="99825920"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hygen Use Models'!$K$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1000 liter tank refill interval, days</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$I$46:$I$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$K$46:$K$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>219.29824561403507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>109.64912280701753</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54.824561403508767</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hygen Use Models'!$M$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Engine maintenance interval, days</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$I$46:$I$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$M$46:$M$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>570.38896583564167</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>284.0979916897507</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>140.95250461680516</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="99834112"/>
+        <c:axId val="99832192"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="99824000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Customer Load, kW</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99825920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="99825920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>$USD</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99824000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="99832192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="540"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99834112"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="60"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="99834112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99832192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HyGen Life</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.44040243138621465"/>
+          <c:y val="9.3800045756119894E-3"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11101384943924164"/>
+          <c:y val="9.2522060512247276E-2"/>
+          <c:w val="0.77908813492081308"/>
+          <c:h val="0.7405269111309406"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Engine Life in Years</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$D$103:$D$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$G$103:$G$105</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>23.440642431601713</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.675259932455509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7925686828824041</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Battery Life in Years</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$D$112:$D$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hygen Use Models'!$G$112:$G$114</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10.159991169312509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5182233585799088</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.34253022359679</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="99847168"/>
+        <c:axId val="99857536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="99847168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Customer Load, kW </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99857536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="99857536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Years</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99847168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1005,16 +2106,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>752474</xdr:colOff>
       <xdr:row>98</xdr:row>
-      <xdr:rowOff>14286</xdr:rowOff>
+      <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1028,6 +2129,100 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>733424</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>371476</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>138114</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1326,13 +2521,14 @@
   <dimension ref="A5:R38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1458,7 +2654,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>3.2</v>
@@ -1467,7 +2663,7 @@
         <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1494,7 +2690,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>4.2</v>
@@ -1513,7 +2709,7 @@
         <v>6</v>
       </c>
       <c r="J14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M14" t="s">
         <v>10</v>
@@ -1525,11 +2721,14 @@
       <c r="O14" t="s">
         <v>6</v>
       </c>
-      <c r="P14" t="s">
-        <v>23</v>
+      <c r="P14">
+        <v>260</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>6</v>
       </c>
       <c r="R14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1544,7 +2743,7 @@
         <v>6</v>
       </c>
       <c r="J15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M15" t="s">
         <v>11</v>
@@ -1556,21 +2755,24 @@
       <c r="O15" t="s">
         <v>6</v>
       </c>
-      <c r="P15" t="s">
-        <v>24</v>
+      <c r="P15">
+        <v>296</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>6</v>
       </c>
       <c r="R15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="R16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H17">
         <f>Format_Series*Format_Parallel*Nominal_Energy</f>
@@ -1580,10 +2782,10 @@
         <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N17">
         <f>H17*Format_Series_Stack</f>
@@ -1593,12 +2795,12 @@
         <v>4</v>
       </c>
       <c r="P17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H19">
         <f>Nominal_Capacity_Module/2</f>
@@ -1610,7 +2812,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H20">
         <v>25</v>
@@ -1618,10 +2820,17 @@
       <c r="I20" t="s">
         <v>8</v>
       </c>
+      <c r="J20">
+        <f>(P15+P14)/2*H20</f>
+        <v>6950</v>
+      </c>
+      <c r="K20" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H21">
         <v>50</v>
@@ -1632,12 +2841,12 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C28">
         <v>24.4</v>
@@ -1648,57 +2857,57 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C30">
         <f>220 * 2/SQRT(2)</f>
         <v>311.12698372208087</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C31">
         <f>240*2/SQRT(2)</f>
         <v>339.41125496954277</v>
       </c>
       <c r="D31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1708,10 +2917,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G126"/>
+  <dimension ref="B1:R127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H108" sqref="H108:H109"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,23 +2932,24 @@
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="10" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="13" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" s="3">
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G14">
         <v>15000</v>
@@ -1747,13 +2957,13 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D15">
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G15">
         <f>365*24</f>
@@ -1762,14 +2972,14 @@
     </row>
     <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D16">
         <f>D15*D14</f>
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G16">
         <v>1000</v>
@@ -1777,7 +2987,7 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D17" s="2">
         <v>0.5</v>
@@ -1785,14 +2995,14 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D18">
         <f>D17*Batt_bank_energy__kWh</f>
         <v>5.5</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G18">
         <v>0.38</v>
@@ -1800,13 +3010,13 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D19">
         <v>3000</v>
       </c>
       <c r="F19" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G19">
         <v>1000</v>
@@ -1814,12 +3024,18 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
       <c r="D20">
         <f>D19*2.5</f>
         <v>7500</v>
       </c>
+      <c r="F20" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
@@ -1833,24 +3049,24 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="G25" s="32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="F26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1858,7 +3074,7 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E27" s="4">
         <v>10.3</v>
@@ -1866,14 +3082,14 @@
       <c r="F27" s="4">
         <v>15.3</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="32">
         <v>15.3</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E28" s="5">
         <v>0.7</v>
@@ -1881,16 +3097,16 @@
       <c r="F28" s="5">
         <v>0.7</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="34">
         <v>0.59</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E29" s="6">
         <f>E27*E28</f>
@@ -1900,7 +3116,7 @@
         <f t="shared" ref="F29:G29" si="0">F27*F28</f>
         <v>10.709999999999999</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="35">
         <f t="shared" si="0"/>
         <v>9.0269999999999992</v>
       </c>
@@ -1908,7 +3124,7 @@
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E30" s="5">
         <v>0.88</v>
@@ -1916,16 +3132,16 @@
       <c r="F30" s="5">
         <v>0.88</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="34">
         <v>0.88</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E31" s="6">
         <f>E30*E29</f>
@@ -1935,7 +3151,7 @@
         <f t="shared" ref="F31:G31" si="1">F30*F29</f>
         <v>9.4247999999999994</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="35">
         <f t="shared" si="1"/>
         <v>7.9437599999999993</v>
       </c>
@@ -1943,7 +3159,7 @@
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E32" s="5">
         <v>0.94</v>
@@ -1951,16 +3167,16 @@
       <c r="F32" s="5">
         <v>0.94</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="34">
         <v>0.94</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E33" s="9">
         <f>E32*E31</f>
@@ -1970,17 +3186,17 @@
         <f t="shared" ref="F33:G33" si="2">F32*F31</f>
         <v>8.8593119999999992</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="35">
         <f t="shared" si="2"/>
         <v>7.4671343999999991</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
         <v>59</v>
-      </c>
-      <c r="C34" t="s">
-        <v>61</v>
       </c>
       <c r="E34" s="4">
         <v>7.5</v>
@@ -1993,10 +3209,10 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E35" s="5">
         <v>0.99</v>
@@ -2004,16 +3220,16 @@
       <c r="F35" s="5">
         <v>0.99</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="34">
         <v>0.99</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E36" s="6">
         <f>E35*E33</f>
@@ -2023,15 +3239,15 @@
         <f>F35*F34</f>
         <v>8.7707188799999987</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36" s="35">
         <f>G35*G34</f>
         <v>7.4249999999999998</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E37" s="5">
         <v>0.95</v>
@@ -2039,16 +3255,16 @@
       <c r="F37" s="5">
         <v>0.95</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="34">
         <v>0.95</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E38" s="6">
         <f>E37*E36</f>
@@ -2058,17 +3274,17 @@
         <f t="shared" ref="F38:G38" si="3">F37*F36</f>
         <v>8.3321829359999988</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="35">
         <f t="shared" si="3"/>
         <v>7.0537499999999991</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E39" s="4">
         <v>0.5</v>
@@ -2076,14 +3292,14 @@
       <c r="F39" s="4">
         <v>0.5</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="32">
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E40" s="5">
         <f>E37</f>
@@ -2093,17 +3309,17 @@
         <f t="shared" ref="F40:G40" si="4">F37</f>
         <v>0.95</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="34">
         <f t="shared" si="4"/>
         <v>0.95</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E41" s="7">
         <f>E39/E40</f>
@@ -2113,17 +3329,17 @@
         <f t="shared" ref="F41:G41" si="5">F39/F40</f>
         <v>0.52631578947368418</v>
       </c>
-      <c r="G41" s="7">
+      <c r="G41" s="36">
         <f t="shared" si="5"/>
         <v>0.52631578947368418</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E42" s="8">
         <f>E38-E41</f>
@@ -2133,44 +3349,60 @@
         <f t="shared" ref="F42:G42" si="6">F38-F41</f>
         <v>7.8058671465263147</v>
       </c>
-      <c r="G42" s="8">
+      <c r="G42" s="37">
         <f t="shared" si="6"/>
         <v>6.527434210526315</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="C44" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="C45" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="8"/>
+      <c r="I45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J45" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="K45" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="L45" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="M45" s="27" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" t="s">
         <v>86</v>
-      </c>
-      <c r="C46" t="s">
-        <v>88</v>
       </c>
       <c r="D46" s="4">
         <v>0</v>
@@ -2187,17 +3419,26 @@
         <f t="shared" si="7"/>
         <v>6.8709833795013848</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="11"/>
+      <c r="I46" s="4">
+        <v>0</v>
+      </c>
+      <c r="J46" s="26">
+        <f t="shared" ref="J46:J53" si="8">$I46*24*30.5*SFC__l_kWh*Diesel_cost____l</f>
+        <v>0</v>
+      </c>
+      <c r="M46" s="4"/>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D47" s="4">
         <v>0.5</v>
       </c>
       <c r="E47" s="11">
-        <f t="shared" ref="E47:E48" si="8">E$36-($D47+E$41)/E$37</f>
+        <f t="shared" ref="E47:E48" si="9">E$36-($D47+E$41)/E$37</f>
         <v>4.8241384700277008</v>
       </c>
       <c r="F47" s="11">
@@ -2208,17 +3449,37 @@
         <f t="shared" si="7"/>
         <v>6.3446675900277008</v>
       </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="11"/>
+      <c r="I47" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="J47" s="28">
+        <f t="shared" si="8"/>
+        <v>139.08000000000001</v>
+      </c>
+      <c r="K47" s="30">
+        <f t="shared" ref="K47:K53" si="10">Fuel_Tank_Capacity__l/($I47*24*SFC__l_kWh)</f>
+        <v>219.29824561403507</v>
+      </c>
+      <c r="L47" s="30">
+        <f t="shared" ref="L47:L53" si="11">K47/4</f>
+        <v>54.824561403508767</v>
+      </c>
+      <c r="M47" s="24">
+        <f t="shared" ref="M47:M53" si="12">G121</f>
+        <v>570.38896583564167</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
       <c r="C48" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
       </c>
       <c r="E48" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.2978226805540167</v>
       </c>
       <c r="F48" s="11">
@@ -2229,17 +3490,37 @@
         <f t="shared" si="7"/>
         <v>5.8183518005540167</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="11"/>
+      <c r="I48" s="29">
+        <v>1</v>
+      </c>
+      <c r="J48" s="28">
+        <f t="shared" si="8"/>
+        <v>278.16000000000003</v>
+      </c>
+      <c r="K48" s="30">
+        <f t="shared" si="10"/>
+        <v>109.64912280701753</v>
+      </c>
+      <c r="L48" s="30">
+        <f t="shared" si="11"/>
+        <v>27.412280701754383</v>
+      </c>
+      <c r="M48" s="24">
+        <f t="shared" si="12"/>
+        <v>284.0979916897507</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
       <c r="C49" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D49" s="4">
         <v>2</v>
       </c>
       <c r="E49" s="11">
-        <f t="shared" ref="E49:E53" si="9">E$36-($D49+E$41)/E$37</f>
+        <f t="shared" ref="E49:E53" si="13">E$36-($D49+E$41)/E$37</f>
         <v>3.2451911016066481</v>
       </c>
       <c r="F49" s="11">
@@ -2250,17 +3531,37 @@
         <f t="shared" si="7"/>
         <v>4.7657202216066477</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="11"/>
+      <c r="I49" s="4">
+        <v>2</v>
+      </c>
+      <c r="J49" s="26">
+        <f t="shared" si="8"/>
+        <v>556.32000000000005</v>
+      </c>
+      <c r="K49" s="3">
+        <f t="shared" si="10"/>
+        <v>54.824561403508767</v>
+      </c>
+      <c r="L49" s="3">
+        <f t="shared" si="11"/>
+        <v>13.706140350877192</v>
+      </c>
+      <c r="M49" s="7">
+        <f t="shared" si="12"/>
+        <v>140.95250461680516</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
       <c r="C50" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D50" s="4">
         <v>3</v>
       </c>
       <c r="E50" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.1925595226592796</v>
       </c>
       <c r="F50" s="11">
@@ -2271,17 +3572,37 @@
         <f t="shared" si="7"/>
         <v>3.7130886426592795</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="11"/>
+      <c r="I50" s="4">
+        <v>3</v>
+      </c>
+      <c r="J50" s="26">
+        <f t="shared" si="8"/>
+        <v>834.48</v>
+      </c>
+      <c r="K50" s="3">
+        <f t="shared" si="10"/>
+        <v>36.549707602339183</v>
+      </c>
+      <c r="L50" s="3">
+        <f t="shared" si="11"/>
+        <v>9.1374269005847957</v>
+      </c>
+      <c r="M50" s="7">
+        <f t="shared" si="12"/>
+        <v>93.237342259156648</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D51" s="4">
         <v>4</v>
       </c>
       <c r="E51" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.1399279437119114</v>
       </c>
       <c r="F51" s="11">
@@ -2292,17 +3613,37 @@
         <f t="shared" si="7"/>
         <v>2.6604570637119114</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="11"/>
+      <c r="I51" s="4">
+        <v>4</v>
+      </c>
+      <c r="J51" s="26">
+        <f t="shared" si="8"/>
+        <v>1112.6400000000001</v>
+      </c>
+      <c r="K51" s="3">
+        <f t="shared" si="10"/>
+        <v>27.412280701754383</v>
+      </c>
+      <c r="L51" s="3">
+        <f t="shared" si="11"/>
+        <v>6.8530701754385959</v>
+      </c>
+      <c r="M51" s="7">
+        <f t="shared" si="12"/>
+        <v>69.379761080332415</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D52" s="4">
         <v>5</v>
       </c>
       <c r="E52" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>8.7296364764542389E-2</v>
       </c>
       <c r="F52" s="11">
@@ -2313,17 +3654,37 @@
         <f t="shared" si="7"/>
         <v>1.6078254847645423</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="11"/>
+      <c r="I52" s="4">
+        <v>5</v>
+      </c>
+      <c r="J52" s="26">
+        <f t="shared" si="8"/>
+        <v>1390.8</v>
+      </c>
+      <c r="K52" s="3">
+        <f t="shared" si="10"/>
+        <v>21.929824561403507</v>
+      </c>
+      <c r="L52" s="3">
+        <f t="shared" si="11"/>
+        <v>5.4824561403508767</v>
+      </c>
+      <c r="M52" s="7">
+        <f t="shared" si="12"/>
+        <v>55.065212373037859</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
       <c r="C53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D53" s="4">
         <v>6</v>
       </c>
       <c r="E53" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-0.96533521418282575</v>
       </c>
       <c r="F53" s="11">
@@ -2334,1201 +3695,1199 @@
         <f t="shared" si="7"/>
         <v>0.5551939058171742</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="11"/>
+      <c r="I53" s="4">
+        <v>6</v>
+      </c>
+      <c r="J53" s="26">
+        <f t="shared" si="8"/>
+        <v>1668.96</v>
+      </c>
+      <c r="K53" s="3">
+        <f t="shared" si="10"/>
+        <v>18.274853801169591</v>
+      </c>
+      <c r="L53" s="3">
+        <f t="shared" si="11"/>
+        <v>4.5687134502923978</v>
+      </c>
+      <c r="M53" s="7">
+        <f t="shared" si="12"/>
+        <v>45.522179901508146</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C55" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D55" s="17"/>
       <c r="E55" s="18">
-        <f>E46/Batt_bank_energy__kWh</f>
+        <f t="shared" ref="E55:G62" si="14">E46/Batt_bank_energy__kWh</f>
         <v>0.48640493268194407</v>
       </c>
       <c r="F55" s="21">
-        <f>F46/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.74697293268194398</v>
       </c>
       <c r="G55" s="21">
-        <f>G46/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.62463485268194407</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C56" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D56" s="17"/>
       <c r="E56" s="18">
-        <f>E47/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.43855804272979099</v>
       </c>
       <c r="F56" s="21">
-        <f>F47/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.69912604272979084</v>
       </c>
       <c r="G56" s="21">
-        <f>G47/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.57678796272979094</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C57" s="17" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D57" s="17"/>
       <c r="E57" s="18">
-        <f>E48/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.3907111527776379</v>
       </c>
       <c r="F57" s="21">
-        <f>F48/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.65127915277763782</v>
       </c>
       <c r="G57" s="21">
-        <f>G48/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.52894107277763791</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C58" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D58" s="17"/>
       <c r="E58" s="18">
-        <f>E49/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.29501737287333163</v>
       </c>
       <c r="F58" s="21">
-        <f>F49/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.55558537287333154</v>
       </c>
       <c r="G58" s="18">
-        <f>G49/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.43324729287333158</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C59" s="17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D59" s="17"/>
       <c r="E59" s="18">
-        <f>E50/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.19932359296902541</v>
       </c>
       <c r="F59" s="18">
-        <f>F50/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.45989159296902532</v>
       </c>
       <c r="G59" s="18">
-        <f>G50/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.33755351296902542</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C60" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D60" s="17"/>
       <c r="E60" s="18">
-        <f>E51/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.10362981306471922</v>
       </c>
       <c r="F60" s="18">
-        <f>F51/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.3641978130647191</v>
       </c>
       <c r="G60" s="18">
-        <f>G51/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.24185973306471922</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C61" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D61" s="17"/>
       <c r="E61" s="18">
-        <f>E52/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>7.9360331604129437E-3</v>
       </c>
       <c r="F61" s="18">
-        <f>F52/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.26850403316041282</v>
       </c>
       <c r="G61" s="18">
-        <f>G52/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.14616595316041295</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C62" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D62" s="17"/>
       <c r="E62" s="21">
-        <f>E53/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>-8.775774674389325E-2</v>
       </c>
       <c r="F62" s="18">
-        <f>F53/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>0.17281025325610663</v>
       </c>
       <c r="G62" s="18">
-        <f>G53/Batt_bank_energy__kWh</f>
+        <f t="shared" si="14"/>
         <v>5.0472173256106749E-2</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" t="s">
+        <v>91</v>
+      </c>
+      <c r="E64" s="13">
+        <f t="shared" ref="E64:G71" si="15">1/E55*Depth_of_Discharge</f>
+        <v>1.0279501016634336</v>
+      </c>
+      <c r="F64" s="13">
+        <f t="shared" si="15"/>
+        <v>0.66936829719490865</v>
+      </c>
+      <c r="G64" s="13">
+        <f t="shared" si="15"/>
+        <v>0.80046766179183004</v>
+      </c>
+    </row>
+    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>132</v>
+      </c>
+      <c r="E65" s="13">
+        <f t="shared" si="15"/>
+        <v>1.1400999440980844</v>
+      </c>
+      <c r="F65" s="13">
+        <f t="shared" si="15"/>
+        <v>0.71517862222341477</v>
+      </c>
+      <c r="G65" s="13">
+        <f t="shared" si="15"/>
+        <v>0.86686968575701018</v>
+      </c>
+    </row>
+    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>133</v>
+      </c>
+      <c r="E66" s="13">
+        <f t="shared" si="15"/>
+        <v>1.2797177568272813</v>
+      </c>
+      <c r="F66" s="13">
+        <f t="shared" si="15"/>
+        <v>0.76771995213965016</v>
+      </c>
+      <c r="G66" s="13">
+        <f t="shared" si="15"/>
+        <v>0.94528488282133372</v>
+      </c>
+    </row>
+    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>92</v>
+      </c>
+      <c r="E67" s="13">
+        <f t="shared" si="15"/>
+        <v>1.6948154446981654</v>
+      </c>
+      <c r="F67" s="13">
+        <f t="shared" si="15"/>
+        <v>0.89995169853759904</v>
+      </c>
+      <c r="G67" s="13">
+        <f t="shared" si="15"/>
+        <v>1.1540753011610505</v>
+      </c>
+    </row>
+    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>134</v>
+      </c>
+      <c r="E68" s="13">
+        <f t="shared" si="15"/>
+        <v>2.5084837803305065</v>
+      </c>
+      <c r="F68" s="13">
+        <f t="shared" si="15"/>
+        <v>1.0872127424031344</v>
+      </c>
+      <c r="G68" s="13">
+        <f t="shared" si="15"/>
+        <v>1.4812466195423095</v>
+      </c>
+    </row>
+    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>93</v>
+      </c>
+      <c r="E69" s="13">
+        <f t="shared" si="15"/>
+        <v>4.8248663701413648</v>
+      </c>
+      <c r="F69" s="13">
+        <f t="shared" si="15"/>
+        <v>1.3728802921481256</v>
+      </c>
+      <c r="G69" s="13">
+        <f t="shared" si="15"/>
+        <v>2.0673139495535828</v>
+      </c>
+    </row>
+    <row r="70" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>135</v>
+      </c>
+      <c r="E70" s="13">
+        <f t="shared" si="15"/>
+        <v>63.00376899811026</v>
+      </c>
+      <c r="F70" s="13">
+        <f t="shared" si="15"/>
+        <v>1.8621694211247999</v>
+      </c>
+      <c r="G70" s="13">
+        <f t="shared" si="15"/>
+        <v>3.4207692639014526</v>
+      </c>
+    </row>
+    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>94</v>
+      </c>
+      <c r="E71" s="21">
+        <f t="shared" si="15"/>
+        <v>-5.697502711175674</v>
+      </c>
+      <c r="F71" s="13">
+        <f t="shared" si="15"/>
+        <v>2.8933468389690669</v>
+      </c>
+      <c r="G71" s="13">
+        <f t="shared" si="15"/>
+        <v>9.9064487963078509</v>
+      </c>
+    </row>
+    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="R72" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>100</v>
+      </c>
+      <c r="C74" t="s">
+        <v>95</v>
+      </c>
+      <c r="D74" s="4">
+        <v>0</v>
+      </c>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+    </row>
+    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>136</v>
+      </c>
+      <c r="D75" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E75" s="13">
+        <f t="shared" ref="E75:G81" si="16">Cycle_energy__kWh/$D75</f>
+        <v>11</v>
+      </c>
+      <c r="F75" s="13">
+        <f t="shared" si="16"/>
+        <v>11</v>
+      </c>
+      <c r="G75" s="13">
+        <f t="shared" si="16"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>137</v>
+      </c>
+      <c r="D76" s="4">
+        <v>1</v>
+      </c>
+      <c r="E76" s="13">
+        <f t="shared" si="16"/>
+        <v>5.5</v>
+      </c>
+      <c r="F76" s="13">
+        <f t="shared" si="16"/>
+        <v>5.5</v>
+      </c>
+      <c r="G76" s="13">
+        <f t="shared" si="16"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>96</v>
+      </c>
+      <c r="D77" s="4">
+        <v>2</v>
+      </c>
+      <c r="E77" s="13">
+        <f t="shared" si="16"/>
+        <v>2.75</v>
+      </c>
+      <c r="F77" s="13">
+        <f t="shared" si="16"/>
+        <v>2.75</v>
+      </c>
+      <c r="G77" s="13">
+        <f t="shared" si="16"/>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>138</v>
+      </c>
+      <c r="D78" s="4">
+        <v>3</v>
+      </c>
+      <c r="E78" s="13">
+        <f t="shared" si="16"/>
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="F78" s="13">
+        <f t="shared" si="16"/>
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="G78" s="13">
+        <f t="shared" si="16"/>
+        <v>1.8333333333333333</v>
+      </c>
+    </row>
+    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>97</v>
+      </c>
+      <c r="D79" s="4">
+        <v>4</v>
+      </c>
+      <c r="E79" s="13">
+        <f t="shared" si="16"/>
+        <v>1.375</v>
+      </c>
+      <c r="F79" s="13">
+        <f t="shared" si="16"/>
+        <v>1.375</v>
+      </c>
+      <c r="G79" s="13">
+        <f t="shared" si="16"/>
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="80" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>139</v>
+      </c>
+      <c r="D80" s="4">
+        <v>5</v>
+      </c>
+      <c r="E80" s="13">
+        <f t="shared" si="16"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F80" s="13">
+        <f t="shared" si="16"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G80" s="13">
+        <f t="shared" si="16"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>98</v>
+      </c>
+      <c r="D81" s="4">
+        <v>6</v>
+      </c>
+      <c r="E81" s="21">
+        <f t="shared" si="16"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F81" s="13">
+        <f t="shared" si="16"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="G81" s="13">
+        <f t="shared" si="16"/>
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
         <v>101</v>
       </c>
-      <c r="C64" t="s">
-        <v>93</v>
-      </c>
-      <c r="E64" s="13">
-        <f>1/E55*Depth_of_Discharge</f>
-        <v>1.0279501016634336</v>
-      </c>
-      <c r="F64" s="13">
-        <f>1/F55*Depth_of_Discharge</f>
-        <v>0.66936829719490865</v>
-      </c>
-      <c r="G64" s="13">
-        <f>1/G55*Depth_of_Discharge</f>
-        <v>0.80046766179183004</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
-        <v>135</v>
-      </c>
-      <c r="E65" s="13">
-        <f>1/E56*Depth_of_Discharge</f>
-        <v>1.1400999440980844</v>
-      </c>
-      <c r="F65" s="13">
-        <f>1/F56*Depth_of_Discharge</f>
-        <v>0.71517862222341477</v>
-      </c>
-      <c r="G65" s="13">
-        <f>1/G56*Depth_of_Discharge</f>
-        <v>0.86686968575701018</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
-        <v>136</v>
-      </c>
-      <c r="E66" s="13">
-        <f>1/E57*Depth_of_Discharge</f>
-        <v>1.2797177568272813</v>
-      </c>
-      <c r="F66" s="13">
-        <f>1/F57*Depth_of_Discharge</f>
-        <v>0.76771995213965016</v>
-      </c>
-      <c r="G66" s="13">
-        <f>1/G57*Depth_of_Discharge</f>
-        <v>0.94528488282133372</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
-        <v>94</v>
-      </c>
-      <c r="E67" s="13">
-        <f>1/E58*Depth_of_Discharge</f>
-        <v>1.6948154446981654</v>
-      </c>
-      <c r="F67" s="13">
-        <f>1/F58*Depth_of_Discharge</f>
-        <v>0.89995169853759904</v>
-      </c>
-      <c r="G67" s="13">
-        <f>1/G58*Depth_of_Discharge</f>
-        <v>1.1540753011610505</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
-        <v>137</v>
-      </c>
-      <c r="E68" s="13">
-        <f>1/E59*Depth_of_Discharge</f>
-        <v>2.5084837803305065</v>
-      </c>
-      <c r="F68" s="13">
-        <f>1/F59*Depth_of_Discharge</f>
-        <v>1.0872127424031344</v>
-      </c>
-      <c r="G68" s="13">
-        <f>1/G59*Depth_of_Discharge</f>
-        <v>1.4812466195423095</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>95</v>
-      </c>
-      <c r="E69" s="13">
-        <f>1/E60*Depth_of_Discharge</f>
-        <v>4.8248663701413648</v>
-      </c>
-      <c r="F69" s="13">
-        <f>1/F60*Depth_of_Discharge</f>
-        <v>1.3728802921481256</v>
-      </c>
-      <c r="G69" s="13">
-        <f>1/G60*Depth_of_Discharge</f>
-        <v>2.0673139495535828</v>
-      </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>138</v>
-      </c>
-      <c r="E70" s="13">
-        <f>1/E61*Depth_of_Discharge</f>
-        <v>63.00376899811026</v>
-      </c>
-      <c r="F70" s="13">
-        <f>1/F61*Depth_of_Discharge</f>
-        <v>1.8621694211247999</v>
-      </c>
-      <c r="G70" s="13">
-        <f>1/G61*Depth_of_Discharge</f>
-        <v>3.4207692639014526</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>96</v>
-      </c>
-      <c r="E71" s="13">
-        <f>1/E62*Depth_of_Discharge</f>
-        <v>-5.697502711175674</v>
-      </c>
-      <c r="F71" s="13">
-        <f>1/F62*Depth_of_Discharge</f>
-        <v>2.8933468389690669</v>
-      </c>
-      <c r="G71" s="13">
-        <f>1/G62*Depth_of_Discharge</f>
-        <v>9.9064487963078509</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="C83" t="s">
         <v>102</v>
       </c>
-      <c r="C73" t="s">
-        <v>97</v>
-      </c>
-      <c r="D73" s="4">
-        <v>0</v>
-      </c>
-      <c r="E73" s="13" t="e">
-        <f t="shared" ref="E73:G80" si="10">Cycle_energy__kWh/$D73</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F73" s="13" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G73" s="13" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
-        <v>139</v>
-      </c>
-      <c r="D74" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E74" s="13">
-        <f t="shared" si="10"/>
-        <v>11</v>
-      </c>
-      <c r="F74" s="13">
-        <f t="shared" si="10"/>
-        <v>11</v>
-      </c>
-      <c r="G74" s="13">
-        <f t="shared" si="10"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>140</v>
-      </c>
-      <c r="D75" s="4">
-        <v>1</v>
-      </c>
-      <c r="E75" s="13">
-        <f t="shared" si="10"/>
-        <v>5.5</v>
-      </c>
-      <c r="F75" s="13">
-        <f t="shared" si="10"/>
-        <v>5.5</v>
-      </c>
-      <c r="G75" s="13">
-        <f t="shared" si="10"/>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
-        <v>98</v>
-      </c>
-      <c r="D76" s="4">
-        <v>2</v>
-      </c>
-      <c r="E76" s="13">
-        <f t="shared" si="10"/>
-        <v>2.75</v>
-      </c>
-      <c r="F76" s="13">
-        <f t="shared" si="10"/>
-        <v>2.75</v>
-      </c>
-      <c r="G76" s="13">
-        <f t="shared" si="10"/>
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>141</v>
-      </c>
-      <c r="D77" s="4">
-        <v>3</v>
-      </c>
-      <c r="E77" s="13">
-        <f t="shared" si="10"/>
-        <v>1.8333333333333333</v>
-      </c>
-      <c r="F77" s="13">
-        <f t="shared" si="10"/>
-        <v>1.8333333333333333</v>
-      </c>
-      <c r="G77" s="13">
-        <f t="shared" si="10"/>
-        <v>1.8333333333333333</v>
-      </c>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
-        <v>99</v>
-      </c>
-      <c r="D78" s="4">
-        <v>4</v>
-      </c>
-      <c r="E78" s="13">
-        <f t="shared" si="10"/>
-        <v>1.375</v>
-      </c>
-      <c r="F78" s="13">
-        <f t="shared" si="10"/>
-        <v>1.375</v>
-      </c>
-      <c r="G78" s="13">
-        <f t="shared" si="10"/>
-        <v>1.375</v>
-      </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>142</v>
-      </c>
-      <c r="D79" s="4">
-        <v>5</v>
-      </c>
-      <c r="E79" s="13">
-        <f t="shared" si="10"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F79" s="13">
-        <f t="shared" si="10"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G79" s="13">
-        <f t="shared" si="10"/>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
-        <v>100</v>
-      </c>
-      <c r="D80" s="4">
-        <v>6</v>
-      </c>
-      <c r="E80" s="13">
-        <f t="shared" si="10"/>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="F80" s="13">
-        <f t="shared" si="10"/>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="G80" s="13">
-        <f t="shared" si="10"/>
-        <v>0.91666666666666663</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>103</v>
-      </c>
-      <c r="C82" t="s">
-        <v>104</v>
-      </c>
-      <c r="E82" s="7" t="e">
-        <f>E64+E73</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F82" s="7" t="e">
-        <f t="shared" ref="F82:G82" si="11">F64+F73</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G82" s="7" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
-        <v>143</v>
-      </c>
-      <c r="E83" s="7">
-        <f t="shared" ref="E83:G83" si="12">E65+E74</f>
-        <v>12.140099944098084</v>
-      </c>
-      <c r="F83" s="7">
-        <f t="shared" si="12"/>
-        <v>11.715178622223414</v>
-      </c>
-      <c r="G83" s="7">
-        <f t="shared" si="12"/>
-        <v>11.86686968575701</v>
-      </c>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E84" s="7">
-        <f t="shared" ref="E84:G84" si="13">E66+E75</f>
-        <v>6.7797177568272815</v>
+        <f t="shared" ref="E84:G90" si="17">E65+E75</f>
+        <v>12.140099944098084</v>
       </c>
       <c r="F84" s="7">
-        <f t="shared" si="13"/>
-        <v>6.2677199521396503</v>
+        <f t="shared" si="17"/>
+        <v>11.715178622223414</v>
       </c>
       <c r="G84" s="7">
-        <f t="shared" si="13"/>
-        <v>6.4452848828213334</v>
+        <f t="shared" si="17"/>
+        <v>11.86686968575701</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="E85" s="7">
-        <f t="shared" ref="E85:G85" si="14">E67+E76</f>
-        <v>4.4448154446981656</v>
+        <f t="shared" si="17"/>
+        <v>6.7797177568272815</v>
       </c>
       <c r="F85" s="7">
-        <f t="shared" si="14"/>
-        <v>3.649951698537599</v>
+        <f t="shared" si="17"/>
+        <v>6.2677199521396503</v>
       </c>
       <c r="G85" s="7">
-        <f t="shared" si="14"/>
-        <v>3.9040753011610505</v>
+        <f t="shared" si="17"/>
+        <v>6.4452848828213334</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="E86" s="7">
-        <f t="shared" ref="E86:G86" si="15">E68+E77</f>
-        <v>4.3418171136638399</v>
+        <f t="shared" si="17"/>
+        <v>4.4448154446981656</v>
       </c>
       <c r="F86" s="7">
-        <f t="shared" si="15"/>
-        <v>2.9205460757364676</v>
+        <f t="shared" si="17"/>
+        <v>3.649951698537599</v>
       </c>
       <c r="G86" s="7">
-        <f t="shared" si="15"/>
-        <v>3.3145799528756426</v>
+        <f t="shared" si="17"/>
+        <v>3.9040753011610505</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="E87" s="7">
-        <f t="shared" ref="E87:G87" si="16">E69+E78</f>
-        <v>6.1998663701413648</v>
+        <f t="shared" si="17"/>
+        <v>4.3418171136638399</v>
       </c>
       <c r="F87" s="7">
-        <f t="shared" si="16"/>
-        <v>2.7478802921481256</v>
+        <f t="shared" si="17"/>
+        <v>2.9205460757364676</v>
       </c>
       <c r="G87" s="7">
-        <f t="shared" si="16"/>
-        <v>3.4423139495535828</v>
+        <f t="shared" si="17"/>
+        <v>3.3145799528756426</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="E88" s="7">
-        <f t="shared" ref="E88:G88" si="17">E70+E79</f>
-        <v>64.103768998110255</v>
+        <f t="shared" si="17"/>
+        <v>6.1998663701413648</v>
       </c>
       <c r="F88" s="7">
         <f t="shared" si="17"/>
-        <v>2.9621694211248002</v>
+        <v>2.7478802921481256</v>
       </c>
       <c r="G88" s="7">
         <f t="shared" si="17"/>
-        <v>4.5207692639014532</v>
+        <v>3.4423139495535828</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="E89" s="7">
-        <f t="shared" ref="E89:G89" si="18">E71+E80</f>
+        <f t="shared" si="17"/>
+        <v>64.103768998110255</v>
+      </c>
+      <c r="F89" s="7">
+        <f t="shared" si="17"/>
+        <v>2.9621694211248002</v>
+      </c>
+      <c r="G89" s="7">
+        <f t="shared" si="17"/>
+        <v>4.5207692639014532</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>105</v>
+      </c>
+      <c r="E90" s="31">
+        <f t="shared" si="17"/>
         <v>-4.780836044509007</v>
       </c>
-      <c r="F89" s="7">
-        <f t="shared" si="18"/>
+      <c r="F90" s="7">
+        <f t="shared" si="17"/>
         <v>3.8100135056357334</v>
       </c>
-      <c r="G89" s="7">
-        <f t="shared" si="18"/>
+      <c r="G90" s="7">
+        <f t="shared" si="17"/>
         <v>10.823115462974517</v>
-      </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
-        <v>108</v>
-      </c>
-      <c r="E91" s="7" t="e">
-        <f>E64/E82</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F91" s="7" t="e">
-        <f>F64/F82</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G91" s="7" t="e">
-        <f>G64/G82</f>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>147</v>
-      </c>
-      <c r="E92" s="7">
-        <f t="shared" ref="E92:G92" si="19">E65/E83</f>
-        <v>9.3911907591201049E-2</v>
-      </c>
-      <c r="F92" s="7">
-        <f t="shared" si="19"/>
-        <v>6.1047180353420986E-2</v>
-      </c>
-      <c r="G92" s="7">
-        <f t="shared" si="19"/>
-        <v>7.3049566457905446E-2</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E93" s="7">
-        <f t="shared" ref="E93:G93" si="20">E66/E84</f>
-        <v>0.18875678940153306</v>
+        <f t="shared" ref="E93:G98" si="18">E65/E84</f>
+        <v>9.3911907591201049E-2</v>
       </c>
       <c r="F93" s="7">
-        <f t="shared" si="20"/>
-        <v>0.12248791554216919</v>
+        <f t="shared" si="18"/>
+        <v>6.1047180353420986E-2</v>
       </c>
       <c r="G93" s="7">
-        <f t="shared" si="20"/>
-        <v>0.14666301024812861</v>
+        <f t="shared" si="18"/>
+        <v>7.3049566457905446E-2</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="E94" s="7">
-        <f t="shared" ref="E94:G94" si="21">E67/E85</f>
-        <v>0.38130164588042986</v>
+        <f t="shared" si="18"/>
+        <v>0.18875678940153306</v>
       </c>
       <c r="F94" s="7">
-        <f t="shared" si="21"/>
-        <v>0.2465653720563416</v>
+        <f t="shared" si="18"/>
+        <v>0.12248791554216919</v>
       </c>
       <c r="G94" s="7">
-        <f t="shared" si="21"/>
-        <v>0.29560784875687074</v>
+        <f t="shared" si="18"/>
+        <v>0.14666301024812861</v>
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="E95" s="7">
-        <f t="shared" ref="E95:G95" si="22">E68/E86</f>
-        <v>0.57774975653309446</v>
+        <f t="shared" si="18"/>
+        <v>0.38130164588042986</v>
       </c>
       <c r="F95" s="7">
-        <f t="shared" si="22"/>
-        <v>0.37226351312706968</v>
+        <f t="shared" si="18"/>
+        <v>0.2465653720563416</v>
       </c>
       <c r="G95" s="7">
-        <f t="shared" si="22"/>
-        <v>0.44688818510991685</v>
+        <f t="shared" si="18"/>
+        <v>0.29560784875687074</v>
       </c>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
-        <v>110</v>
-      </c>
-      <c r="D96" s="20"/>
+        <v>146</v>
+      </c>
       <c r="E96" s="7">
-        <f t="shared" ref="E96:G96" si="23">E69/E87</f>
-        <v>0.77822102640437263</v>
+        <f t="shared" si="18"/>
+        <v>0.57774975653309446</v>
       </c>
       <c r="F96" s="7">
-        <f t="shared" si="23"/>
-        <v>0.49961430127470774</v>
+        <f t="shared" si="18"/>
+        <v>0.37226351312706968</v>
       </c>
       <c r="G96" s="7">
-        <f t="shared" si="23"/>
-        <v>0.60055938530001973</v>
+        <f t="shared" si="18"/>
+        <v>0.44688818510991685</v>
       </c>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="D97" s="20"/>
       <c r="E97" s="7">
-        <f t="shared" ref="E97:G97" si="24">E70/E88</f>
-        <v>0.98284032253965559</v>
+        <f t="shared" si="18"/>
+        <v>0.77822102640437263</v>
       </c>
       <c r="F97" s="7">
-        <f t="shared" si="24"/>
-        <v>0.62865054505143514</v>
+        <f t="shared" si="18"/>
+        <v>0.49961430127470774</v>
       </c>
       <c r="G97" s="7">
-        <f t="shared" si="24"/>
-        <v>0.756678579288806</v>
+        <f t="shared" si="18"/>
+        <v>0.60055938530001973</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="D98" s="20"/>
-      <c r="E98" s="7" t="s">
-        <v>118</v>
+      <c r="E98" s="7">
+        <f t="shared" si="18"/>
+        <v>0.98284032253965559</v>
       </c>
       <c r="F98" s="7">
-        <f t="shared" ref="F98:G98" si="25">F71/F89</f>
+        <f t="shared" si="18"/>
+        <v>0.62865054505143514</v>
+      </c>
+      <c r="G98" s="7">
+        <f t="shared" si="18"/>
+        <v>0.756678579288806</v>
+      </c>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>109</v>
+      </c>
+      <c r="D99" s="20"/>
+      <c r="E99" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="F99" s="7">
+        <f>F71/F90</f>
         <v>0.759405927220273</v>
       </c>
-      <c r="G98" s="7">
-        <f t="shared" si="25"/>
+      <c r="G99" s="7">
+        <f>G71/G90</f>
         <v>0.9153047318212072</v>
       </c>
-    </row>
-    <row r="99" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D99" s="20"/>
-      <c r="E99" s="7"/>
-      <c r="F99" s="7"/>
-      <c r="G99" s="7"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D100" s="20"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="7"/>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C101" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D101" s="14">
+      <c r="D101" s="20"/>
+    </row>
+    <row r="102" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C102" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D102" s="14">
         <v>0</v>
       </c>
-      <c r="E101" s="15" t="e">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E91</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F101" s="15" t="e">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F91</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G101" s="15" t="e">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G91</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="102" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C102" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="D102" s="23">
-        <v>500</v>
-      </c>
-      <c r="E102" s="24">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E92</f>
-        <v>18.233350924752401</v>
-      </c>
-      <c r="F102" s="24">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F92</f>
-        <v>28.049268732971569</v>
-      </c>
-      <c r="G102" s="24">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G92</f>
-        <v>23.440642431601713</v>
-      </c>
+      <c r="E102" s="15"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="15"/>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C103" s="23" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D103" s="23">
-        <v>1000</v>
+        <v>0.5</v>
       </c>
       <c r="E103" s="24">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E93</f>
+        <f t="shared" ref="E103:G108" si="19">Engine_spec_d_life__h/Hours_in_a_year__h/E93</f>
+        <v>18.233350924752401</v>
+      </c>
+      <c r="F103" s="24">
+        <f t="shared" si="19"/>
+        <v>28.049268732971569</v>
+      </c>
+      <c r="G103" s="24">
+        <f t="shared" si="19"/>
+        <v>23.440642431601713</v>
+      </c>
+    </row>
+    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C104" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="D104" s="23">
+        <v>1</v>
+      </c>
+      <c r="E104" s="24">
+        <f t="shared" si="19"/>
         <v>9.0716141790308509</v>
       </c>
-      <c r="F103" s="24">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F93</f>
+      <c r="F104" s="24">
+        <f t="shared" si="19"/>
         <v>13.979573083140437</v>
       </c>
-      <c r="G103" s="24">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G93</f>
+      <c r="G104" s="24">
+        <f t="shared" si="19"/>
         <v>11.675259932455509</v>
-      </c>
-    </row>
-    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C104" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D104" s="14">
-        <v>2000</v>
-      </c>
-      <c r="E104" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E94</f>
-        <v>4.4907458061700751</v>
-      </c>
-      <c r="F104" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F94</f>
-        <v>6.9447252582248682</v>
-      </c>
-      <c r="G104" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G94</f>
-        <v>5.7925686828824041</v>
       </c>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C105" s="14" t="s">
-        <v>153</v>
+        <v>113</v>
       </c>
       <c r="D105" s="14">
-        <v>3000</v>
+        <v>2</v>
       </c>
       <c r="E105" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E95</f>
-        <v>2.9637896818831506</v>
+        <f t="shared" si="19"/>
+        <v>4.4907458061700751</v>
       </c>
       <c r="F105" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F95</f>
-        <v>4.5997759832530125</v>
+        <f t="shared" si="19"/>
+        <v>6.9447252582248682</v>
       </c>
       <c r="G105" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G95</f>
-        <v>3.8316715996913686</v>
+        <f t="shared" si="19"/>
+        <v>5.7925686828824041</v>
       </c>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C106" s="14" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="D106" s="14">
-        <v>4000</v>
+        <v>3</v>
       </c>
       <c r="E106" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E96</f>
-        <v>2.2003116197396881</v>
+        <f t="shared" si="19"/>
+        <v>2.9637896818831506</v>
       </c>
       <c r="F106" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F96</f>
-        <v>3.4273013457670847</v>
+        <f t="shared" si="19"/>
+        <v>4.5997759832530125</v>
       </c>
       <c r="G106" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G96</f>
-        <v>2.8512230580958526</v>
+        <f t="shared" si="19"/>
+        <v>3.8316715996913686</v>
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C107" s="14" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="D107" s="14">
-        <v>5000</v>
+        <v>4</v>
       </c>
       <c r="E107" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/E97</f>
-        <v>1.7422247824536103</v>
+        <f t="shared" si="19"/>
+        <v>2.2003116197396881</v>
       </c>
       <c r="F107" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F97</f>
-        <v>2.7238165632755282</v>
+        <f t="shared" si="19"/>
+        <v>3.4273013457670847</v>
       </c>
       <c r="G107" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G97</f>
-        <v>2.262953933138542</v>
+        <f t="shared" si="19"/>
+        <v>2.8512230580958526</v>
       </c>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C108" s="14" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="D108" s="14">
-        <v>6000</v>
-      </c>
-      <c r="E108" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E108" s="15">
+        <f t="shared" si="19"/>
+        <v>1.7422247824536103</v>
+      </c>
+      <c r="F108" s="15">
+        <f t="shared" si="19"/>
+        <v>2.7238165632755282</v>
+      </c>
+      <c r="G108" s="15">
+        <f t="shared" si="19"/>
+        <v>2.262953933138542</v>
+      </c>
+    </row>
+    <row r="109" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C109" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D109" s="14">
+        <v>6</v>
+      </c>
+      <c r="E109" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="F109" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F99</f>
+        <v>2.2548267082811564</v>
+      </c>
+      <c r="G109" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G99</f>
+        <v>1.8707745165003349</v>
+      </c>
+    </row>
+    <row r="110" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C110" s="14"/>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="14"/>
+      <c r="G110" s="14"/>
+    </row>
+    <row r="111" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C111" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="F108" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F98</f>
-        <v>2.2548267082811564</v>
-      </c>
-      <c r="G108" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G98</f>
-        <v>1.8707745165003349</v>
-      </c>
-    </row>
-    <row r="109" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C109" s="14"/>
-      <c r="D109" s="14"/>
-      <c r="E109" s="14"/>
-      <c r="F109" s="14"/>
-      <c r="G109" s="14"/>
-    </row>
-    <row r="110" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C110" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D110" s="14">
+      <c r="D111" s="14">
         <v>0</v>
       </c>
-      <c r="E110" s="16" t="e">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E82)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F110" s="16" t="e">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F82)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G110" s="16" t="e">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G82)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="111" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C111" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="D111" s="23">
-        <v>500</v>
-      </c>
-      <c r="E111" s="24">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E83)</f>
-        <v>10.393921185015483</v>
-      </c>
-      <c r="F111" s="24">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F83)</f>
-        <v>10.030118683410457</v>
-      </c>
-      <c r="G111" s="24">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G83)</f>
-        <v>10.159991169312509</v>
-      </c>
+      <c r="E111" s="16"/>
+      <c r="F111" s="16"/>
+      <c r="G111" s="16"/>
     </row>
     <row r="112" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C112" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D112" s="23">
-        <v>1000</v>
+        <v>0.5</v>
       </c>
       <c r="E112" s="24">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E84)</f>
+        <f t="shared" ref="E112:G117" si="20">Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E84)</f>
+        <v>10.393921185015483</v>
+      </c>
+      <c r="F112" s="24">
+        <f t="shared" si="20"/>
+        <v>10.030118683410457</v>
+      </c>
+      <c r="G112" s="24">
+        <f t="shared" si="20"/>
+        <v>10.159991169312509</v>
+      </c>
+    </row>
+    <row r="113" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C113" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D113" s="23">
+        <v>1</v>
+      </c>
+      <c r="E113" s="24">
+        <f t="shared" si="20"/>
         <v>5.8045528739959602</v>
       </c>
-      <c r="F112" s="24">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F84)</f>
+      <c r="F113" s="24">
+        <f t="shared" si="20"/>
         <v>5.3661985891606596</v>
       </c>
-      <c r="G112" s="24">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G84)</f>
+      <c r="G113" s="24">
+        <f t="shared" si="20"/>
         <v>5.5182233585799088</v>
-      </c>
-    </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C113" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="D113" s="14">
-        <v>2000</v>
-      </c>
-      <c r="E113" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E85)</f>
-        <v>3.8054926752552789</v>
-      </c>
-      <c r="F113" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F85)</f>
-        <v>3.1249586460082184</v>
-      </c>
-      <c r="G113" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G85)</f>
-        <v>3.34253022359679</v>
       </c>
     </row>
     <row r="114" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C114" s="14" t="s">
-        <v>157</v>
+        <v>119</v>
       </c>
       <c r="D114" s="14">
-        <v>3000</v>
+        <v>2</v>
       </c>
       <c r="E114" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E86)</f>
-        <v>3.717309172657397</v>
+        <f t="shared" si="20"/>
+        <v>3.8054926752552789</v>
       </c>
       <c r="F114" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F86)</f>
-        <v>2.5004675305962909</v>
+        <f t="shared" si="20"/>
+        <v>3.1249586460082184</v>
       </c>
       <c r="G114" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G86)</f>
-        <v>2.837825302119557</v>
+        <f t="shared" si="20"/>
+        <v>3.34253022359679</v>
       </c>
     </row>
     <row r="115" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C115" s="14" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="D115" s="14">
-        <v>4000</v>
+        <v>3</v>
       </c>
       <c r="E115" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E87)</f>
-        <v>5.3081047689566478</v>
+        <f t="shared" si="20"/>
+        <v>3.717309172657397</v>
       </c>
       <c r="F115" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F87)</f>
-        <v>2.3526372364281896</v>
+        <f t="shared" si="20"/>
+        <v>2.5004675305962909</v>
       </c>
       <c r="G115" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G87)</f>
-        <v>2.9471866006451912</v>
+        <f t="shared" si="20"/>
+        <v>2.837825302119557</v>
       </c>
     </row>
     <row r="116" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C116" s="14" t="s">
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="D116" s="14">
-        <v>5000</v>
+        <v>4</v>
       </c>
       <c r="E116" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E88)</f>
-        <v>54.883363868245084</v>
+        <f t="shared" si="20"/>
+        <v>5.3081047689566478</v>
       </c>
       <c r="F116" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F88)</f>
-        <v>2.5361039564424659</v>
+        <f t="shared" si="20"/>
+        <v>2.3526372364281896</v>
       </c>
       <c r="G116" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G88)</f>
-        <v>3.8705216300526137</v>
+        <f t="shared" si="20"/>
+        <v>2.9471866006451912</v>
       </c>
     </row>
     <row r="117" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C117" s="14" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="D117" s="14">
-        <v>6000</v>
-      </c>
-      <c r="E117" s="15" t="s">
-        <v>118</v>
+        <v>5</v>
+      </c>
+      <c r="E117" s="15">
+        <f t="shared" si="20"/>
+        <v>54.883363868245084</v>
       </c>
       <c r="F117" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F89)</f>
+        <f t="shared" si="20"/>
+        <v>2.5361039564424659</v>
+      </c>
+      <c r="G117" s="15">
+        <f t="shared" si="20"/>
+        <v>3.8705216300526137</v>
+      </c>
+    </row>
+    <row r="118" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C118" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D118" s="14">
+        <v>6</v>
+      </c>
+      <c r="E118" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="F118" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F90)</f>
         <v>3.2619978644141554</v>
       </c>
-      <c r="G117" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G89)</f>
+      <c r="G118" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G90)</f>
         <v>9.2663659785740737</v>
-      </c>
-    </row>
-    <row r="119" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C119" t="s">
-        <v>126</v>
-      </c>
-      <c r="E119" s="4" t="e">
-        <f>(Engine_service_interval__h/E91)/24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F119" s="4" t="e">
-        <f>(Engine_service_interval__h/F91)/24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G119" s="4" t="e">
-        <f>(Engine_service_interval__h/G91)/24</f>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="120" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C120" t="s">
-        <v>159</v>
-      </c>
-      <c r="E120" s="7">
-        <f>(Engine_service_interval__h/E92)/24</f>
+        <v>123</v>
+      </c>
+      <c r="D120" s="20">
+        <v>0</v>
+      </c>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
+    </row>
+    <row r="121" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C121" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="D121" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E121" s="24">
+        <f t="shared" ref="E121:G126" si="21">(Engine_service_interval__h/E93)/24</f>
         <v>443.67820583564179</v>
       </c>
-      <c r="F120" s="7">
-        <f>(Engine_service_interval__h/F92)/24</f>
+      <c r="F121" s="24">
+        <f t="shared" si="21"/>
         <v>682.53220583564155</v>
       </c>
-      <c r="G120" s="7">
-        <f>(Engine_service_interval__h/G92)/24</f>
+      <c r="G121" s="24">
+        <f t="shared" si="21"/>
         <v>570.38896583564167</v>
       </c>
     </row>
-    <row r="121" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C121" t="s">
-        <v>160</v>
-      </c>
-      <c r="E121" s="7">
-        <f>(Engine_service_interval__h/E93)/24</f>
+    <row r="122" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C122" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D122" s="23">
+        <v>1</v>
+      </c>
+      <c r="E122" s="24">
+        <f t="shared" si="21"/>
         <v>220.7426116897507</v>
       </c>
-      <c r="F121" s="7">
-        <f>(Engine_service_interval__h/F93)/24</f>
+      <c r="F122" s="24">
+        <f t="shared" si="21"/>
         <v>340.16961168975064</v>
       </c>
-      <c r="G121" s="7">
-        <f>(Engine_service_interval__h/G93)/24</f>
+      <c r="G122" s="24">
+        <f t="shared" si="21"/>
         <v>284.0979916897507</v>
-      </c>
-    </row>
-    <row r="122" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C122" t="s">
-        <v>127</v>
-      </c>
-      <c r="E122" s="7">
-        <f>(Engine_service_interval__h/E94)/24</f>
-        <v>109.27481461680516</v>
-      </c>
-      <c r="F122" s="7">
-        <f>(Engine_service_interval__h/F94)/24</f>
-        <v>168.98831461680513</v>
-      </c>
-      <c r="G122" s="7">
-        <f>(Engine_service_interval__h/G94)/24</f>
-        <v>140.95250461680516</v>
       </c>
     </row>
     <row r="123" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
-        <v>161</v>
+        <v>124</v>
+      </c>
+      <c r="D123" s="20">
+        <v>2</v>
       </c>
       <c r="E123" s="7">
-        <f>(Engine_service_interval__h/E95)/24</f>
-        <v>72.118882259156663</v>
+        <f t="shared" si="21"/>
+        <v>109.27481461680516</v>
       </c>
       <c r="F123" s="7">
-        <f>(Engine_service_interval__h/F95)/24</f>
-        <v>111.92788225915665</v>
+        <f t="shared" si="21"/>
+        <v>168.98831461680513</v>
       </c>
       <c r="G123" s="7">
-        <f>(Engine_service_interval__h/G95)/24</f>
-        <v>93.237342259156648</v>
+        <f t="shared" si="21"/>
+        <v>140.95250461680516</v>
       </c>
     </row>
     <row r="124" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
-        <v>128</v>
+        <v>158</v>
+      </c>
+      <c r="D124" s="20">
+        <v>3</v>
       </c>
       <c r="E124" s="7">
-        <f>(Engine_service_interval__h/E96)/24</f>
-        <v>53.540916080332408</v>
+        <f t="shared" si="21"/>
+        <v>72.118882259156663</v>
       </c>
       <c r="F124" s="7">
-        <f>(Engine_service_interval__h/F96)/24</f>
-        <v>83.397666080332399</v>
+        <f t="shared" si="21"/>
+        <v>111.92788225915665</v>
       </c>
       <c r="G124" s="7">
-        <f>(Engine_service_interval__h/G96)/24</f>
-        <v>69.379761080332415</v>
+        <f t="shared" si="21"/>
+        <v>93.237342259156648</v>
       </c>
     </row>
     <row r="125" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C125" t="s">
-        <v>162</v>
+        <v>125</v>
+      </c>
+      <c r="D125" s="20">
+        <v>4</v>
       </c>
       <c r="E125" s="7">
-        <f>(Engine_service_interval__h/E97)/24</f>
-        <v>42.394136373037853</v>
+        <f t="shared" si="21"/>
+        <v>53.540916080332408</v>
       </c>
       <c r="F125" s="7">
-        <f>(Engine_service_interval__h/F97)/24</f>
-        <v>66.279536373037857</v>
+        <f t="shared" si="21"/>
+        <v>83.397666080332399</v>
       </c>
       <c r="G125" s="7">
-        <f>(Engine_service_interval__h/G97)/24</f>
-        <v>55.065212373037859</v>
+        <f t="shared" si="21"/>
+        <v>69.379761080332415</v>
       </c>
     </row>
     <row r="126" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
-        <v>129</v>
-      </c>
-      <c r="E126" s="7" t="s">
-        <v>118</v>
+        <v>159</v>
+      </c>
+      <c r="D126" s="20">
+        <v>5</v>
+      </c>
+      <c r="E126" s="7">
+        <f t="shared" si="21"/>
+        <v>42.394136373037853</v>
       </c>
       <c r="F126" s="7">
-        <f>(Engine_service_interval__h/F98)/24</f>
+        <f t="shared" si="21"/>
+        <v>66.279536373037857</v>
+      </c>
+      <c r="G126" s="7">
+        <f t="shared" si="21"/>
+        <v>55.065212373037859</v>
+      </c>
+    </row>
+    <row r="127" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C127" t="s">
+        <v>126</v>
+      </c>
+      <c r="D127" s="20">
+        <v>6</v>
+      </c>
+      <c r="E127" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="F127" s="7">
+        <f>(Engine_service_interval__h/F99)/24</f>
         <v>54.867449901508138</v>
       </c>
-      <c r="G126" s="7">
-        <f>(Engine_service_interval__h/G98)/24</f>
+      <c r="G127" s="7">
+        <f>(Engine_service_interval__h/G99)/24</f>
         <v>45.522179901508146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Using Beckett's reported cycle life at 50% DOD from Boston Power, 10k cycles, instead of my earlier estimate of 7500. Also, changed cycle energy to average cycle energy over life of batteries. In other words, if end of life batteries have 80% nameplate capacity, then the average cycle energy over the lifetime of the batteries is 90% of nameplate capacity.
</commit_message>
<xml_diff>
--- a/Control and Data Systems/BMs Hygen System Design Calcs.xlsx
+++ b/Control and Data Systems/BMs Hygen System Design Calcs.xlsx
@@ -12,20 +12,22 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="Avg_bank_energy_over_lifetime">'Hygen Use Models'!$D$18</definedName>
     <definedName name="Batt_bank_energy__kWh">'Hygen Use Models'!$D$16</definedName>
-    <definedName name="Batt_Cycles_50__DOD__guesstimated">'Hygen Use Models'!$D$20</definedName>
-    <definedName name="Batt_Cycles_80__DOD">'Hygen Use Models'!$D$19</definedName>
+    <definedName name="Batt_Cycles_50__DOD__guesstimated">'Hygen Use Models'!$D$22</definedName>
+    <definedName name="Batt_Cycles_80__DOD">'Hygen Use Models'!$D$21</definedName>
+    <definedName name="Batt_end_of_life_definition__capacity_degradation">'Hygen Use Models'!$D$17</definedName>
     <definedName name="Beckett_module_nominal_energy__kWh">'Hygen Use Models'!$D$14</definedName>
-    <definedName name="Cycle_energy__kWh">'Hygen Use Models'!$D$18</definedName>
-    <definedName name="Depth_of_Discharge">'Hygen Use Models'!$D$17</definedName>
-    <definedName name="Diesel_cost____l">'Hygen Use Models'!$G$20</definedName>
+    <definedName name="Cycle_energy__kWh">'Hygen Use Models'!$D$20</definedName>
+    <definedName name="Depth_of_Discharge">'Hygen Use Models'!$D$19</definedName>
+    <definedName name="Diesel_cost____l">'Hygen Use Models'!$G$22</definedName>
     <definedName name="Engine_service_interval__h">'Hygen Use Models'!$G$16</definedName>
     <definedName name="Engine_spec_d_life__h">'Hygen Use Models'!$G$14</definedName>
     <definedName name="Format_Parallel">'Beckett Battery Modules'!$H$7</definedName>
     <definedName name="Format_Parallel_Stack">'Beckett Battery Modules'!$N$7</definedName>
     <definedName name="Format_Series">'Beckett Battery Modules'!$H$6</definedName>
     <definedName name="Format_Series_Stack">'Beckett Battery Modules'!$N$6</definedName>
-    <definedName name="Fuel_Tank_Capacity__l">'Hygen Use Models'!$G$19</definedName>
+    <definedName name="Fuel_Tank_Capacity__l">'Hygen Use Models'!$G$21</definedName>
     <definedName name="Hours_in_a_year__h">'Hygen Use Models'!$G$15</definedName>
     <definedName name="Max_charge_rate">'Beckett Battery Modules'!$C$9</definedName>
     <definedName name="Max_discharge_rate">'Beckett Battery Modules'!$C$10</definedName>
@@ -35,7 +37,7 @@
     <definedName name="Nominal_Energy_Module">'Beckett Battery Modules'!$H$9</definedName>
     <definedName name="Nominal_Voltage">'Beckett Battery Modules'!$C$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Hygen Use Models'!$B$1:$P$127</definedName>
-    <definedName name="SFC__l_kWh">'Hygen Use Models'!$G$18</definedName>
+    <definedName name="SFC__l_kWh">'Hygen Use Models'!$G$20</definedName>
     <definedName name="Stack_height">'Hygen Use Models'!$D$15</definedName>
     <definedName name="Voltage_at_0">'Beckett Battery Modules'!$B$11:$C$11</definedName>
     <definedName name="Voltage_at_100">'Beckett Battery Modules'!$B$14:$C$14</definedName>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="172">
   <si>
     <t>Boston Swing 5300</t>
   </si>
@@ -557,6 +559,12 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>Batt end of life definition, capacity degradation</t>
+  </si>
+  <si>
+    <t>Avg bank energy over lifetime</t>
   </si>
 </sst>
 </file>
@@ -739,8 +747,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF99"/>
       <color rgb="FFFF9999"/>
-      <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
   <extLst>
@@ -815,7 +823,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hygen Use Models'!$D$103:$D$109</c:f>
+              <c:f>'Hygen Use Models'!$D$105:$D$111</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -845,27 +853,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hygen Use Models'!$G$103:$G$109</c:f>
+              <c:f>'Hygen Use Models'!$G$105:$G$111</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>23.440642431601713</c:v>
+                  <c:v>23.440642431601717</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.675259932455509</c:v>
+                  <c:v>11.675259932455507</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.7925686828824041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8316715996913686</c:v>
+                  <c:v>3.8316715996913695</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.8512230580958526</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.262953933138542</c:v>
+                  <c:v>2.2629539331385415</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.8707745165003349</c:v>
@@ -883,7 +891,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hygen Use Models'!$D$112:$D$118</c:f>
+              <c:f>'Hygen Use Models'!$D$114:$D$120</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -913,30 +921,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hygen Use Models'!$G$112:$G$118</c:f>
+              <c:f>'Hygen Use Models'!$G$114:$G$120</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10.159991169312509</c:v>
+                  <c:v>12.191989403175011</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5182233585799088</c:v>
+                  <c:v>6.6218680302958912</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.34253022359679</c:v>
+                  <c:v>4.0110362683161478</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.837825302119557</c:v>
+                  <c:v>3.4053903625434692</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9471866006451912</c:v>
+                  <c:v>3.5366239207742294</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.8705216300526137</c:v>
+                  <c:v>4.6446259560631358</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.2663659785740737</c:v>
+                  <c:v>11.119639174288887</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -951,11 +959,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="100256000"/>
-        <c:axId val="109233280"/>
+        <c:axId val="40146048"/>
+        <c:axId val="40147968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100256000"/>
+        <c:axId val="40146048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -985,12 +993,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109233280"/>
+        <c:crossAx val="40147968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109233280"/>
+        <c:axId val="40147968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,7 +1028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100256000"/>
+        <c:crossAx val="40146048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1181,8 +1189,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="99794304"/>
-        <c:axId val="99800576"/>
+        <c:axId val="39982592"/>
+        <c:axId val="39984512"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -1274,11 +1282,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="99804672"/>
-        <c:axId val="99802496"/>
+        <c:axId val="39992704"/>
+        <c:axId val="39990784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99794304"/>
+        <c:axId val="39982592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,12 +1316,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99800576"/>
+        <c:crossAx val="39984512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99800576"/>
+        <c:axId val="39984512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1343,12 +1351,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99794304"/>
+        <c:crossAx val="39982592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99802496"/>
+        <c:axId val="39990784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="270"/>
@@ -1379,13 +1387,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99804672"/>
+        <c:crossAx val="39992704"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99804672"/>
+        <c:axId val="39992704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1395,7 +1403,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99802496"/>
+        <c:crossAx val="39990784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1538,8 +1546,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="99824000"/>
-        <c:axId val="99825920"/>
+        <c:axId val="40036608"/>
+        <c:axId val="40038784"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -1641,7 +1649,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="1">
-                  <c:v>570.38896583564167</c:v>
+                  <c:v>570.38896583564178</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>284.0979916897507</c:v>
@@ -1662,11 +1670,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="99834112"/>
-        <c:axId val="99832192"/>
+        <c:axId val="40128896"/>
+        <c:axId val="40040704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99824000"/>
+        <c:axId val="40036608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -1697,13 +1705,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99825920"/>
+        <c:crossAx val="40038784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99825920"/>
+        <c:axId val="40038784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1733,12 +1741,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99824000"/>
+        <c:crossAx val="40036608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99832192"/>
+        <c:axId val="40040704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="540"/>
@@ -1769,13 +1777,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99834112"/>
+        <c:crossAx val="40128896"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99834112"/>
+        <c:axId val="40128896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1785,7 +1793,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99832192"/>
+        <c:crossAx val="40040704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1877,7 +1885,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hygen Use Models'!$D$103:$D$105</c:f>
+              <c:f>'Hygen Use Models'!$D$105:$D$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1895,15 +1903,15 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hygen Use Models'!$G$103:$G$105</c:f>
+              <c:f>'Hygen Use Models'!$G$105:$G$107</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23.440642431601713</c:v>
+                  <c:v>23.440642431601717</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.675259932455509</c:v>
+                  <c:v>11.675259932455507</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.7925686828824041</c:v>
@@ -1921,7 +1929,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Hygen Use Models'!$D$112:$D$114</c:f>
+              <c:f>'Hygen Use Models'!$D$114:$D$116</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1939,18 +1947,18 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Hygen Use Models'!$G$112:$G$114</c:f>
+              <c:f>'Hygen Use Models'!$G$114:$G$116</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10.159991169312509</c:v>
+                  <c:v>12.191989403175011</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5182233585799088</c:v>
+                  <c:v>6.6218680302958912</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.34253022359679</c:v>
+                  <c:v>4.0110362683161478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1965,11 +1973,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="99847168"/>
-        <c:axId val="99857536"/>
+        <c:axId val="40211584"/>
+        <c:axId val="40213504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99847168"/>
+        <c:axId val="40211584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -2000,13 +2008,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99857536"/>
+        <c:crossAx val="40213504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99857536"/>
+        <c:axId val="40213504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2036,7 +2044,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99847168"/>
+        <c:crossAx val="40211584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2917,10 +2925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R127"/>
+  <dimension ref="B1:R129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2987,396 +2995,393 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="2">
+        <f>(1+D17)/2</f>
+        <v>0.9</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D19" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>88</v>
       </c>
-      <c r="D18">
-        <f>D17*Batt_bank_energy__kWh</f>
-        <v>5.5</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="D20">
+        <f>D19*Batt_bank_energy__kWh*Avg_bank_energy_over_lifetime</f>
+        <v>4.95</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G18">
+      <c r="G20">
         <v>0.38</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>117</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>3000</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F21" t="s">
         <v>161</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="1" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D20">
-        <f>D19*2.5</f>
-        <v>7500</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="D22">
+        <v>10000</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G22" s="25">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="19"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G27" s="32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="F26" s="1" t="s">
+    <row r="28" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G26" s="33" t="s">
+      <c r="G28" s="33" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="4">
-        <v>10.3</v>
-      </c>
-      <c r="F27" s="4">
-        <v>15.3</v>
-      </c>
-      <c r="G27" s="32">
-        <v>15.3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
-      <c r="C28" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="F28" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="G28" s="34">
-        <v>0.59</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="6">
-        <f>E27*E28</f>
-        <v>7.21</v>
-      </c>
-      <c r="F29" s="6">
-        <f t="shared" ref="F29:G29" si="0">F27*F28</f>
-        <v>10.709999999999999</v>
-      </c>
-      <c r="G29" s="35">
-        <f t="shared" si="0"/>
-        <v>9.0269999999999992</v>
+        <v>49</v>
+      </c>
+      <c r="E29" s="4">
+        <v>10.3</v>
+      </c>
+      <c r="F29" s="4">
+        <v>15.3</v>
+      </c>
+      <c r="G29" s="32">
+        <v>15.3</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" s="5">
-        <v>0.88</v>
+        <v>0.7</v>
       </c>
       <c r="F30" s="5">
-        <v>0.88</v>
+        <v>0.7</v>
       </c>
       <c r="G30" s="34">
-        <v>0.88</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E31" s="6">
-        <f>E30*E29</f>
-        <v>6.3448000000000002</v>
+        <f>E29*E30</f>
+        <v>7.21</v>
       </c>
       <c r="F31" s="6">
-        <f t="shared" ref="F31:G31" si="1">F30*F29</f>
-        <v>9.4247999999999994</v>
+        <f t="shared" ref="F31:G31" si="0">F29*F30</f>
+        <v>10.709999999999999</v>
       </c>
       <c r="G31" s="35">
-        <f t="shared" si="1"/>
-        <v>7.9437599999999993</v>
+        <f t="shared" si="0"/>
+        <v>9.0269999999999992</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E32" s="5">
-        <v>0.94</v>
+        <v>0.88</v>
       </c>
       <c r="F32" s="5">
-        <v>0.94</v>
+        <v>0.88</v>
       </c>
       <c r="G32" s="34">
-        <v>0.94</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="6">
+        <f>E32*E31</f>
+        <v>6.3448000000000002</v>
+      </c>
+      <c r="F33" s="6">
+        <f t="shared" ref="F33:G33" si="1">F32*F31</f>
+        <v>9.4247999999999994</v>
+      </c>
+      <c r="G33" s="35">
+        <f t="shared" si="1"/>
+        <v>7.9437599999999993</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0.94</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0.94</v>
+      </c>
+      <c r="G34" s="34">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="9">
-        <f>E32*E31</f>
+      <c r="E35" s="9">
+        <f>E34*E33</f>
         <v>5.9641120000000001</v>
       </c>
-      <c r="F33" s="6">
-        <f t="shared" ref="F33:G33" si="2">F32*F31</f>
+      <c r="F35" s="6">
+        <f t="shared" ref="F35:G35" si="2">F34*F33</f>
         <v>8.8593119999999992</v>
       </c>
-      <c r="G33" s="35">
+      <c r="G35" s="35">
         <f t="shared" si="2"/>
         <v>7.4671343999999991</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="F34" s="9">
-        <f>F33</f>
-        <v>8.8593119999999992</v>
-      </c>
-      <c r="G34" s="10">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
-      <c r="C35" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35" s="5">
-        <v>0.99</v>
-      </c>
-      <c r="F35" s="5">
-        <v>0.99</v>
-      </c>
-      <c r="G35" s="34">
-        <v>0.99</v>
-      </c>
-    </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
-      </c>
-      <c r="E36" s="6">
-        <f>E35*E33</f>
-        <v>5.9044708799999999</v>
-      </c>
-      <c r="F36" s="6">
-        <f>F35*F34</f>
-        <v>8.7707188799999987</v>
-      </c>
-      <c r="G36" s="35">
-        <f>G35*G34</f>
-        <v>7.4249999999999998</v>
+        <v>59</v>
+      </c>
+      <c r="E36" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="F36" s="9">
+        <f>F35</f>
+        <v>8.8593119999999992</v>
+      </c>
+      <c r="G36" s="10">
+        <v>7.5</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E37" s="5">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
       <c r="F37" s="5">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
       <c r="G37" s="34">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="6">
+        <f>E37*E35</f>
+        <v>5.9044708799999999</v>
+      </c>
+      <c r="F38" s="6">
+        <f>F37*F36</f>
+        <v>8.7707188799999987</v>
+      </c>
+      <c r="G38" s="35">
+        <f>G37*G36</f>
+        <v>7.4249999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="G39" s="34">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="6">
-        <f>E37*E36</f>
+      <c r="E40" s="6">
+        <f>E39*E38</f>
         <v>5.6092473359999993</v>
       </c>
-      <c r="F38" s="6">
-        <f t="shared" ref="F38:G38" si="3">F37*F36</f>
+      <c r="F40" s="6">
+        <f t="shared" ref="F40:G40" si="3">F39*F38</f>
         <v>8.3321829359999988</v>
       </c>
-      <c r="G38" s="35">
+      <c r="G40" s="35">
         <f t="shared" si="3"/>
         <v>7.0537499999999991</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>72</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E41" s="4">
         <v>0.5</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F41" s="4">
         <v>0.5</v>
       </c>
-      <c r="G39" s="32">
+      <c r="G41" s="32">
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
-      <c r="C40" t="s">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" t="s">
         <v>73</v>
       </c>
-      <c r="E40" s="5">
-        <f>E37</f>
+      <c r="E42" s="5">
+        <f>E39</f>
         <v>0.95</v>
       </c>
-      <c r="F40" s="5">
-        <f t="shared" ref="F40:G40" si="4">F37</f>
+      <c r="F42" s="5">
+        <f t="shared" ref="F42:G42" si="4">F39</f>
         <v>0.95</v>
       </c>
-      <c r="G40" s="34">
+      <c r="G42" s="34">
         <f t="shared" si="4"/>
         <v>0.95</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>68</v>
       </c>
-      <c r="E41" s="7">
-        <f>E39/E40</f>
+      <c r="E43" s="7">
+        <f>E41/E42</f>
         <v>0.52631578947368418</v>
       </c>
-      <c r="F41" s="7">
-        <f t="shared" ref="F41:G41" si="5">F39/F40</f>
+      <c r="F43" s="7">
+        <f t="shared" ref="F43:G43" si="5">F41/F42</f>
         <v>0.52631578947368418</v>
       </c>
-      <c r="G41" s="36">
+      <c r="G43" s="36">
         <f t="shared" si="5"/>
         <v>0.52631578947368418</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="8">
-        <f>E38-E41</f>
+      <c r="E44" s="8">
+        <f>E40-E43</f>
         <v>5.0829315465263152</v>
       </c>
-      <c r="F42" s="8">
-        <f t="shared" ref="F42:G42" si="6">F38-F41</f>
+      <c r="F44" s="8">
+        <f t="shared" ref="F44:G44" si="6">F40-F43</f>
         <v>7.8058671465263147</v>
       </c>
-      <c r="G42" s="37">
+      <c r="G44" s="37">
         <f t="shared" si="6"/>
         <v>6.527434210526315</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="4"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="4"/>
-      <c r="C44" t="s">
-        <v>127</v>
-      </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-    </row>
     <row r="45" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
-      <c r="C45" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -3398,116 +3403,95 @@
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="B46" s="4"/>
       <c r="C46" t="s">
-        <v>86</v>
-      </c>
-      <c r="D46" s="4">
-        <v>0</v>
-      </c>
-      <c r="E46" s="11">
-        <f>E$36-($D46+E$41)/E$37</f>
-        <v>5.3504542595013849</v>
-      </c>
-      <c r="F46" s="11">
-        <f t="shared" ref="F46:G53" si="7">F$36-($D46+F$41)/F$37</f>
-        <v>8.2167022595013837</v>
-      </c>
-      <c r="G46" s="11">
-        <f t="shared" si="7"/>
-        <v>6.8709833795013848</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
       <c r="H46" s="11"/>
       <c r="I46" s="4">
         <v>0</v>
       </c>
       <c r="J46" s="26">
-        <f t="shared" ref="J46:J53" si="8">$I46*24*30.5*SFC__l_kWh*Diesel_cost____l</f>
+        <f t="shared" ref="J46:J53" si="7">$I46*24*30.5*SFC__l_kWh*Diesel_cost____l</f>
         <v>0</v>
       </c>
       <c r="M46" s="4"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
-      <c r="C47" t="s">
-        <v>86</v>
-      </c>
-      <c r="D47" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E47" s="11">
-        <f t="shared" ref="E47:E48" si="9">E$36-($D47+E$41)/E$37</f>
-        <v>4.8241384700277008</v>
-      </c>
-      <c r="F47" s="11">
-        <f t="shared" si="7"/>
-        <v>7.6903864700276996</v>
-      </c>
-      <c r="G47" s="11">
-        <f t="shared" si="7"/>
-        <v>6.3446675900277008</v>
-      </c>
+      <c r="C47" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
       <c r="H47" s="11"/>
       <c r="I47" s="29">
         <v>0.5</v>
       </c>
       <c r="J47" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>139.08000000000001</v>
       </c>
       <c r="K47" s="30">
-        <f t="shared" ref="K47:K53" si="10">Fuel_Tank_Capacity__l/($I47*24*SFC__l_kWh)</f>
+        <f t="shared" ref="K47:K53" si="8">Fuel_Tank_Capacity__l/($I47*24*SFC__l_kWh)</f>
         <v>219.29824561403507</v>
       </c>
       <c r="L47" s="30">
-        <f t="shared" ref="L47:L53" si="11">K47/4</f>
+        <f t="shared" ref="L47:L53" si="9">K47/4</f>
         <v>54.824561403508767</v>
       </c>
       <c r="M47" s="24">
-        <f t="shared" ref="M47:M53" si="12">G121</f>
-        <v>570.38896583564167</v>
+        <f t="shared" ref="M47:M53" si="10">G123</f>
+        <v>570.38896583564178</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="4"/>
+      <c r="B48" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="C48" t="s">
         <v>86</v>
       </c>
       <c r="D48" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" s="11">
-        <f t="shared" si="9"/>
-        <v>4.2978226805540167</v>
+        <f>E$38-($D48+E$43)/E$39</f>
+        <v>5.3504542595013849</v>
       </c>
       <c r="F48" s="11">
-        <f t="shared" si="7"/>
-        <v>7.1640706805540155</v>
+        <f>F$38-($D48+F$43)/F$39</f>
+        <v>8.2167022595013837</v>
       </c>
       <c r="G48" s="11">
-        <f t="shared" si="7"/>
-        <v>5.8183518005540167</v>
+        <f>G$38-($D48+G$43)/G$39</f>
+        <v>6.8709833795013848</v>
       </c>
       <c r="H48" s="11"/>
       <c r="I48" s="29">
         <v>1</v>
       </c>
       <c r="J48" s="28">
+        <f t="shared" si="7"/>
+        <v>278.16000000000003</v>
+      </c>
+      <c r="K48" s="30">
         <f t="shared" si="8"/>
-        <v>278.16000000000003</v>
-      </c>
-      <c r="K48" s="30">
+        <v>109.64912280701753</v>
+      </c>
+      <c r="L48" s="30">
+        <f t="shared" si="9"/>
+        <v>27.412280701754383</v>
+      </c>
+      <c r="M48" s="24">
         <f t="shared" si="10"/>
-        <v>109.64912280701753</v>
-      </c>
-      <c r="L48" s="30">
-        <f t="shared" si="11"/>
-        <v>27.412280701754383</v>
-      </c>
-      <c r="M48" s="24">
-        <f t="shared" si="12"/>
         <v>284.0979916897507</v>
       </c>
     </row>
@@ -3517,38 +3501,38 @@
         <v>86</v>
       </c>
       <c r="D49" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E49" s="11">
-        <f t="shared" ref="E49:E53" si="13">E$36-($D49+E$41)/E$37</f>
-        <v>3.2451911016066481</v>
+        <f>E$38-($D49+E$43)/E$39</f>
+        <v>4.8241384700277008</v>
       </c>
       <c r="F49" s="11">
-        <f t="shared" si="7"/>
-        <v>6.1114391016066474</v>
+        <f>F$38-($D49+F$43)/F$39</f>
+        <v>7.6903864700276996</v>
       </c>
       <c r="G49" s="11">
-        <f t="shared" si="7"/>
-        <v>4.7657202216066477</v>
+        <f>G$38-($D49+G$43)/G$39</f>
+        <v>6.3446675900277008</v>
       </c>
       <c r="H49" s="11"/>
       <c r="I49" s="4">
         <v>2</v>
       </c>
       <c r="J49" s="26">
+        <f t="shared" si="7"/>
+        <v>556.32000000000005</v>
+      </c>
+      <c r="K49" s="3">
         <f t="shared" si="8"/>
-        <v>556.32000000000005</v>
-      </c>
-      <c r="K49" s="3">
+        <v>54.824561403508767</v>
+      </c>
+      <c r="L49" s="3">
+        <f t="shared" si="9"/>
+        <v>13.706140350877192</v>
+      </c>
+      <c r="M49" s="7">
         <f t="shared" si="10"/>
-        <v>54.824561403508767</v>
-      </c>
-      <c r="L49" s="3">
-        <f t="shared" si="11"/>
-        <v>13.706140350877192</v>
-      </c>
-      <c r="M49" s="7">
-        <f t="shared" si="12"/>
         <v>140.95250461680516</v>
       </c>
     </row>
@@ -3558,39 +3542,39 @@
         <v>86</v>
       </c>
       <c r="D50" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E50" s="11">
-        <f t="shared" si="13"/>
-        <v>2.1925595226592796</v>
+        <f>E$38-($D50+E$43)/E$39</f>
+        <v>4.2978226805540167</v>
       </c>
       <c r="F50" s="11">
-        <f t="shared" si="7"/>
-        <v>5.0588075226592784</v>
+        <f>F$38-($D50+F$43)/F$39</f>
+        <v>7.1640706805540155</v>
       </c>
       <c r="G50" s="11">
-        <f t="shared" si="7"/>
-        <v>3.7130886426592795</v>
+        <f>G$38-($D50+G$43)/G$39</f>
+        <v>5.8183518005540167</v>
       </c>
       <c r="H50" s="11"/>
       <c r="I50" s="4">
         <v>3</v>
       </c>
       <c r="J50" s="26">
+        <f t="shared" si="7"/>
+        <v>834.48</v>
+      </c>
+      <c r="K50" s="3">
         <f t="shared" si="8"/>
-        <v>834.48</v>
-      </c>
-      <c r="K50" s="3">
+        <v>36.549707602339183</v>
+      </c>
+      <c r="L50" s="3">
+        <f t="shared" si="9"/>
+        <v>9.1374269005847957</v>
+      </c>
+      <c r="M50" s="7">
         <f t="shared" si="10"/>
-        <v>36.549707602339183</v>
-      </c>
-      <c r="L50" s="3">
-        <f t="shared" si="11"/>
-        <v>9.1374269005847957</v>
-      </c>
-      <c r="M50" s="7">
-        <f t="shared" si="12"/>
-        <v>93.237342259156648</v>
+        <v>93.237342259156662</v>
       </c>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.25">
@@ -3599,38 +3583,38 @@
         <v>86</v>
       </c>
       <c r="D51" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E51" s="11">
-        <f t="shared" si="13"/>
-        <v>1.1399279437119114</v>
+        <f>E$38-($D51+E$43)/E$39</f>
+        <v>3.2451911016066481</v>
       </c>
       <c r="F51" s="11">
-        <f t="shared" si="7"/>
-        <v>4.0061759437119102</v>
+        <f>F$38-($D51+F$43)/F$39</f>
+        <v>6.1114391016066474</v>
       </c>
       <c r="G51" s="11">
-        <f t="shared" si="7"/>
-        <v>2.6604570637119114</v>
+        <f>G$38-($D51+G$43)/G$39</f>
+        <v>4.7657202216066477</v>
       </c>
       <c r="H51" s="11"/>
       <c r="I51" s="4">
         <v>4</v>
       </c>
       <c r="J51" s="26">
+        <f t="shared" si="7"/>
+        <v>1112.6400000000001</v>
+      </c>
+      <c r="K51" s="3">
         <f t="shared" si="8"/>
-        <v>1112.6400000000001</v>
-      </c>
-      <c r="K51" s="3">
+        <v>27.412280701754383</v>
+      </c>
+      <c r="L51" s="3">
+        <f t="shared" si="9"/>
+        <v>6.8530701754385959</v>
+      </c>
+      <c r="M51" s="7">
         <f t="shared" si="10"/>
-        <v>27.412280701754383</v>
-      </c>
-      <c r="L51" s="3">
-        <f t="shared" si="11"/>
-        <v>6.8530701754385959</v>
-      </c>
-      <c r="M51" s="7">
-        <f t="shared" si="12"/>
         <v>69.379761080332415</v>
       </c>
     </row>
@@ -3640,39 +3624,39 @@
         <v>86</v>
       </c>
       <c r="D52" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E52" s="11">
-        <f t="shared" si="13"/>
-        <v>8.7296364764542389E-2</v>
+        <f>E$38-($D52+E$43)/E$39</f>
+        <v>2.1925595226592796</v>
       </c>
       <c r="F52" s="11">
-        <f t="shared" si="7"/>
-        <v>2.9535443647645412</v>
+        <f>F$38-($D52+F$43)/F$39</f>
+        <v>5.0588075226592784</v>
       </c>
       <c r="G52" s="11">
-        <f t="shared" si="7"/>
-        <v>1.6078254847645423</v>
+        <f>G$38-($D52+G$43)/G$39</f>
+        <v>3.7130886426592795</v>
       </c>
       <c r="H52" s="11"/>
       <c r="I52" s="4">
         <v>5</v>
       </c>
       <c r="J52" s="26">
+        <f t="shared" si="7"/>
+        <v>1390.8</v>
+      </c>
+      <c r="K52" s="3">
         <f t="shared" si="8"/>
-        <v>1390.8</v>
-      </c>
-      <c r="K52" s="3">
+        <v>21.929824561403507</v>
+      </c>
+      <c r="L52" s="3">
+        <f t="shared" si="9"/>
+        <v>5.4824561403508767</v>
+      </c>
+      <c r="M52" s="7">
         <f t="shared" si="10"/>
-        <v>21.929824561403507</v>
-      </c>
-      <c r="L52" s="3">
-        <f t="shared" si="11"/>
-        <v>5.4824561403508767</v>
-      </c>
-      <c r="M52" s="7">
-        <f t="shared" si="12"/>
-        <v>55.065212373037859</v>
+        <v>55.065212373037845</v>
       </c>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
@@ -3681,1213 +3665,1255 @@
         <v>86</v>
       </c>
       <c r="D53" s="4">
-        <v>6</v>
-      </c>
-      <c r="E53" s="22">
-        <f t="shared" si="13"/>
-        <v>-0.96533521418282575</v>
+        <v>4</v>
+      </c>
+      <c r="E53" s="11">
+        <f>E$38-($D53+E$43)/E$39</f>
+        <v>1.1399279437119114</v>
       </c>
       <c r="F53" s="11">
-        <f t="shared" si="7"/>
-        <v>1.900912785817173</v>
+        <f>F$38-($D53+F$43)/F$39</f>
+        <v>4.0061759437119102</v>
       </c>
       <c r="G53" s="11">
-        <f t="shared" si="7"/>
-        <v>0.5551939058171742</v>
+        <f>G$38-($D53+G$43)/G$39</f>
+        <v>2.6604570637119114</v>
       </c>
       <c r="H53" s="11"/>
       <c r="I53" s="4">
         <v>6</v>
       </c>
       <c r="J53" s="26">
+        <f t="shared" si="7"/>
+        <v>1668.96</v>
+      </c>
+      <c r="K53" s="3">
         <f t="shared" si="8"/>
-        <v>1668.96</v>
-      </c>
-      <c r="K53" s="3">
+        <v>18.274853801169591</v>
+      </c>
+      <c r="L53" s="3">
+        <f t="shared" si="9"/>
+        <v>4.5687134502923978</v>
+      </c>
+      <c r="M53" s="7">
         <f t="shared" si="10"/>
-        <v>18.274853801169591</v>
-      </c>
-      <c r="L53" s="3">
-        <f t="shared" si="11"/>
-        <v>4.5687134502923978</v>
-      </c>
-      <c r="M53" s="7">
-        <f t="shared" si="12"/>
         <v>45.522179901508146</v>
       </c>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
+      <c r="B54" s="4"/>
+      <c r="C54" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" s="4">
+        <v>5</v>
+      </c>
+      <c r="E54" s="11">
+        <f>E$38-($D54+E$43)/E$39</f>
+        <v>8.7296364764542389E-2</v>
+      </c>
+      <c r="F54" s="11">
+        <f>F$38-($D54+F$43)/F$39</f>
+        <v>2.9535443647645412</v>
+      </c>
+      <c r="G54" s="11">
+        <f>G$38-($D54+G$43)/G$39</f>
+        <v>1.6078254847645423</v>
+      </c>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C55" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D55" s="17"/>
-      <c r="E55" s="18">
-        <f t="shared" ref="E55:G62" si="14">E46/Batt_bank_energy__kWh</f>
-        <v>0.48640493268194407</v>
-      </c>
-      <c r="F55" s="21">
-        <f t="shared" si="14"/>
-        <v>0.74697293268194398</v>
-      </c>
-      <c r="G55" s="21">
-        <f t="shared" si="14"/>
-        <v>0.62463485268194407</v>
+      <c r="B55" s="4"/>
+      <c r="C55" t="s">
+        <v>86</v>
+      </c>
+      <c r="D55" s="4">
+        <v>6</v>
+      </c>
+      <c r="E55" s="22">
+        <f>E$38-($D55+E$43)/E$39</f>
+        <v>-0.96533521418282575</v>
+      </c>
+      <c r="F55" s="11">
+        <f>F$38-($D55+F$43)/F$39</f>
+        <v>1.900912785817173</v>
+      </c>
+      <c r="G55" s="11">
+        <f>G$38-($D55+G$43)/G$39</f>
+        <v>0.5551939058171742</v>
       </c>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C56" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="D56" s="17"/>
-      <c r="E56" s="18">
-        <f t="shared" si="14"/>
-        <v>0.43855804272979099</v>
-      </c>
-      <c r="F56" s="21">
-        <f t="shared" si="14"/>
-        <v>0.69912604272979084</v>
-      </c>
-      <c r="G56" s="21">
-        <f t="shared" si="14"/>
-        <v>0.57678796272979094</v>
-      </c>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C57" s="17" t="s">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="D57" s="17"/>
-      <c r="E57" s="18">
-        <f t="shared" si="14"/>
-        <v>0.3907111527776379</v>
+      <c r="E57" s="21">
+        <f>E48/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.54044992520216006</v>
       </c>
       <c r="F57" s="21">
-        <f t="shared" si="14"/>
-        <v>0.65127915277763782</v>
+        <f>F48/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.82996992520215995</v>
       </c>
       <c r="G57" s="21">
-        <f t="shared" si="14"/>
-        <v>0.52894107277763791</v>
+        <f>G48/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.69403872520216003</v>
       </c>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C58" s="17" t="s">
-        <v>75</v>
+        <v>128</v>
       </c>
       <c r="D58" s="17"/>
       <c r="E58" s="18">
-        <f t="shared" si="14"/>
-        <v>0.29501737287333163</v>
+        <f>E49/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.48728671414421221</v>
       </c>
       <c r="F58" s="21">
-        <f t="shared" si="14"/>
-        <v>0.55558537287333154</v>
-      </c>
-      <c r="G58" s="18">
-        <f t="shared" si="14"/>
-        <v>0.43324729287333158</v>
+        <f>F49/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.7768067141442121</v>
+      </c>
+      <c r="G58" s="21">
+        <f>G49/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.64087551414421218</v>
       </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C59" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D59" s="17"/>
       <c r="E59" s="18">
-        <f t="shared" si="14"/>
-        <v>0.19932359296902541</v>
-      </c>
-      <c r="F59" s="18">
-        <f t="shared" si="14"/>
-        <v>0.45989159296902532</v>
-      </c>
-      <c r="G59" s="18">
-        <f t="shared" si="14"/>
-        <v>0.33755351296902542</v>
+        <f>E50/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.4341235030862643</v>
+      </c>
+      <c r="F59" s="21">
+        <f>F50/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.72364350308626413</v>
+      </c>
+      <c r="G59" s="21">
+        <f>G50/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.58771230308626432</v>
       </c>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C60" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D60" s="17"/>
       <c r="E60" s="18">
-        <f t="shared" si="14"/>
-        <v>0.10362981306471922</v>
-      </c>
-      <c r="F60" s="18">
-        <f t="shared" si="14"/>
-        <v>0.3641978130647191</v>
+        <f>E51/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.32779708097036847</v>
+      </c>
+      <c r="F60" s="21">
+        <f>F51/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.61731708097036841</v>
       </c>
       <c r="G60" s="18">
-        <f t="shared" si="14"/>
-        <v>0.24185973306471922</v>
+        <f>G51/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.48138588097036844</v>
       </c>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C61" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D61" s="17"/>
       <c r="E61" s="18">
-        <f t="shared" si="14"/>
-        <v>7.9360331604129437E-3</v>
-      </c>
-      <c r="F61" s="18">
-        <f t="shared" si="14"/>
-        <v>0.26850403316041282</v>
+        <f>E52/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.22147065885447267</v>
+      </c>
+      <c r="F61" s="21">
+        <f>F52/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.51099065885447259</v>
       </c>
       <c r="G61" s="18">
-        <f t="shared" si="14"/>
-        <v>0.14616595316041295</v>
+        <f>G52/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.37505945885447267</v>
       </c>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C62" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D62" s="17"/>
+      <c r="E62" s="18">
+        <f>E53/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.1151442367385769</v>
+      </c>
+      <c r="F62" s="18">
+        <f>F53/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.40466423673857677</v>
+      </c>
+      <c r="G62" s="18">
+        <f>G53/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.2687330367385769</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C63" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D63" s="17"/>
+      <c r="E63" s="18">
+        <f>E54/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>8.8178146226810493E-3</v>
+      </c>
+      <c r="F63" s="18">
+        <f>F54/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.29833781462268094</v>
+      </c>
+      <c r="G63" s="18">
+        <f>G54/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.16240661462268105</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C64" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D62" s="17"/>
-      <c r="E62" s="21">
-        <f t="shared" si="14"/>
-        <v>-8.775774674389325E-2</v>
-      </c>
-      <c r="F62" s="18">
-        <f t="shared" si="14"/>
-        <v>0.17281025325610663</v>
-      </c>
-      <c r="G62" s="18">
-        <f t="shared" si="14"/>
-        <v>5.0472173256106749E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+      <c r="D64" s="17"/>
+      <c r="E64" s="18">
+        <f>E55/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>-9.7508607493214716E-2</v>
+      </c>
+      <c r="F64" s="18">
+        <f>F55/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>0.19201139250678514</v>
+      </c>
+      <c r="G64" s="18">
+        <f>G55/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <v>5.6080192506785274E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>99</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C66" t="s">
         <v>91</v>
       </c>
-      <c r="E64" s="13">
-        <f t="shared" ref="E64:G71" si="15">1/E55*Depth_of_Discharge</f>
-        <v>1.0279501016634336</v>
-      </c>
-      <c r="F64" s="13">
-        <f t="shared" si="15"/>
-        <v>0.66936829719490865</v>
-      </c>
-      <c r="G64" s="13">
-        <f t="shared" si="15"/>
-        <v>0.80046766179183004</v>
-      </c>
-    </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
-        <v>132</v>
-      </c>
-      <c r="E65" s="13">
-        <f t="shared" si="15"/>
-        <v>1.1400999440980844</v>
-      </c>
-      <c r="F65" s="13">
-        <f t="shared" si="15"/>
-        <v>0.71517862222341477</v>
-      </c>
-      <c r="G65" s="13">
-        <f t="shared" si="15"/>
-        <v>0.86686968575701018</v>
-      </c>
-    </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
-        <v>133</v>
-      </c>
       <c r="E66" s="13">
-        <f t="shared" si="15"/>
-        <v>1.2797177568272813</v>
+        <f t="shared" ref="E66:G73" si="11">1/E57*Depth_of_Discharge</f>
+        <v>0.9251550914970903</v>
       </c>
       <c r="F66" s="13">
-        <f t="shared" si="15"/>
-        <v>0.76771995213965016</v>
+        <f t="shared" si="11"/>
+        <v>0.60243146747541787</v>
       </c>
       <c r="G66" s="13">
-        <f t="shared" si="15"/>
-        <v>0.94528488282133372</v>
+        <f t="shared" si="11"/>
+        <v>0.72042089561264711</v>
       </c>
     </row>
     <row r="67" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="E67" s="13">
-        <f t="shared" si="15"/>
-        <v>1.6948154446981654</v>
+        <f t="shared" si="11"/>
+        <v>1.0260899496882758</v>
       </c>
       <c r="F67" s="13">
-        <f t="shared" si="15"/>
-        <v>0.89995169853759904</v>
+        <f t="shared" si="11"/>
+        <v>0.6436607600010732</v>
       </c>
       <c r="G67" s="13">
-        <f t="shared" si="15"/>
-        <v>1.1540753011610505</v>
+        <f t="shared" si="11"/>
+        <v>0.78018271718130916</v>
       </c>
     </row>
     <row r="68" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E68" s="13">
-        <f t="shared" si="15"/>
-        <v>2.5084837803305065</v>
+        <f t="shared" si="11"/>
+        <v>1.1517459811445534</v>
       </c>
       <c r="F68" s="13">
-        <f t="shared" si="15"/>
-        <v>1.0872127424031344</v>
+        <f t="shared" si="11"/>
+        <v>0.69094795692568522</v>
       </c>
       <c r="G68" s="13">
-        <f t="shared" si="15"/>
-        <v>1.4812466195423095</v>
+        <f t="shared" si="11"/>
+        <v>0.85075639453920038</v>
       </c>
     </row>
     <row r="69" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E69" s="13">
-        <f t="shared" si="15"/>
-        <v>4.8248663701413648</v>
+        <f t="shared" si="11"/>
+        <v>1.5253339002283488</v>
       </c>
       <c r="F69" s="13">
-        <f t="shared" si="15"/>
-        <v>1.3728802921481256</v>
+        <f t="shared" si="11"/>
+        <v>0.80995652868383905</v>
       </c>
       <c r="G69" s="13">
-        <f t="shared" si="15"/>
-        <v>2.0673139495535828</v>
+        <f t="shared" si="11"/>
+        <v>1.0386677710449455</v>
       </c>
     </row>
     <row r="70" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E70" s="13">
-        <f t="shared" si="15"/>
-        <v>63.00376899811026</v>
+        <f t="shared" si="11"/>
+        <v>2.2576354022974559</v>
       </c>
       <c r="F70" s="13">
-        <f t="shared" si="15"/>
-        <v>1.8621694211247999</v>
+        <f t="shared" si="11"/>
+        <v>0.97849146816282084</v>
       </c>
       <c r="G70" s="13">
-        <f t="shared" si="15"/>
-        <v>3.4207692639014526</v>
+        <f t="shared" si="11"/>
+        <v>1.3331219575880786</v>
       </c>
     </row>
     <row r="71" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>94</v>
-      </c>
-      <c r="E71" s="21">
-        <f t="shared" si="15"/>
-        <v>-5.697502711175674</v>
+        <v>93</v>
+      </c>
+      <c r="E71" s="13">
+        <f t="shared" si="11"/>
+        <v>4.3423797331272285</v>
       </c>
       <c r="F71" s="13">
-        <f t="shared" si="15"/>
-        <v>2.8933468389690669</v>
+        <f t="shared" si="11"/>
+        <v>1.2355922629333131</v>
       </c>
       <c r="G71" s="13">
-        <f t="shared" si="15"/>
-        <v>9.9064487963078509</v>
+        <f t="shared" si="11"/>
+        <v>1.8605825545982249</v>
       </c>
     </row>
     <row r="72" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
+      <c r="C72" t="s">
+        <v>135</v>
+      </c>
+      <c r="E72" s="13">
+        <f t="shared" si="11"/>
+        <v>56.703392098299226</v>
+      </c>
+      <c r="F72" s="13">
+        <f t="shared" si="11"/>
+        <v>1.6759524790123197</v>
+      </c>
+      <c r="G72" s="13">
+        <f t="shared" si="11"/>
+        <v>3.0786923375113076</v>
+      </c>
       <c r="R72" t="s">
         <v>167</v>
       </c>
     </row>
+    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>94</v>
+      </c>
+      <c r="E73" s="21">
+        <f t="shared" si="11"/>
+        <v>-5.1277524400581074</v>
+      </c>
+      <c r="F73" s="13">
+        <f t="shared" si="11"/>
+        <v>2.60401215507216</v>
+      </c>
+      <c r="G73" s="13">
+        <f t="shared" si="11"/>
+        <v>8.9158039166770653</v>
+      </c>
+    </row>
     <row r="74" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>100</v>
-      </c>
-      <c r="C74" t="s">
-        <v>95</v>
-      </c>
-      <c r="D74" s="4">
-        <v>0</v>
-      </c>
       <c r="E74" s="13"/>
       <c r="F74" s="13"/>
       <c r="G74" s="13"/>
     </row>
-    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>136</v>
-      </c>
-      <c r="D75" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E75" s="13">
-        <f t="shared" ref="E75:G81" si="16">Cycle_energy__kWh/$D75</f>
-        <v>11</v>
-      </c>
-      <c r="F75" s="13">
-        <f t="shared" si="16"/>
-        <v>11</v>
-      </c>
-      <c r="G75" s="13">
-        <f t="shared" si="16"/>
-        <v>11</v>
-      </c>
-    </row>
     <row r="76" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>100</v>
+      </c>
       <c r="C76" t="s">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="D76" s="4">
-        <v>1</v>
-      </c>
-      <c r="E76" s="13">
-        <f t="shared" si="16"/>
-        <v>5.5</v>
-      </c>
-      <c r="F76" s="13">
-        <f t="shared" si="16"/>
-        <v>5.5</v>
-      </c>
-      <c r="G76" s="13">
-        <f t="shared" si="16"/>
-        <v>5.5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
     </row>
     <row r="77" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="D77" s="4">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E77" s="13">
-        <f t="shared" si="16"/>
-        <v>2.75</v>
+        <f>Cycle_energy__kWh/$D77</f>
+        <v>9.9</v>
       </c>
       <c r="F77" s="13">
-        <f t="shared" si="16"/>
-        <v>2.75</v>
+        <f>Cycle_energy__kWh/$D77</f>
+        <v>9.9</v>
       </c>
       <c r="G77" s="13">
-        <f t="shared" si="16"/>
-        <v>2.75</v>
+        <f>Cycle_energy__kWh/$D77</f>
+        <v>9.9</v>
       </c>
     </row>
     <row r="78" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D78" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E78" s="13">
-        <f t="shared" si="16"/>
-        <v>1.8333333333333333</v>
+        <f>Cycle_energy__kWh/$D78</f>
+        <v>4.95</v>
       </c>
       <c r="F78" s="13">
-        <f t="shared" si="16"/>
-        <v>1.8333333333333333</v>
+        <f>Cycle_energy__kWh/$D78</f>
+        <v>4.95</v>
       </c>
       <c r="G78" s="13">
-        <f t="shared" si="16"/>
-        <v>1.8333333333333333</v>
+        <f>Cycle_energy__kWh/$D78</f>
+        <v>4.95</v>
       </c>
     </row>
     <row r="79" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D79" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E79" s="13">
-        <f t="shared" si="16"/>
-        <v>1.375</v>
+        <f>Cycle_energy__kWh/$D79</f>
+        <v>2.4750000000000001</v>
       </c>
       <c r="F79" s="13">
-        <f t="shared" si="16"/>
-        <v>1.375</v>
+        <f>Cycle_energy__kWh/$D79</f>
+        <v>2.4750000000000001</v>
       </c>
       <c r="G79" s="13">
-        <f t="shared" si="16"/>
-        <v>1.375</v>
+        <f>Cycle_energy__kWh/$D79</f>
+        <v>2.4750000000000001</v>
       </c>
     </row>
     <row r="80" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D80" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E80" s="13">
-        <f t="shared" si="16"/>
-        <v>1.1000000000000001</v>
+        <f>Cycle_energy__kWh/$D80</f>
+        <v>1.6500000000000001</v>
       </c>
       <c r="F80" s="13">
-        <f t="shared" si="16"/>
-        <v>1.1000000000000001</v>
+        <f>Cycle_energy__kWh/$D80</f>
+        <v>1.6500000000000001</v>
       </c>
       <c r="G80" s="13">
-        <f t="shared" si="16"/>
-        <v>1.1000000000000001</v>
+        <f>Cycle_energy__kWh/$D80</f>
+        <v>1.6500000000000001</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
+        <v>97</v>
+      </c>
+      <c r="D81" s="4">
+        <v>4</v>
+      </c>
+      <c r="E81" s="13">
+        <f>Cycle_energy__kWh/$D81</f>
+        <v>1.2375</v>
+      </c>
+      <c r="F81" s="13">
+        <f>Cycle_energy__kWh/$D81</f>
+        <v>1.2375</v>
+      </c>
+      <c r="G81" s="13">
+        <f>Cycle_energy__kWh/$D81</f>
+        <v>1.2375</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>139</v>
+      </c>
+      <c r="D82" s="4">
+        <v>5</v>
+      </c>
+      <c r="E82" s="13">
+        <f>Cycle_energy__kWh/$D82</f>
+        <v>0.99</v>
+      </c>
+      <c r="F82" s="13">
+        <f>Cycle_energy__kWh/$D82</f>
+        <v>0.99</v>
+      </c>
+      <c r="G82" s="13">
+        <f>Cycle_energy__kWh/$D82</f>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
         <v>98</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D83" s="4">
         <v>6</v>
       </c>
-      <c r="E81" s="21">
-        <f t="shared" si="16"/>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="F81" s="13">
-        <f t="shared" si="16"/>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="G81" s="13">
-        <f t="shared" si="16"/>
-        <v>0.91666666666666663</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+      <c r="E83" s="21">
+        <f>Cycle_energy__kWh/$D83</f>
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="F83" s="13">
+        <f>Cycle_energy__kWh/$D83</f>
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="G83" s="13">
+        <f>Cycle_energy__kWh/$D83</f>
+        <v>0.82500000000000007</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>101</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C85" t="s">
         <v>102</v>
       </c>
-      <c r="E83" s="7"/>
-      <c r="F83" s="7"/>
-      <c r="G83" s="7"/>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
-        <v>140</v>
-      </c>
-      <c r="E84" s="7">
-        <f t="shared" ref="E84:G90" si="17">E65+E75</f>
-        <v>12.140099944098084</v>
-      </c>
-      <c r="F84" s="7">
-        <f t="shared" si="17"/>
-        <v>11.715178622223414</v>
-      </c>
-      <c r="G84" s="7">
-        <f t="shared" si="17"/>
-        <v>11.86686968575701</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
-        <v>141</v>
-      </c>
-      <c r="E85" s="7">
-        <f t="shared" si="17"/>
-        <v>6.7797177568272815</v>
-      </c>
-      <c r="F85" s="7">
-        <f t="shared" si="17"/>
-        <v>6.2677199521396503</v>
-      </c>
-      <c r="G85" s="7">
-        <f t="shared" si="17"/>
-        <v>6.4452848828213334</v>
-      </c>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>103</v>
+        <v>140</v>
       </c>
       <c r="E86" s="7">
-        <f t="shared" si="17"/>
-        <v>4.4448154446981656</v>
+        <f t="shared" ref="E86:G92" si="12">E67+E77</f>
+        <v>10.926089949688276</v>
       </c>
       <c r="F86" s="7">
-        <f t="shared" si="17"/>
-        <v>3.649951698537599</v>
+        <f t="shared" si="12"/>
+        <v>10.543660760001073</v>
       </c>
       <c r="G86" s="7">
-        <f t="shared" si="17"/>
-        <v>3.9040753011610505</v>
+        <f t="shared" si="12"/>
+        <v>10.68018271718131</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E87" s="7">
-        <f t="shared" si="17"/>
-        <v>4.3418171136638399</v>
+        <f t="shared" si="12"/>
+        <v>6.1017459811445534</v>
       </c>
       <c r="F87" s="7">
-        <f t="shared" si="17"/>
-        <v>2.9205460757364676</v>
+        <f t="shared" si="12"/>
+        <v>5.6409479569256851</v>
       </c>
       <c r="G87" s="7">
-        <f t="shared" si="17"/>
-        <v>3.3145799528756426</v>
+        <f t="shared" si="12"/>
+        <v>5.8007563945392002</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E88" s="7">
-        <f t="shared" si="17"/>
-        <v>6.1998663701413648</v>
+        <f t="shared" si="12"/>
+        <v>4.0003339002283491</v>
       </c>
       <c r="F88" s="7">
-        <f t="shared" si="17"/>
-        <v>2.7478802921481256</v>
+        <f t="shared" si="12"/>
+        <v>3.2849565286838391</v>
       </c>
       <c r="G88" s="7">
-        <f t="shared" si="17"/>
-        <v>3.4423139495535828</v>
+        <f t="shared" si="12"/>
+        <v>3.5136677710449455</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E89" s="7">
-        <f t="shared" si="17"/>
-        <v>64.103768998110255</v>
+        <f t="shared" si="12"/>
+        <v>3.9076354022974558</v>
       </c>
       <c r="F89" s="7">
-        <f t="shared" si="17"/>
-        <v>2.9621694211248002</v>
+        <f t="shared" si="12"/>
+        <v>2.6284914681628209</v>
       </c>
       <c r="G89" s="7">
-        <f t="shared" si="17"/>
-        <v>4.5207692639014532</v>
+        <f t="shared" si="12"/>
+        <v>2.9831219575880787</v>
       </c>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
-        <v>105</v>
-      </c>
-      <c r="E90" s="31">
-        <f t="shared" si="17"/>
-        <v>-4.780836044509007</v>
+        <v>104</v>
+      </c>
+      <c r="E90" s="7">
+        <f t="shared" si="12"/>
+        <v>5.5798797331272283</v>
       </c>
       <c r="F90" s="7">
-        <f t="shared" si="17"/>
-        <v>3.8100135056357334</v>
+        <f t="shared" si="12"/>
+        <v>2.4730922629333132</v>
       </c>
       <c r="G90" s="7">
-        <f t="shared" si="17"/>
-        <v>10.823115462974517</v>
+        <f t="shared" si="12"/>
+        <v>3.0980825545982249</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>143</v>
+      </c>
+      <c r="E91" s="7">
+        <f t="shared" si="12"/>
+        <v>57.693392098299228</v>
+      </c>
+      <c r="F91" s="7">
+        <f t="shared" si="12"/>
+        <v>2.6659524790123195</v>
+      </c>
+      <c r="G91" s="7">
+        <f t="shared" si="12"/>
+        <v>4.0686923375113073</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>106</v>
-      </c>
-      <c r="E92" s="7"/>
-      <c r="F92" s="7"/>
-      <c r="G92" s="7"/>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C93" t="s">
-        <v>144</v>
-      </c>
-      <c r="E93" s="7">
-        <f t="shared" ref="E93:G98" si="18">E65/E84</f>
-        <v>9.3911907591201049E-2</v>
-      </c>
-      <c r="F93" s="7">
-        <f t="shared" si="18"/>
-        <v>6.1047180353420986E-2</v>
-      </c>
-      <c r="G93" s="7">
-        <f t="shared" si="18"/>
-        <v>7.3049566457905446E-2</v>
+        <v>105</v>
+      </c>
+      <c r="E92" s="31">
+        <f t="shared" si="12"/>
+        <v>-4.3027524400581072</v>
+      </c>
+      <c r="F92" s="7">
+        <f t="shared" si="12"/>
+        <v>3.4290121550721602</v>
+      </c>
+      <c r="G92" s="7">
+        <f t="shared" si="12"/>
+        <v>9.7408039166770646</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
-        <v>145</v>
-      </c>
-      <c r="E94" s="7">
-        <f t="shared" si="18"/>
-        <v>0.18875678940153306</v>
-      </c>
-      <c r="F94" s="7">
-        <f t="shared" si="18"/>
-        <v>0.12248791554216919</v>
-      </c>
-      <c r="G94" s="7">
-        <f t="shared" si="18"/>
-        <v>0.14666301024812861</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
       <c r="E95" s="7">
-        <f t="shared" si="18"/>
-        <v>0.38130164588042986</v>
+        <f t="shared" ref="E95:G100" si="13">E67/E86</f>
+        <v>9.3911907591201049E-2</v>
       </c>
       <c r="F95" s="7">
-        <f t="shared" si="18"/>
-        <v>0.2465653720563416</v>
+        <f t="shared" si="13"/>
+        <v>6.1047180353420979E-2</v>
       </c>
       <c r="G95" s="7">
-        <f t="shared" si="18"/>
-        <v>0.29560784875687074</v>
+        <f t="shared" si="13"/>
+        <v>7.3049566457905432E-2</v>
       </c>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E96" s="7">
-        <f t="shared" si="18"/>
-        <v>0.57774975653309446</v>
+        <f t="shared" si="13"/>
+        <v>0.18875678940153309</v>
       </c>
       <c r="F96" s="7">
-        <f t="shared" si="18"/>
-        <v>0.37226351312706968</v>
+        <f t="shared" si="13"/>
+        <v>0.1224879155421692</v>
       </c>
       <c r="G96" s="7">
-        <f t="shared" si="18"/>
-        <v>0.44688818510991685</v>
+        <f t="shared" si="13"/>
+        <v>0.14666301024812864</v>
       </c>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
-        <v>108</v>
-      </c>
-      <c r="D97" s="20"/>
+        <v>107</v>
+      </c>
       <c r="E97" s="7">
-        <f t="shared" si="18"/>
-        <v>0.77822102640437263</v>
+        <f t="shared" si="13"/>
+        <v>0.38130164588042986</v>
       </c>
       <c r="F97" s="7">
-        <f t="shared" si="18"/>
-        <v>0.49961430127470774</v>
+        <f t="shared" si="13"/>
+        <v>0.24656537205634158</v>
       </c>
       <c r="G97" s="7">
-        <f t="shared" si="18"/>
-        <v>0.60055938530001973</v>
+        <f t="shared" si="13"/>
+        <v>0.29560784875687074</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
-        <v>147</v>
-      </c>
-      <c r="D98" s="20"/>
+        <v>146</v>
+      </c>
       <c r="E98" s="7">
-        <f t="shared" si="18"/>
-        <v>0.98284032253965559</v>
+        <f t="shared" si="13"/>
+        <v>0.57774975653309446</v>
       </c>
       <c r="F98" s="7">
-        <f t="shared" si="18"/>
-        <v>0.62865054505143514</v>
+        <f t="shared" si="13"/>
+        <v>0.37226351312706962</v>
       </c>
       <c r="G98" s="7">
-        <f t="shared" si="18"/>
-        <v>0.756678579288806</v>
+        <f t="shared" si="13"/>
+        <v>0.44688818510991679</v>
       </c>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
+        <v>108</v>
+      </c>
+      <c r="D99" s="20"/>
+      <c r="E99" s="7">
+        <f t="shared" si="13"/>
+        <v>0.77822102640437263</v>
+      </c>
+      <c r="F99" s="7">
+        <f t="shared" si="13"/>
+        <v>0.49961430127470779</v>
+      </c>
+      <c r="G99" s="7">
+        <f t="shared" si="13"/>
+        <v>0.60055938530001973</v>
+      </c>
+    </row>
+    <row r="100" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>147</v>
+      </c>
+      <c r="D100" s="20"/>
+      <c r="E100" s="7">
+        <f t="shared" si="13"/>
+        <v>0.98284032253965548</v>
+      </c>
+      <c r="F100" s="7">
+        <f t="shared" si="13"/>
+        <v>0.62865054505143525</v>
+      </c>
+      <c r="G100" s="7">
+        <f t="shared" si="13"/>
+        <v>0.75667857928880611</v>
+      </c>
+    </row>
+    <row r="101" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
         <v>109</v>
       </c>
-      <c r="D99" s="20"/>
-      <c r="E99" s="31" t="s">
+      <c r="D101" s="20"/>
+      <c r="E101" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="F99" s="7">
-        <f>F71/F90</f>
-        <v>0.759405927220273</v>
-      </c>
-      <c r="G99" s="7">
-        <f>G71/G90</f>
+      <c r="F101" s="7">
+        <f>F73/F92</f>
+        <v>0.75940592722027289</v>
+      </c>
+      <c r="G101" s="7">
+        <f>G73/G92</f>
         <v>0.9153047318212072</v>
       </c>
     </row>
-    <row r="100" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D100" s="20"/>
-      <c r="E100" s="7"/>
-      <c r="F100" s="7"/>
-      <c r="G100" s="7"/>
-    </row>
-    <row r="101" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D101" s="20"/>
-    </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C102" s="14" t="s">
+      <c r="D102" s="20"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7"/>
+    </row>
+    <row r="103" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D103" s="20"/>
+    </row>
+    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C104" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D102" s="14">
+      <c r="D104" s="14">
         <v>0</v>
       </c>
-      <c r="E102" s="15"/>
-      <c r="F102" s="15"/>
-      <c r="G102" s="15"/>
-    </row>
-    <row r="103" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C103" s="23" t="s">
+      <c r="E104" s="15"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="15"/>
+    </row>
+    <row r="105" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C105" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D103" s="23">
+      <c r="D105" s="23">
         <v>0.5</v>
       </c>
-      <c r="E103" s="24">
-        <f t="shared" ref="E103:G108" si="19">Engine_spec_d_life__h/Hours_in_a_year__h/E93</f>
+      <c r="E105" s="24">
+        <f t="shared" ref="E105:G110" si="14">Engine_spec_d_life__h/Hours_in_a_year__h/E95</f>
         <v>18.233350924752401</v>
       </c>
-      <c r="F103" s="24">
-        <f t="shared" si="19"/>
-        <v>28.049268732971569</v>
-      </c>
-      <c r="G103" s="24">
-        <f t="shared" si="19"/>
-        <v>23.440642431601713</v>
-      </c>
-    </row>
-    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C104" s="23" t="s">
+      <c r="F105" s="24">
+        <f t="shared" si="14"/>
+        <v>28.049268732971573</v>
+      </c>
+      <c r="G105" s="24">
+        <f t="shared" si="14"/>
+        <v>23.440642431601717</v>
+      </c>
+    </row>
+    <row r="106" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C106" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="D104" s="23">
+      <c r="D106" s="23">
         <v>1</v>
       </c>
-      <c r="E104" s="24">
-        <f t="shared" si="19"/>
-        <v>9.0716141790308509</v>
-      </c>
-      <c r="F104" s="24">
-        <f t="shared" si="19"/>
-        <v>13.979573083140437</v>
-      </c>
-      <c r="G104" s="24">
-        <f t="shared" si="19"/>
-        <v>11.675259932455509</v>
-      </c>
-    </row>
-    <row r="105" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C105" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D105" s="14">
-        <v>2</v>
-      </c>
-      <c r="E105" s="15">
-        <f t="shared" si="19"/>
-        <v>4.4907458061700751</v>
-      </c>
-      <c r="F105" s="15">
-        <f t="shared" si="19"/>
-        <v>6.9447252582248682</v>
-      </c>
-      <c r="G105" s="15">
-        <f t="shared" si="19"/>
-        <v>5.7925686828824041</v>
-      </c>
-    </row>
-    <row r="106" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C106" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="D106" s="14">
-        <v>3</v>
-      </c>
-      <c r="E106" s="15">
-        <f t="shared" si="19"/>
-        <v>2.9637896818831506</v>
-      </c>
-      <c r="F106" s="15">
-        <f t="shared" si="19"/>
-        <v>4.5997759832530125</v>
-      </c>
-      <c r="G106" s="15">
-        <f t="shared" si="19"/>
-        <v>3.8316715996913686</v>
+      <c r="E106" s="24">
+        <f t="shared" si="14"/>
+        <v>9.0716141790308491</v>
+      </c>
+      <c r="F106" s="24">
+        <f t="shared" si="14"/>
+        <v>13.979573083140435</v>
+      </c>
+      <c r="G106" s="24">
+        <f t="shared" si="14"/>
+        <v>11.675259932455507</v>
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C107" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D107" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E107" s="15">
-        <f t="shared" si="19"/>
-        <v>2.2003116197396881</v>
+        <f t="shared" si="14"/>
+        <v>4.4907458061700751</v>
       </c>
       <c r="F107" s="15">
-        <f t="shared" si="19"/>
-        <v>3.4273013457670847</v>
+        <f t="shared" si="14"/>
+        <v>6.9447252582248691</v>
       </c>
       <c r="G107" s="15">
-        <f t="shared" si="19"/>
-        <v>2.8512230580958526</v>
+        <f t="shared" si="14"/>
+        <v>5.7925686828824041</v>
       </c>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C108" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D108" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E108" s="15">
-        <f t="shared" si="19"/>
-        <v>1.7422247824536103</v>
+        <f t="shared" si="14"/>
+        <v>2.9637896818831506</v>
       </c>
       <c r="F108" s="15">
-        <f t="shared" si="19"/>
-        <v>2.7238165632755282</v>
+        <f t="shared" si="14"/>
+        <v>4.5997759832530134</v>
       </c>
       <c r="G108" s="15">
-        <f t="shared" si="19"/>
-        <v>2.262953933138542</v>
+        <f t="shared" si="14"/>
+        <v>3.8316715996913695</v>
       </c>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C109" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D109" s="14">
-        <v>6</v>
-      </c>
-      <c r="E109" s="31" t="s">
-        <v>116</v>
+        <v>4</v>
+      </c>
+      <c r="E109" s="15">
+        <f t="shared" si="14"/>
+        <v>2.2003116197396881</v>
       </c>
       <c r="F109" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F99</f>
-        <v>2.2548267082811564</v>
+        <f t="shared" si="14"/>
+        <v>3.4273013457670847</v>
       </c>
       <c r="G109" s="15">
-        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G99</f>
-        <v>1.8707745165003349</v>
+        <f t="shared" si="14"/>
+        <v>2.8512230580958526</v>
       </c>
     </row>
     <row r="110" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C110" s="14"/>
-      <c r="D110" s="14"/>
-      <c r="E110" s="14"/>
-      <c r="F110" s="14"/>
-      <c r="G110" s="14"/>
+      <c r="C110" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D110" s="14">
+        <v>5</v>
+      </c>
+      <c r="E110" s="15">
+        <f t="shared" si="14"/>
+        <v>1.7422247824536106</v>
+      </c>
+      <c r="F110" s="15">
+        <f t="shared" si="14"/>
+        <v>2.7238165632755278</v>
+      </c>
+      <c r="G110" s="15">
+        <f t="shared" si="14"/>
+        <v>2.2629539331385415</v>
+      </c>
     </row>
     <row r="111" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C111" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D111" s="14">
+        <v>6</v>
+      </c>
+      <c r="E111" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="F111" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/F101</f>
+        <v>2.2548267082811568</v>
+      </c>
+      <c r="G111" s="15">
+        <f>Engine_spec_d_life__h/Hours_in_a_year__h/G101</f>
+        <v>1.8707745165003349</v>
+      </c>
+    </row>
+    <row r="112" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C112" s="14"/>
+      <c r="D112" s="14"/>
+      <c r="E112" s="14"/>
+      <c r="F112" s="14"/>
+      <c r="G112" s="14"/>
+    </row>
+    <row r="113" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C113" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="D111" s="14">
+      <c r="D113" s="14">
         <v>0</v>
       </c>
-      <c r="E111" s="16"/>
-      <c r="F111" s="16"/>
-      <c r="G111" s="16"/>
-    </row>
-    <row r="112" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C112" s="23" t="s">
+      <c r="E113" s="16"/>
+      <c r="F113" s="16"/>
+      <c r="G113" s="16"/>
+    </row>
+    <row r="114" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C114" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="D112" s="23">
+      <c r="D114" s="23">
         <v>0.5</v>
       </c>
-      <c r="E112" s="24">
-        <f t="shared" ref="E112:G117" si="20">Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E84)</f>
-        <v>10.393921185015483</v>
-      </c>
-      <c r="F112" s="24">
-        <f t="shared" si="20"/>
-        <v>10.030118683410457</v>
-      </c>
-      <c r="G112" s="24">
-        <f t="shared" si="20"/>
-        <v>10.159991169312509</v>
-      </c>
-    </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C113" s="23" t="s">
+      <c r="E114" s="24">
+        <f t="shared" ref="E114:G119" si="15">Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E86)</f>
+        <v>12.47270542201858</v>
+      </c>
+      <c r="F114" s="24">
+        <f t="shared" si="15"/>
+        <v>12.036142420092549</v>
+      </c>
+      <c r="G114" s="24">
+        <f t="shared" si="15"/>
+        <v>12.191989403175011</v>
+      </c>
+    </row>
+    <row r="115" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C115" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="D113" s="23">
+      <c r="D115" s="23">
         <v>1</v>
       </c>
-      <c r="E113" s="24">
-        <f t="shared" si="20"/>
-        <v>5.8045528739959602</v>
-      </c>
-      <c r="F113" s="24">
-        <f t="shared" si="20"/>
-        <v>5.3661985891606596</v>
-      </c>
-      <c r="G113" s="24">
-        <f t="shared" si="20"/>
-        <v>5.5182233585799088</v>
-      </c>
-    </row>
-    <row r="114" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C114" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D114" s="14">
-        <v>2</v>
-      </c>
-      <c r="E114" s="15">
-        <f t="shared" si="20"/>
-        <v>3.8054926752552789</v>
-      </c>
-      <c r="F114" s="15">
-        <f t="shared" si="20"/>
-        <v>3.1249586460082184</v>
-      </c>
-      <c r="G114" s="15">
-        <f t="shared" si="20"/>
-        <v>3.34253022359679</v>
-      </c>
-    </row>
-    <row r="115" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C115" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="D115" s="14">
-        <v>3</v>
-      </c>
-      <c r="E115" s="15">
-        <f t="shared" si="20"/>
-        <v>3.717309172657397</v>
-      </c>
-      <c r="F115" s="15">
-        <f t="shared" si="20"/>
-        <v>2.5004675305962909</v>
-      </c>
-      <c r="G115" s="15">
-        <f t="shared" si="20"/>
-        <v>2.837825302119557</v>
+      <c r="E115" s="24">
+        <f t="shared" si="15"/>
+        <v>6.9654634487951519</v>
+      </c>
+      <c r="F115" s="24">
+        <f t="shared" si="15"/>
+        <v>6.4394383069927912</v>
+      </c>
+      <c r="G115" s="24">
+        <f t="shared" si="15"/>
+        <v>6.6218680302958912</v>
       </c>
     </row>
     <row r="116" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C116" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D116" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E116" s="15">
-        <f t="shared" si="20"/>
-        <v>5.3081047689566478</v>
+        <f t="shared" si="15"/>
+        <v>4.5665912103063349</v>
       </c>
       <c r="F116" s="15">
-        <f t="shared" si="20"/>
-        <v>2.3526372364281896</v>
+        <f t="shared" si="15"/>
+        <v>3.749950375209862</v>
       </c>
       <c r="G116" s="15">
-        <f t="shared" si="20"/>
-        <v>2.9471866006451912</v>
+        <f t="shared" si="15"/>
+        <v>4.0110362683161478</v>
       </c>
     </row>
     <row r="117" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C117" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D117" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E117" s="15">
-        <f t="shared" si="20"/>
-        <v>54.883363868245084</v>
+        <f t="shared" si="15"/>
+        <v>4.4607710071888764</v>
       </c>
       <c r="F117" s="15">
-        <f t="shared" si="20"/>
-        <v>2.5361039564424659</v>
+        <f t="shared" si="15"/>
+        <v>3.0005610367155491</v>
       </c>
       <c r="G117" s="15">
-        <f t="shared" si="20"/>
-        <v>3.8705216300526137</v>
+        <f t="shared" si="15"/>
+        <v>3.4053903625434692</v>
       </c>
     </row>
     <row r="118" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C118" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D118" s="14">
+        <v>4</v>
+      </c>
+      <c r="E118" s="15">
+        <f t="shared" si="15"/>
+        <v>6.3697257227479769</v>
+      </c>
+      <c r="F118" s="15">
+        <f t="shared" si="15"/>
+        <v>2.8231646837138276</v>
+      </c>
+      <c r="G118" s="15">
+        <f t="shared" si="15"/>
+        <v>3.5366239207742294</v>
+      </c>
+    </row>
+    <row r="119" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C119" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D119" s="14">
+        <v>5</v>
+      </c>
+      <c r="E119" s="15">
+        <f t="shared" si="15"/>
+        <v>65.860036641894098</v>
+      </c>
+      <c r="F119" s="15">
+        <f t="shared" si="15"/>
+        <v>3.0433247477309586</v>
+      </c>
+      <c r="G119" s="15">
+        <f t="shared" si="15"/>
+        <v>4.6446259560631358</v>
+      </c>
+    </row>
+    <row r="120" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C120" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="D118" s="14">
+      <c r="D120" s="14">
         <v>6</v>
       </c>
-      <c r="E118" s="31" t="s">
+      <c r="E120" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="F118" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F90)</f>
-        <v>3.2619978644141554</v>
-      </c>
-      <c r="G118" s="15">
-        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G90)</f>
-        <v>9.2663659785740737</v>
-      </c>
-    </row>
-    <row r="120" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C120" t="s">
+      <c r="F120" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F92)</f>
+        <v>3.9143974372969867</v>
+      </c>
+      <c r="G120" s="15">
+        <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G92)</f>
+        <v>11.119639174288887</v>
+      </c>
+    </row>
+    <row r="122" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
         <v>123</v>
       </c>
-      <c r="D120" s="20">
+      <c r="D122" s="20">
         <v>0</v>
       </c>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
-      <c r="G120" s="4"/>
-    </row>
-    <row r="121" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C121" s="23" t="s">
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+    </row>
+    <row r="123" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C123" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="D121" s="23">
+      <c r="D123" s="23">
         <v>0.5</v>
       </c>
-      <c r="E121" s="24">
-        <f t="shared" ref="E121:G126" si="21">(Engine_service_interval__h/E93)/24</f>
+      <c r="E123" s="24">
+        <f t="shared" ref="E123:G128" si="16">(Engine_service_interval__h/E95)/24</f>
         <v>443.67820583564179</v>
       </c>
-      <c r="F121" s="24">
-        <f t="shared" si="21"/>
-        <v>682.53220583564155</v>
-      </c>
-      <c r="G121" s="24">
-        <f t="shared" si="21"/>
-        <v>570.38896583564167</v>
-      </c>
-    </row>
-    <row r="122" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C122" s="23" t="s">
+      <c r="F123" s="24">
+        <f t="shared" si="16"/>
+        <v>682.53220583564166</v>
+      </c>
+      <c r="G123" s="24">
+        <f t="shared" si="16"/>
+        <v>570.38896583564178</v>
+      </c>
+    </row>
+    <row r="124" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C124" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="D122" s="23">
+      <c r="D124" s="23">
         <v>1</v>
       </c>
-      <c r="E122" s="24">
-        <f t="shared" si="21"/>
-        <v>220.7426116897507</v>
-      </c>
-      <c r="F122" s="24">
-        <f t="shared" si="21"/>
+      <c r="E124" s="24">
+        <f t="shared" si="16"/>
+        <v>220.74261168975067</v>
+      </c>
+      <c r="F124" s="24">
+        <f t="shared" si="16"/>
         <v>340.16961168975064</v>
       </c>
-      <c r="G122" s="24">
-        <f t="shared" si="21"/>
+      <c r="G124" s="24">
+        <f t="shared" si="16"/>
         <v>284.0979916897507</v>
-      </c>
-    </row>
-    <row r="123" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C123" t="s">
-        <v>124</v>
-      </c>
-      <c r="D123" s="20">
-        <v>2</v>
-      </c>
-      <c r="E123" s="7">
-        <f t="shared" si="21"/>
-        <v>109.27481461680516</v>
-      </c>
-      <c r="F123" s="7">
-        <f t="shared" si="21"/>
-        <v>168.98831461680513</v>
-      </c>
-      <c r="G123" s="7">
-        <f t="shared" si="21"/>
-        <v>140.95250461680516</v>
-      </c>
-    </row>
-    <row r="124" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C124" t="s">
-        <v>158</v>
-      </c>
-      <c r="D124" s="20">
-        <v>3</v>
-      </c>
-      <c r="E124" s="7">
-        <f t="shared" si="21"/>
-        <v>72.118882259156663</v>
-      </c>
-      <c r="F124" s="7">
-        <f t="shared" si="21"/>
-        <v>111.92788225915665</v>
-      </c>
-      <c r="G124" s="7">
-        <f t="shared" si="21"/>
-        <v>93.237342259156648</v>
       </c>
     </row>
     <row r="125" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C125" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D125" s="20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E125" s="7">
-        <f t="shared" si="21"/>
-        <v>53.540916080332408</v>
+        <f t="shared" si="16"/>
+        <v>109.27481461680516</v>
       </c>
       <c r="F125" s="7">
-        <f t="shared" si="21"/>
-        <v>83.397666080332399</v>
+        <f t="shared" si="16"/>
+        <v>168.98831461680516</v>
       </c>
       <c r="G125" s="7">
-        <f t="shared" si="21"/>
-        <v>69.379761080332415</v>
+        <f t="shared" si="16"/>
+        <v>140.95250461680516</v>
       </c>
     </row>
     <row r="126" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D126" s="20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E126" s="7">
-        <f t="shared" si="21"/>
-        <v>42.394136373037853</v>
+        <f t="shared" si="16"/>
+        <v>72.118882259156663</v>
       </c>
       <c r="F126" s="7">
-        <f t="shared" si="21"/>
-        <v>66.279536373037857</v>
+        <f t="shared" si="16"/>
+        <v>111.92788225915666</v>
       </c>
       <c r="G126" s="7">
-        <f t="shared" si="21"/>
-        <v>55.065212373037859</v>
+        <f t="shared" si="16"/>
+        <v>93.237342259156662</v>
       </c>
     </row>
     <row r="127" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C127" t="s">
+        <v>125</v>
+      </c>
+      <c r="D127" s="20">
+        <v>4</v>
+      </c>
+      <c r="E127" s="7">
+        <f t="shared" si="16"/>
+        <v>53.540916080332408</v>
+      </c>
+      <c r="F127" s="7">
+        <f t="shared" si="16"/>
+        <v>83.397666080332399</v>
+      </c>
+      <c r="G127" s="7">
+        <f t="shared" si="16"/>
+        <v>69.379761080332415</v>
+      </c>
+    </row>
+    <row r="128" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
+        <v>159</v>
+      </c>
+      <c r="D128" s="20">
+        <v>5</v>
+      </c>
+      <c r="E128" s="7">
+        <f t="shared" si="16"/>
+        <v>42.39413637303786</v>
+      </c>
+      <c r="F128" s="7">
+        <f t="shared" si="16"/>
+        <v>66.279536373037843</v>
+      </c>
+      <c r="G128" s="7">
+        <f t="shared" si="16"/>
+        <v>55.065212373037845</v>
+      </c>
+    </row>
+    <row r="129" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
         <v>126</v>
       </c>
-      <c r="D127" s="20">
+      <c r="D129" s="20">
         <v>6</v>
       </c>
-      <c r="E127" s="31" t="s">
+      <c r="E129" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="F127" s="7">
-        <f>(Engine_service_interval__h/F99)/24</f>
-        <v>54.867449901508138</v>
-      </c>
-      <c r="G127" s="7">
-        <f>(Engine_service_interval__h/G99)/24</f>
+      <c r="F129" s="7">
+        <f>(Engine_service_interval__h/F101)/24</f>
+        <v>54.867449901508145</v>
+      </c>
+      <c r="G129" s="7">
+        <f>(Engine_service_interval__h/G101)/24</f>
         <v>45.522179901508146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor tweaks to DOD and various efficiencies based on early HyGen v2 runs.
</commit_message>
<xml_diff>
--- a/Control and Data Systems/BMs Hygen System Design Calcs.xlsx
+++ b/Control and Data Systems/BMs Hygen System Design Calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="15315" windowHeight="12075" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="15315" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Beckett Battery Modules" sheetId="1" r:id="rId1"/>
@@ -78,11 +78,12 @@
     <definedName name="Voltage_at_80">'Beckett Battery Modules'!$C$13</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="192">
   <si>
     <t>Boston Swing 5300</t>
   </si>
@@ -646,6 +647,18 @@
   </si>
   <si>
     <t>PPI 50% DOD guestimate</t>
+  </si>
+  <si>
+    <t>Updates</t>
+  </si>
+  <si>
+    <t>Our voltage limit switches are giving us about 16% to 79% SOC.</t>
+  </si>
+  <si>
+    <t>We're actually running the NovaTorque above it spec.</t>
+  </si>
+  <si>
+    <t>BK calculated this efficiency from our first 4kW Charge/Discharge cycle test.</t>
   </si>
 </sst>
 </file>
@@ -738,7 +751,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -868,6 +881,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -989,25 +1005,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>31.254189908802292</c:v>
+                  <c:v>32.288440184051723</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.56701324327401</c:v>
+                  <c:v>16.068765661633794</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.7234249105098725</c:v>
+                  <c:v>7.9589284004248251</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.1088954662551593</c:v>
+                  <c:v>5.2556493133551694</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8016307441278037</c:v>
+                  <c:v>3.9040097698203415</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.017271910851389</c:v>
+                  <c:v>3.0930260436994446</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4943660220004467</c:v>
+                  <c:v>2.5523702262855132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1057,25 +1073,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12.191989403175011</c:v>
+                  <c:v>15.323226339665265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.6218680302958912</c:v>
+                  <c:v>8.2990154268002563</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0110362683161478</c:v>
+                  <c:v>4.991917134927097</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4053903625434692</c:v>
+                  <c:v>4.1961251038281713</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5366239207742294</c:v>
+                  <c:v>4.2871141590662507</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.6446259560631358</c:v>
+                  <c:v>5.4380417748215653</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.119639174288887</c:v>
+                  <c:v>11.248220551248643</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1090,11 +1106,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185335808"/>
-        <c:axId val="185337728"/>
+        <c:axId val="121258368"/>
+        <c:axId val="121261440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="185335808"/>
+        <c:axId val="121258368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1124,14 +1140,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185337728"/>
+        <c:crossAx val="121261440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185337728"/>
+        <c:axId val="121261440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="20"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1159,9 +1176,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185335808"/>
+        <c:crossAx val="121258368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1513,11 +1531,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186205312"/>
-        <c:axId val="186207616"/>
+        <c:axId val="170325120"/>
+        <c:axId val="170327424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186205312"/>
+        <c:axId val="170325120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1553,19 +1571,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186207616"/>
+        <c:crossAx val="170327424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186207616"/>
+        <c:axId val="170327424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1595,14 +1612,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186205312"/>
+        <c:crossAx val="170325120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -1611,7 +1627,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2039,11 +2054,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186292480"/>
-        <c:axId val="186298368"/>
+        <c:axId val="171512576"/>
+        <c:axId val="171514112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186292480"/>
+        <c:axId val="171512576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2054,13 +2069,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186298368"/>
+        <c:crossAx val="171514112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186298368"/>
+        <c:axId val="171514112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2073,14 +2088,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186292480"/>
+        <c:crossAx val="171512576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2235,8 +2249,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185381248"/>
-        <c:axId val="185383168"/>
+        <c:axId val="190689280"/>
+        <c:axId val="190691200"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2328,11 +2342,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185391360"/>
-        <c:axId val="185389440"/>
+        <c:axId val="169027840"/>
+        <c:axId val="169025920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="185381248"/>
+        <c:axId val="190689280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2362,12 +2376,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185383168"/>
+        <c:crossAx val="190691200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185383168"/>
+        <c:axId val="190691200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2397,12 +2411,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185381248"/>
+        <c:crossAx val="190689280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185389440"/>
+        <c:axId val="169025920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="270"/>
@@ -2433,13 +2447,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185391360"/>
+        <c:crossAx val="169027840"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185391360"/>
+        <c:axId val="169027840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2449,7 +2463,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185389440"/>
+        <c:crossAx val="169025920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2507,7 +2521,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2592,8 +2605,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185959552"/>
-        <c:axId val="185961472"/>
+        <c:axId val="169043072"/>
+        <c:axId val="169044992"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2695,13 +2708,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="1">
-                  <c:v>570.38896583564178</c:v>
+                  <c:v>589.26403335894395</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>284.0979916897507</c:v>
+                  <c:v>293.25497332481672</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>140.95250461680516</c:v>
+                  <c:v>145.25044330775305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2716,11 +2729,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185965568"/>
-        <c:axId val="185963648"/>
+        <c:axId val="169053184"/>
+        <c:axId val="169051264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="185959552"/>
+        <c:axId val="169043072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -2744,20 +2757,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185961472"/>
+        <c:crossAx val="169044992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185961472"/>
+        <c:axId val="169044992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2780,19 +2792,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185959552"/>
+        <c:crossAx val="169043072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185963648"/>
+        <c:axId val="169051264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="540"/>
@@ -2816,20 +2827,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185965568"/>
+        <c:crossAx val="169053184"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185965568"/>
+        <c:axId val="169053184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2839,7 +2849,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185963648"/>
+        <c:crossAx val="169051264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2852,7 +2862,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2954,13 +2963,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>31.254189908802292</c:v>
+                  <c:v>32.288440184051723</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.56701324327401</c:v>
+                  <c:v>16.068765661633794</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.7234249105098725</c:v>
+                  <c:v>7.9589284004248251</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2998,13 +3007,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12.191989403175011</c:v>
+                  <c:v>15.323226339665265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.6218680302958912</c:v>
+                  <c:v>8.2990154268002563</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0110362683161478</c:v>
+                  <c:v>4.991917134927097</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3019,11 +3028,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186070528"/>
-        <c:axId val="186072448"/>
+        <c:axId val="169152512"/>
+        <c:axId val="169154432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186070528"/>
+        <c:axId val="169152512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -3047,20 +3056,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186072448"/>
+        <c:crossAx val="169154432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186072448"/>
+        <c:axId val="169154432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3083,21 +3091,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186070528"/>
+        <c:crossAx val="169152512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3780,11 +3786,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185496704"/>
-        <c:axId val="185499008"/>
+        <c:axId val="169245696"/>
+        <c:axId val="169248256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="185496704"/>
+        <c:axId val="169245696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3820,19 +3826,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185499008"/>
+        <c:crossAx val="169248256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185499008"/>
+        <c:axId val="169248256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -3862,14 +3867,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185496704"/>
+        <c:crossAx val="169245696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -3878,7 +3882,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3923,7 +3926,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4032,8 +4034,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185546240"/>
-        <c:axId val="185548160"/>
+        <c:axId val="169267584"/>
+        <c:axId val="169269504"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -4125,11 +4127,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185556352"/>
-        <c:axId val="185554432"/>
+        <c:axId val="169273600"/>
+        <c:axId val="169271680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="185546240"/>
+        <c:axId val="169267584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4152,19 +4154,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185548160"/>
+        <c:crossAx val="169269504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185548160"/>
+        <c:axId val="169269504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4187,19 +4188,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185546240"/>
+        <c:crossAx val="169267584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185554432"/>
+        <c:axId val="169271680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="270"/>
@@ -4223,20 +4223,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185556352"/>
+        <c:crossAx val="169273600"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185556352"/>
+        <c:axId val="169273600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4246,7 +4245,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185554432"/>
+        <c:crossAx val="169271680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4259,7 +4258,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4304,7 +4302,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4389,8 +4386,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185586432"/>
-        <c:axId val="185588352"/>
+        <c:axId val="169583744"/>
+        <c:axId val="169585664"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -4513,11 +4510,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="184027776"/>
-        <c:axId val="184025856"/>
+        <c:axId val="169597952"/>
+        <c:axId val="169596032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="185586432"/>
+        <c:axId val="169583744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -4541,20 +4538,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185588352"/>
+        <c:crossAx val="169585664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185588352"/>
+        <c:axId val="169585664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4577,19 +4573,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185586432"/>
+        <c:crossAx val="169583744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="184025856"/>
+        <c:axId val="169596032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="540"/>
@@ -4613,20 +4608,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184027776"/>
+        <c:crossAx val="169597952"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="184027776"/>
+        <c:axId val="169597952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4636,7 +4630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184025856"/>
+        <c:crossAx val="169596032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4649,7 +4643,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4816,11 +4809,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="184044544"/>
-        <c:axId val="184059008"/>
+        <c:axId val="169794560"/>
+        <c:axId val="169800832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="184044544"/>
+        <c:axId val="169794560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -4844,20 +4837,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184059008"/>
+        <c:crossAx val="169800832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="184059008"/>
+        <c:axId val="169800832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4880,21 +4872,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184044544"/>
+        <c:crossAx val="169794560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5318,11 +5308,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186137984"/>
-        <c:axId val="186140544"/>
+        <c:axId val="170274176"/>
+        <c:axId val="170284928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186137984"/>
+        <c:axId val="170274176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5358,19 +5348,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186140544"/>
+        <c:crossAx val="170284928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186140544"/>
+        <c:axId val="170284928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -5400,14 +5389,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186137984"/>
+        <c:crossAx val="170274176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -5416,7 +5404,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7320,8 +7307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7337,12 +7324,17 @@
     <col min="9" max="14" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="55" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>80</v>
       </c>
@@ -7356,7 +7348,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>82</v>
       </c>
@@ -7371,7 +7363,7 @@
         <v>8760</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>83</v>
       </c>
@@ -7386,7 +7378,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>169</v>
       </c>
@@ -7395,7 +7387,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>170</v>
       </c>
@@ -7405,21 +7397,24 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D19" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+        <v>0.63</v>
+      </c>
+      <c r="H19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>88</v>
       </c>
       <c r="D20">
         <f>D19*Batt_bank_energy__kWh*Avg_bank_energy_over_lifetime</f>
-        <v>4.95</v>
+        <v>6.2370000000000001</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>160</v>
@@ -7428,7 +7423,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>117</v>
       </c>
@@ -7442,7 +7437,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>171</v>
       </c>
@@ -7456,17 +7451,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="19"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>63</v>
       </c>
@@ -7480,7 +7475,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="F28" s="1" t="s">
         <v>89</v>
       </c>
@@ -7488,7 +7483,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>8</v>
       </c>
@@ -7505,7 +7500,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" t="s">
         <v>52</v>
@@ -7520,7 +7515,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>50</v>
       </c>
@@ -7540,7 +7535,7 @@
         <v>9.0269999999999992</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" t="s">
         <v>53</v>
@@ -7625,7 +7620,10 @@
         <v>8.8593119999999992</v>
       </c>
       <c r="G36" s="10">
-        <v>7.5</v>
+        <v>7.75</v>
+      </c>
+      <c r="H36" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
@@ -7660,7 +7658,7 @@
       </c>
       <c r="G38" s="35">
         <f>G37*G36</f>
-        <v>7.4249999999999998</v>
+        <v>7.6725000000000003</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
@@ -7675,7 +7673,10 @@
         <v>0.95</v>
       </c>
       <c r="G39" s="34">
-        <v>0.95</v>
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="H39" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
@@ -7695,7 +7696,7 @@
       </c>
       <c r="G40" s="35">
         <f>G39*G38</f>
-        <v>7.0537499999999991</v>
+        <v>7.1968049999999995</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
@@ -7730,7 +7731,7 @@
       </c>
       <c r="G42" s="34">
         <f>G39</f>
-        <v>0.95</v>
+        <v>0.93799999999999994</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
@@ -7750,7 +7751,7 @@
       </c>
       <c r="G43" s="36">
         <f>G41/G42</f>
-        <v>0.52631578947368418</v>
+        <v>0.53304904051172708</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
@@ -7770,7 +7771,7 @@
       </c>
       <c r="G44" s="37">
         <f>G40-G43</f>
-        <v>6.527434210526315</v>
+        <v>6.663755959488272</v>
       </c>
     </row>
     <row r="45" spans="2:14" ht="45" x14ac:dyDescent="0.25">
@@ -7816,7 +7817,7 @@
       </c>
       <c r="M46" s="4"/>
       <c r="N46">
-        <f>I46*24*SFC__l_kWh</f>
+        <f t="shared" ref="N46:N53" si="1">I46*24*SFC__l_kWh</f>
         <v>0</v>
       </c>
     </row>
@@ -7840,19 +7841,19 @@
         <v>139.08000000000001</v>
       </c>
       <c r="K47" s="30">
-        <f t="shared" ref="K47:K53" si="1">Fuel_Tank_Capacity__l/($I47*24*SFC__l_kWh)</f>
+        <f t="shared" ref="K47:K53" si="2">Fuel_Tank_Capacity__l/($I47*24*SFC__l_kWh)</f>
         <v>219.29824561403507</v>
       </c>
       <c r="L47" s="30">
-        <f t="shared" ref="L47:L53" si="2">K47/4</f>
+        <f t="shared" ref="L47:L53" si="3">K47/4</f>
         <v>54.824561403508767</v>
       </c>
       <c r="M47" s="24">
-        <f t="shared" ref="M47:M53" si="3">G123</f>
-        <v>570.38896583564178</v>
+        <f t="shared" ref="M47:M53" si="4">G123</f>
+        <v>589.26403335894395</v>
       </c>
       <c r="N47">
-        <f>I47*24*SFC__l_kWh</f>
+        <f t="shared" si="1"/>
         <v>4.5600000000000005</v>
       </c>
     </row>
@@ -7867,16 +7868,16 @@
         <v>0</v>
       </c>
       <c r="E48" s="11">
-        <f t="shared" ref="E48:G55" si="4">E$38-($D48+E$43)/E$39</f>
+        <f t="shared" ref="E48:G55" si="5">E$38-($D48+E$43)/E$39</f>
         <v>5.3504542595013849</v>
       </c>
       <c r="F48" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.2167022595013837</v>
       </c>
-      <c r="G48" s="11">
-        <f t="shared" si="4"/>
-        <v>6.8709833795013848</v>
+      <c r="G48" s="13">
+        <f t="shared" si="5"/>
+        <v>7.1042174408190544</v>
       </c>
       <c r="H48" s="11"/>
       <c r="I48" s="29">
@@ -7887,19 +7888,19 @@
         <v>278.16000000000003</v>
       </c>
       <c r="K48" s="30">
+        <f t="shared" si="2"/>
+        <v>109.64912280701753</v>
+      </c>
+      <c r="L48" s="30">
+        <f t="shared" si="3"/>
+        <v>27.412280701754383</v>
+      </c>
+      <c r="M48" s="24">
+        <f t="shared" si="4"/>
+        <v>293.25497332481672</v>
+      </c>
+      <c r="N48">
         <f t="shared" si="1"/>
-        <v>109.64912280701753</v>
-      </c>
-      <c r="L48" s="30">
-        <f t="shared" si="2"/>
-        <v>27.412280701754383</v>
-      </c>
-      <c r="M48" s="24">
-        <f t="shared" si="3"/>
-        <v>284.0979916897507</v>
-      </c>
-      <c r="N48">
-        <f>I48*24*SFC__l_kWh</f>
         <v>9.120000000000001</v>
       </c>
     </row>
@@ -7912,16 +7913,16 @@
         <v>0.5</v>
       </c>
       <c r="E49" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.8241384700277008</v>
       </c>
       <c r="F49" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.6903864700276996</v>
       </c>
       <c r="G49" s="11">
-        <f t="shared" si="4"/>
-        <v>6.3446675900277008</v>
+        <f t="shared" si="5"/>
+        <v>6.5711684003073279</v>
       </c>
       <c r="H49" s="11"/>
       <c r="I49" s="4">
@@ -7932,19 +7933,19 @@
         <v>556.32000000000005</v>
       </c>
       <c r="K49" s="3">
+        <f t="shared" si="2"/>
+        <v>54.824561403508767</v>
+      </c>
+      <c r="L49" s="3">
+        <f t="shared" si="3"/>
+        <v>13.706140350877192</v>
+      </c>
+      <c r="M49" s="7">
+        <f t="shared" si="4"/>
+        <v>145.25044330775305</v>
+      </c>
+      <c r="N49">
         <f t="shared" si="1"/>
-        <v>54.824561403508767</v>
-      </c>
-      <c r="L49" s="3">
-        <f t="shared" si="2"/>
-        <v>13.706140350877192</v>
-      </c>
-      <c r="M49" s="7">
-        <f t="shared" si="3"/>
-        <v>140.95250461680516</v>
-      </c>
-      <c r="N49">
-        <f>I49*24*SFC__l_kWh</f>
         <v>18.240000000000002</v>
       </c>
     </row>
@@ -7957,16 +7958,16 @@
         <v>1</v>
       </c>
       <c r="E50" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.2978226805540167</v>
       </c>
       <c r="F50" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.1640706805540155</v>
       </c>
       <c r="G50" s="11">
-        <f t="shared" si="4"/>
-        <v>5.8183518005540167</v>
+        <f t="shared" si="5"/>
+        <v>6.0381193597956004</v>
       </c>
       <c r="H50" s="11"/>
       <c r="I50" s="4">
@@ -7977,19 +7978,19 @@
         <v>834.48</v>
       </c>
       <c r="K50" s="3">
+        <f t="shared" si="2"/>
+        <v>36.549707602339183</v>
+      </c>
+      <c r="L50" s="3">
+        <f t="shared" si="3"/>
+        <v>9.1374269005847957</v>
+      </c>
+      <c r="M50" s="7">
+        <f t="shared" si="4"/>
+        <v>95.91559996873184</v>
+      </c>
+      <c r="N50">
         <f t="shared" si="1"/>
-        <v>36.549707602339183</v>
-      </c>
-      <c r="L50" s="3">
-        <f t="shared" si="2"/>
-        <v>9.1374269005847957</v>
-      </c>
-      <c r="M50" s="7">
-        <f t="shared" si="3"/>
-        <v>93.237342259156662</v>
-      </c>
-      <c r="N50">
-        <f>I50*24*SFC__l_kWh</f>
         <v>27.36</v>
       </c>
     </row>
@@ -8002,16 +8003,16 @@
         <v>2</v>
       </c>
       <c r="E51" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.2451911016066481</v>
       </c>
       <c r="F51" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.1114391016066474</v>
       </c>
       <c r="G51" s="11">
-        <f t="shared" si="4"/>
-        <v>4.7657202216066477</v>
+        <f t="shared" si="5"/>
+        <v>4.9720212787721465</v>
       </c>
       <c r="H51" s="11"/>
       <c r="I51" s="4">
@@ -8022,19 +8023,19 @@
         <v>1112.6400000000001</v>
       </c>
       <c r="K51" s="3">
+        <f t="shared" si="2"/>
+        <v>27.412280701754383</v>
+      </c>
+      <c r="L51" s="3">
+        <f t="shared" si="3"/>
+        <v>6.8530701754385959</v>
+      </c>
+      <c r="M51" s="7">
+        <f t="shared" si="4"/>
+        <v>71.248178299221237</v>
+      </c>
+      <c r="N51">
         <f t="shared" si="1"/>
-        <v>27.412280701754383</v>
-      </c>
-      <c r="L51" s="3">
-        <f t="shared" si="2"/>
-        <v>6.8530701754385959</v>
-      </c>
-      <c r="M51" s="7">
-        <f t="shared" si="3"/>
-        <v>69.379761080332415</v>
-      </c>
-      <c r="N51">
-        <f>I51*24*SFC__l_kWh</f>
         <v>36.480000000000004</v>
       </c>
     </row>
@@ -8047,16 +8048,16 @@
         <v>3</v>
       </c>
       <c r="E52" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.1925595226592796</v>
       </c>
       <c r="F52" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.0588075226592784</v>
       </c>
       <c r="G52" s="11">
-        <f t="shared" si="4"/>
-        <v>3.7130886426592795</v>
+        <f t="shared" si="5"/>
+        <v>3.9059231977486921</v>
       </c>
       <c r="H52" s="11"/>
       <c r="I52" s="4">
@@ -8067,19 +8068,19 @@
         <v>1390.8</v>
       </c>
       <c r="K52" s="3">
+        <f t="shared" si="2"/>
+        <v>21.929824561403507</v>
+      </c>
+      <c r="L52" s="3">
+        <f t="shared" si="3"/>
+        <v>5.4824561403508767</v>
+      </c>
+      <c r="M52" s="7">
+        <f t="shared" si="4"/>
+        <v>56.447725297514857</v>
+      </c>
+      <c r="N52">
         <f t="shared" si="1"/>
-        <v>21.929824561403507</v>
-      </c>
-      <c r="L52" s="3">
-        <f t="shared" si="2"/>
-        <v>5.4824561403508767</v>
-      </c>
-      <c r="M52" s="7">
-        <f t="shared" si="3"/>
-        <v>55.065212373037845</v>
-      </c>
-      <c r="N52">
-        <f>I52*24*SFC__l_kWh</f>
         <v>45.6</v>
       </c>
     </row>
@@ -8092,16 +8093,16 @@
         <v>4</v>
       </c>
       <c r="E53" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.1399279437119114</v>
       </c>
       <c r="F53" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.0061759437119102</v>
       </c>
       <c r="G53" s="11">
-        <f t="shared" si="4"/>
-        <v>2.6604570637119114</v>
+        <f t="shared" si="5"/>
+        <v>2.8398251167252377</v>
       </c>
       <c r="H53" s="11"/>
       <c r="I53" s="4">
@@ -8112,19 +8113,19 @@
         <v>1668.96</v>
       </c>
       <c r="K53" s="3">
+        <f t="shared" si="2"/>
+        <v>18.274853801169591</v>
+      </c>
+      <c r="L53" s="3">
+        <f t="shared" si="3"/>
+        <v>4.5687134502923978</v>
+      </c>
+      <c r="M53" s="7">
+        <f t="shared" si="4"/>
+        <v>46.580756629710613</v>
+      </c>
+      <c r="N53">
         <f t="shared" si="1"/>
-        <v>18.274853801169591</v>
-      </c>
-      <c r="L53" s="3">
-        <f t="shared" si="2"/>
-        <v>4.5687134502923978</v>
-      </c>
-      <c r="M53" s="7">
-        <f t="shared" si="3"/>
-        <v>45.522179901508146</v>
-      </c>
-      <c r="N53">
-        <f>I53*24*SFC__l_kWh</f>
         <v>54.72</v>
       </c>
     </row>
@@ -8137,16 +8138,16 @@
         <v>5</v>
       </c>
       <c r="E54" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.7296364764542389E-2</v>
       </c>
       <c r="F54" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.9535443647645412</v>
       </c>
       <c r="G54" s="11">
-        <f t="shared" si="4"/>
-        <v>1.6078254847645423</v>
+        <f t="shared" si="5"/>
+        <v>1.7737270357017829</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
@@ -8158,16 +8159,16 @@
         <v>6</v>
       </c>
       <c r="E55" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.96533521418282575</v>
       </c>
       <c r="F55" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.900912785817173</v>
       </c>
       <c r="G55" s="11">
-        <f t="shared" si="4"/>
-        <v>0.5551939058171742</v>
+        <f t="shared" si="5"/>
+        <v>0.70762895467832898</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
@@ -8181,16 +8182,16 @@
       </c>
       <c r="D57" s="17"/>
       <c r="E57" s="21">
-        <f t="shared" ref="E57:G64" si="5">E48/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
+        <f t="shared" ref="E57:G64" si="6">E48/(Batt_bank_energy__kWh *Avg_bank_energy_over_lifetime)</f>
         <v>0.54044992520216006</v>
       </c>
       <c r="F57" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.82996992520215995</v>
       </c>
       <c r="G57" s="21">
-        <f t="shared" si="5"/>
-        <v>0.69403872520216003</v>
+        <f t="shared" si="6"/>
+        <v>0.717597721294854</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
@@ -8199,16 +8200,16 @@
       </c>
       <c r="D58" s="17"/>
       <c r="E58" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.48728671414421221</v>
       </c>
       <c r="F58" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.7768067141442121</v>
       </c>
       <c r="G58" s="21">
-        <f t="shared" si="5"/>
-        <v>0.64087551414421218</v>
+        <f t="shared" si="6"/>
+        <v>0.66375438386942698</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
@@ -8217,16 +8218,16 @@
       </c>
       <c r="D59" s="17"/>
       <c r="E59" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.4341235030862643</v>
       </c>
       <c r="F59" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.72364350308626413</v>
       </c>
       <c r="G59" s="21">
-        <f t="shared" si="5"/>
-        <v>0.58771230308626432</v>
+        <f t="shared" si="6"/>
+        <v>0.60991104644400007</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
@@ -8235,16 +8236,16 @@
       </c>
       <c r="D60" s="17"/>
       <c r="E60" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.32779708097036847</v>
       </c>
       <c r="F60" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.61731708097036841</v>
       </c>
       <c r="G60" s="18">
-        <f t="shared" si="5"/>
-        <v>0.48138588097036844</v>
+        <f t="shared" si="6"/>
+        <v>0.50222437159314615</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
@@ -8253,16 +8254,16 @@
       </c>
       <c r="D61" s="17"/>
       <c r="E61" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.22147065885447267</v>
       </c>
       <c r="F61" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.51099065885447259</v>
       </c>
       <c r="G61" s="18">
-        <f t="shared" si="5"/>
-        <v>0.37505945885447267</v>
+        <f t="shared" si="6"/>
+        <v>0.39453769674229211</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
@@ -8271,16 +8272,16 @@
       </c>
       <c r="D62" s="17"/>
       <c r="E62" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.1151442367385769</v>
       </c>
       <c r="F62" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.40466423673857677</v>
       </c>
       <c r="G62" s="18">
-        <f t="shared" si="5"/>
-        <v>0.2687330367385769</v>
+        <f t="shared" si="6"/>
+        <v>0.28685102189143813</v>
       </c>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
@@ -8289,16 +8290,16 @@
       </c>
       <c r="D63" s="17"/>
       <c r="E63" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.8178146226810493E-3</v>
       </c>
       <c r="F63" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.29833781462268094</v>
       </c>
       <c r="G63" s="18">
-        <f t="shared" si="5"/>
-        <v>0.16240661462268105</v>
+        <f t="shared" si="6"/>
+        <v>0.17916434704058412</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
@@ -8307,16 +8308,16 @@
       </c>
       <c r="D64" s="17"/>
       <c r="E64" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-9.7508607493214716E-2</v>
       </c>
       <c r="F64" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.19201139250678514</v>
       </c>
       <c r="G64" s="18">
-        <f t="shared" si="5"/>
-        <v>5.6080192506785274E-2</v>
+        <f t="shared" si="6"/>
+        <v>7.1477672189730196E-2</v>
       </c>
     </row>
     <row r="66" spans="2:18" x14ac:dyDescent="0.25">
@@ -8327,16 +8328,16 @@
         <v>91</v>
       </c>
       <c r="E66" s="13">
-        <f t="shared" ref="E66:G73" si="6">1/E57*Depth_of_Discharge</f>
-        <v>0.9251550914970903</v>
+        <f t="shared" ref="E66:G73" si="7">1/E57*Depth_of_Discharge</f>
+        <v>1.1656954152863337</v>
       </c>
       <c r="F66" s="13">
-        <f t="shared" si="6"/>
-        <v>0.60243146747541787</v>
+        <f t="shared" si="7"/>
+        <v>0.75906364901902657</v>
       </c>
       <c r="G66" s="13">
-        <f t="shared" si="6"/>
-        <v>0.72042089561264711</v>
+        <f t="shared" si="7"/>
+        <v>0.877929209227713</v>
       </c>
     </row>
     <row r="67" spans="2:18" x14ac:dyDescent="0.25">
@@ -8344,16 +8345,16 @@
         <v>132</v>
       </c>
       <c r="E67" s="13">
-        <f t="shared" si="6"/>
-        <v>1.0260899496882758</v>
+        <f t="shared" si="7"/>
+        <v>1.2928733366072276</v>
       </c>
       <c r="F67" s="13">
-        <f t="shared" si="6"/>
-        <v>0.6436607600010732</v>
+        <f t="shared" si="7"/>
+        <v>0.81101255760135227</v>
       </c>
       <c r="G67" s="13">
-        <f t="shared" si="6"/>
-        <v>0.78018271718130916</v>
+        <f t="shared" si="7"/>
+        <v>0.94914627354677161</v>
       </c>
     </row>
     <row r="68" spans="2:18" x14ac:dyDescent="0.25">
@@ -8361,16 +8362,16 @@
         <v>133</v>
       </c>
       <c r="E68" s="13">
-        <f t="shared" si="6"/>
-        <v>1.1517459811445534</v>
+        <f t="shared" si="7"/>
+        <v>1.4511999362421373</v>
       </c>
       <c r="F68" s="13">
-        <f t="shared" si="6"/>
-        <v>0.69094795692568522</v>
+        <f t="shared" si="7"/>
+        <v>0.87059442572636336</v>
       </c>
       <c r="G68" s="13">
-        <f t="shared" si="6"/>
-        <v>0.85075639453920038</v>
+        <f t="shared" si="7"/>
+        <v>1.0329375138770247</v>
       </c>
     </row>
     <row r="69" spans="2:18" x14ac:dyDescent="0.25">
@@ -8378,16 +8379,16 @@
         <v>92</v>
       </c>
       <c r="E69" s="13">
-        <f t="shared" si="6"/>
-        <v>1.5253339002283488</v>
+        <f t="shared" si="7"/>
+        <v>1.9219207142877195</v>
       </c>
       <c r="F69" s="13">
-        <f t="shared" si="6"/>
-        <v>0.80995652868383905</v>
+        <f t="shared" si="7"/>
+        <v>1.0205452261416372</v>
       </c>
       <c r="G69" s="13">
-        <f t="shared" si="6"/>
-        <v>1.0386677710449455</v>
+        <f t="shared" si="7"/>
+        <v>1.2544194101961372</v>
       </c>
     </row>
     <row r="70" spans="2:18" x14ac:dyDescent="0.25">
@@ -8395,16 +8396,16 @@
         <v>134</v>
       </c>
       <c r="E70" s="13">
-        <f t="shared" si="6"/>
-        <v>2.2576354022974559</v>
+        <f t="shared" si="7"/>
+        <v>2.8446206068947943</v>
       </c>
       <c r="F70" s="13">
-        <f t="shared" si="6"/>
-        <v>0.97849146816282084</v>
+        <f t="shared" si="7"/>
+        <v>1.2328992498851543</v>
       </c>
       <c r="G70" s="13">
-        <f t="shared" si="6"/>
-        <v>1.3331219575880786</v>
+        <f t="shared" si="7"/>
+        <v>1.5968055909534784</v>
       </c>
     </row>
     <row r="71" spans="2:18" x14ac:dyDescent="0.25">
@@ -8412,16 +8413,16 @@
         <v>93</v>
       </c>
       <c r="E71" s="13">
-        <f t="shared" si="6"/>
-        <v>4.3423797331272285</v>
+        <f t="shared" si="7"/>
+        <v>5.4713984637403081</v>
       </c>
       <c r="F71" s="13">
-        <f t="shared" si="6"/>
-        <v>1.2355922629333131</v>
+        <f t="shared" si="7"/>
+        <v>1.5568462512959746</v>
       </c>
       <c r="G71" s="13">
-        <f t="shared" si="6"/>
-        <v>1.8605825545982249</v>
+        <f t="shared" si="7"/>
+        <v>2.1962620033420355</v>
       </c>
     </row>
     <row r="72" spans="2:18" x14ac:dyDescent="0.25">
@@ -8429,16 +8430,16 @@
         <v>135</v>
       </c>
       <c r="E72" s="13">
-        <f t="shared" si="6"/>
-        <v>56.703392098299226</v>
+        <f t="shared" si="7"/>
+        <v>71.446274043857031</v>
       </c>
       <c r="F72" s="13">
-        <f t="shared" si="6"/>
-        <v>1.6759524790123197</v>
+        <f t="shared" si="7"/>
+        <v>2.1117001235555226</v>
       </c>
       <c r="G72" s="13">
-        <f t="shared" si="6"/>
-        <v>3.0786923375113076</v>
+        <f t="shared" si="7"/>
+        <v>3.5163245947436912</v>
       </c>
       <c r="R72" t="s">
         <v>167</v>
@@ -8449,16 +8450,16 @@
         <v>94</v>
       </c>
       <c r="E73" s="21">
-        <f t="shared" si="6"/>
-        <v>-5.1277524400581074</v>
+        <f t="shared" si="7"/>
+        <v>-6.4609680744732154</v>
       </c>
       <c r="F73" s="13">
-        <f t="shared" si="6"/>
-        <v>2.60401215507216</v>
+        <f t="shared" si="7"/>
+        <v>3.2810553153909217</v>
       </c>
       <c r="G73" s="13">
-        <f t="shared" si="6"/>
-        <v>8.9158039166770653</v>
+        <f t="shared" si="7"/>
+        <v>8.81394120289381</v>
       </c>
     </row>
     <row r="74" spans="2:18" x14ac:dyDescent="0.25">
@@ -8488,16 +8489,16 @@
         <v>0.5</v>
       </c>
       <c r="E77" s="13">
-        <f t="shared" ref="E77:G83" si="7">Cycle_energy__kWh/$D77</f>
-        <v>9.9</v>
+        <f t="shared" ref="E77:G83" si="8">Cycle_energy__kWh/$D77</f>
+        <v>12.474</v>
       </c>
       <c r="F77" s="13">
-        <f t="shared" si="7"/>
-        <v>9.9</v>
+        <f t="shared" si="8"/>
+        <v>12.474</v>
       </c>
       <c r="G77" s="13">
-        <f t="shared" si="7"/>
-        <v>9.9</v>
+        <f t="shared" si="8"/>
+        <v>12.474</v>
       </c>
     </row>
     <row r="78" spans="2:18" x14ac:dyDescent="0.25">
@@ -8508,16 +8509,16 @@
         <v>1</v>
       </c>
       <c r="E78" s="13">
-        <f t="shared" si="7"/>
-        <v>4.95</v>
+        <f t="shared" si="8"/>
+        <v>6.2370000000000001</v>
       </c>
       <c r="F78" s="13">
-        <f t="shared" si="7"/>
-        <v>4.95</v>
+        <f t="shared" si="8"/>
+        <v>6.2370000000000001</v>
       </c>
       <c r="G78" s="13">
-        <f t="shared" si="7"/>
-        <v>4.95</v>
+        <f t="shared" si="8"/>
+        <v>6.2370000000000001</v>
       </c>
     </row>
     <row r="79" spans="2:18" x14ac:dyDescent="0.25">
@@ -8528,16 +8529,16 @@
         <v>2</v>
       </c>
       <c r="E79" s="13">
-        <f t="shared" si="7"/>
-        <v>2.4750000000000001</v>
+        <f t="shared" si="8"/>
+        <v>3.1185</v>
       </c>
       <c r="F79" s="13">
-        <f t="shared" si="7"/>
-        <v>2.4750000000000001</v>
+        <f t="shared" si="8"/>
+        <v>3.1185</v>
       </c>
       <c r="G79" s="13">
-        <f t="shared" si="7"/>
-        <v>2.4750000000000001</v>
+        <f t="shared" si="8"/>
+        <v>3.1185</v>
       </c>
     </row>
     <row r="80" spans="2:18" x14ac:dyDescent="0.25">
@@ -8548,16 +8549,16 @@
         <v>3</v>
       </c>
       <c r="E80" s="13">
-        <f t="shared" si="7"/>
-        <v>1.6500000000000001</v>
+        <f t="shared" si="8"/>
+        <v>2.0790000000000002</v>
       </c>
       <c r="F80" s="13">
-        <f t="shared" si="7"/>
-        <v>1.6500000000000001</v>
+        <f t="shared" si="8"/>
+        <v>2.0790000000000002</v>
       </c>
       <c r="G80" s="13">
-        <f t="shared" si="7"/>
-        <v>1.6500000000000001</v>
+        <f t="shared" si="8"/>
+        <v>2.0790000000000002</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
@@ -8568,16 +8569,16 @@
         <v>4</v>
       </c>
       <c r="E81" s="13">
-        <f t="shared" si="7"/>
-        <v>1.2375</v>
+        <f t="shared" si="8"/>
+        <v>1.55925</v>
       </c>
       <c r="F81" s="13">
-        <f t="shared" si="7"/>
-        <v>1.2375</v>
+        <f t="shared" si="8"/>
+        <v>1.55925</v>
       </c>
       <c r="G81" s="13">
-        <f t="shared" si="7"/>
-        <v>1.2375</v>
+        <f t="shared" si="8"/>
+        <v>1.55925</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
@@ -8588,16 +8589,16 @@
         <v>5</v>
       </c>
       <c r="E82" s="13">
-        <f t="shared" si="7"/>
-        <v>0.99</v>
+        <f t="shared" si="8"/>
+        <v>1.2474000000000001</v>
       </c>
       <c r="F82" s="13">
-        <f t="shared" si="7"/>
-        <v>0.99</v>
+        <f t="shared" si="8"/>
+        <v>1.2474000000000001</v>
       </c>
       <c r="G82" s="13">
-        <f t="shared" si="7"/>
-        <v>0.99</v>
+        <f t="shared" si="8"/>
+        <v>1.2474000000000001</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
@@ -8608,16 +8609,16 @@
         <v>6</v>
       </c>
       <c r="E83" s="21">
-        <f t="shared" si="7"/>
-        <v>0.82500000000000007</v>
+        <f t="shared" si="8"/>
+        <v>1.0395000000000001</v>
       </c>
       <c r="F83" s="13">
-        <f t="shared" si="7"/>
-        <v>0.82500000000000007</v>
+        <f t="shared" si="8"/>
+        <v>1.0395000000000001</v>
       </c>
       <c r="G83" s="13">
-        <f t="shared" si="7"/>
-        <v>0.82500000000000007</v>
+        <f t="shared" si="8"/>
+        <v>1.0395000000000001</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
@@ -8636,16 +8637,16 @@
         <v>140</v>
       </c>
       <c r="E86" s="7">
-        <f t="shared" ref="E86:G92" si="8">E67+E77</f>
-        <v>10.926089949688276</v>
+        <f t="shared" ref="E86:G92" si="9">E67+E77</f>
+        <v>13.766873336607228</v>
       </c>
       <c r="F86" s="7">
-        <f t="shared" si="8"/>
-        <v>10.543660760001073</v>
+        <f t="shared" si="9"/>
+        <v>13.285012557601352</v>
       </c>
       <c r="G86" s="7">
-        <f t="shared" si="8"/>
-        <v>10.68018271718131</v>
+        <f t="shared" si="9"/>
+        <v>13.423146273546772</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
@@ -8653,16 +8654,16 @@
         <v>141</v>
       </c>
       <c r="E87" s="7">
-        <f t="shared" si="8"/>
-        <v>6.1017459811445534</v>
+        <f t="shared" si="9"/>
+        <v>7.6881999362421372</v>
       </c>
       <c r="F87" s="7">
-        <f t="shared" si="8"/>
-        <v>5.6409479569256851</v>
+        <f t="shared" si="9"/>
+        <v>7.1075944257263632</v>
       </c>
       <c r="G87" s="7">
-        <f t="shared" si="8"/>
-        <v>5.8007563945392002</v>
+        <f t="shared" si="9"/>
+        <v>7.269937513877025</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
@@ -8670,16 +8671,16 @@
         <v>103</v>
       </c>
       <c r="E88" s="7">
-        <f t="shared" si="8"/>
-        <v>4.0003339002283491</v>
+        <f t="shared" si="9"/>
+        <v>5.0404207142877198</v>
       </c>
       <c r="F88" s="7">
-        <f t="shared" si="8"/>
-        <v>3.2849565286838391</v>
+        <f t="shared" si="9"/>
+        <v>4.1390452261416373</v>
       </c>
       <c r="G88" s="7">
-        <f t="shared" si="8"/>
-        <v>3.5136677710449455</v>
+        <f t="shared" si="9"/>
+        <v>4.3729194101961371</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
@@ -8687,16 +8688,16 @@
         <v>142</v>
       </c>
       <c r="E89" s="7">
-        <f t="shared" si="8"/>
-        <v>3.9076354022974558</v>
+        <f t="shared" si="9"/>
+        <v>4.9236206068947945</v>
       </c>
       <c r="F89" s="7">
-        <f t="shared" si="8"/>
-        <v>2.6284914681628209</v>
+        <f t="shared" si="9"/>
+        <v>3.3118992498851547</v>
       </c>
       <c r="G89" s="7">
-        <f t="shared" si="8"/>
-        <v>2.9831219575880787</v>
+        <f t="shared" si="9"/>
+        <v>3.6758055909534786</v>
       </c>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
@@ -8704,16 +8705,16 @@
         <v>104</v>
       </c>
       <c r="E90" s="7">
-        <f t="shared" si="8"/>
-        <v>5.5798797331272283</v>
+        <f t="shared" si="9"/>
+        <v>7.0306484637403077</v>
       </c>
       <c r="F90" s="7">
-        <f t="shared" si="8"/>
-        <v>2.4730922629333132</v>
+        <f t="shared" si="9"/>
+        <v>3.1160962512959749</v>
       </c>
       <c r="G90" s="7">
-        <f t="shared" si="8"/>
-        <v>3.0980825545982249</v>
+        <f t="shared" si="9"/>
+        <v>3.7555120033420355</v>
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
@@ -8721,16 +8722,16 @@
         <v>143</v>
       </c>
       <c r="E91" s="7">
-        <f t="shared" si="8"/>
-        <v>57.693392098299228</v>
+        <f t="shared" si="9"/>
+        <v>72.69367404385703</v>
       </c>
       <c r="F91" s="7">
-        <f t="shared" si="8"/>
-        <v>2.6659524790123195</v>
+        <f t="shared" si="9"/>
+        <v>3.3591001235555229</v>
       </c>
       <c r="G91" s="7">
-        <f t="shared" si="8"/>
-        <v>4.0686923375113073</v>
+        <f t="shared" si="9"/>
+        <v>4.7637245947436915</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
@@ -8738,16 +8739,16 @@
         <v>105</v>
       </c>
       <c r="E92" s="31">
-        <f t="shared" si="8"/>
-        <v>-4.3027524400581072</v>
+        <f t="shared" si="9"/>
+        <v>-5.4214680744732151</v>
       </c>
       <c r="F92" s="7">
-        <f t="shared" si="8"/>
-        <v>3.4290121550721602</v>
+        <f t="shared" si="9"/>
+        <v>4.320555315390922</v>
       </c>
       <c r="G92" s="7">
-        <f t="shared" si="8"/>
-        <v>9.7408039166770646</v>
+        <f t="shared" si="9"/>
+        <v>9.8534412028938103</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
@@ -8763,16 +8764,16 @@
         <v>144</v>
       </c>
       <c r="E95" s="7">
-        <f t="shared" ref="E95:G100" si="9">E67/E86</f>
+        <f t="shared" ref="E95:G100" si="10">E67/E86</f>
         <v>9.3911907591201049E-2</v>
       </c>
       <c r="F95" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.1047180353420979E-2</v>
       </c>
       <c r="G95" s="7">
-        <f t="shared" si="9"/>
-        <v>7.3049566457905432E-2</v>
+        <f t="shared" si="10"/>
+        <v>7.0709672248545088E-2</v>
       </c>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.25">
@@ -8780,16 +8781,16 @@
         <v>145</v>
       </c>
       <c r="E96" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.18875678940153309</v>
       </c>
       <c r="F96" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1224879155421692</v>
       </c>
       <c r="G96" s="7">
-        <f t="shared" si="9"/>
-        <v>0.14666301024812864</v>
+        <f t="shared" si="10"/>
+        <v>0.14208341019511236</v>
       </c>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.25">
@@ -8797,16 +8798,16 @@
         <v>107</v>
       </c>
       <c r="E97" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.38130164588042986</v>
       </c>
       <c r="F97" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.24656537205634158</v>
       </c>
       <c r="G97" s="7">
-        <f t="shared" si="9"/>
-        <v>0.29560784875687074</v>
+        <f t="shared" si="10"/>
+        <v>0.28686085713614218</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
@@ -8814,16 +8815,16 @@
         <v>146</v>
       </c>
       <c r="E98" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.57774975653309446</v>
       </c>
       <c r="F98" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.37226351312706962</v>
       </c>
       <c r="G98" s="7">
-        <f t="shared" si="9"/>
-        <v>0.44688818510991679</v>
+        <f t="shared" si="10"/>
+        <v>0.4344096964440598</v>
       </c>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.25">
@@ -8832,16 +8833,16 @@
       </c>
       <c r="D99" s="20"/>
       <c r="E99" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.77822102640437263</v>
       </c>
       <c r="F99" s="7">
-        <f t="shared" si="9"/>
-        <v>0.49961430127470779</v>
+        <f t="shared" si="10"/>
+        <v>0.49961430127470774</v>
       </c>
       <c r="G99" s="7">
-        <f t="shared" si="9"/>
-        <v>0.60055938530001973</v>
+        <f t="shared" si="10"/>
+        <v>0.58481027390874496</v>
       </c>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
@@ -8850,16 +8851,16 @@
       </c>
       <c r="D100" s="20"/>
       <c r="E100" s="7">
-        <f t="shared" si="9"/>
-        <v>0.98284032253965548</v>
+        <f t="shared" si="10"/>
+        <v>0.98284032253965559</v>
       </c>
       <c r="F100" s="7">
-        <f t="shared" si="9"/>
-        <v>0.62865054505143525</v>
+        <f t="shared" si="10"/>
+        <v>0.62865054505143514</v>
       </c>
       <c r="G100" s="7">
-        <f t="shared" si="9"/>
-        <v>0.75667857928880611</v>
+        <f t="shared" si="10"/>
+        <v>0.73814607137944432</v>
       </c>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.25">
@@ -8876,7 +8877,7 @@
       </c>
       <c r="G101" s="7">
         <f>G73/G92</f>
-        <v>0.9153047318212072</v>
+        <v>0.89450386128099957</v>
       </c>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.25">
@@ -8907,16 +8908,16 @@
         <v>0.5</v>
       </c>
       <c r="E105" s="24">
-        <f t="shared" ref="E105:G110" si="10">Engine_spec_d_life__h/Hours_in_a_year__h/E95</f>
+        <f t="shared" ref="E105:G110" si="11">Engine_spec_d_life__h/Hours_in_a_year__h/E95</f>
         <v>24.311134566336534</v>
       </c>
       <c r="F105" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>37.399024977295433</v>
       </c>
       <c r="G105" s="24">
-        <f t="shared" si="10"/>
-        <v>31.254189908802292</v>
+        <f t="shared" si="11"/>
+        <v>32.288440184051723</v>
       </c>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.25">
@@ -8927,16 +8928,16 @@
         <v>1</v>
       </c>
       <c r="E106" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12.095485572041135</v>
       </c>
       <c r="F106" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>18.639430777520584</v>
       </c>
       <c r="G106" s="24">
-        <f t="shared" si="10"/>
-        <v>15.56701324327401</v>
+        <f t="shared" si="11"/>
+        <v>16.068765661633794</v>
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
@@ -8947,16 +8948,16 @@
         <v>2</v>
       </c>
       <c r="E107" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.9876610748934347</v>
       </c>
       <c r="F107" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.2596336776331594</v>
       </c>
       <c r="G107" s="15">
-        <f t="shared" si="10"/>
-        <v>7.7234249105098725</v>
+        <f t="shared" si="11"/>
+        <v>7.9589284004248251</v>
       </c>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
@@ -8967,16 +8968,16 @@
         <v>3</v>
       </c>
       <c r="E108" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.951719575844201</v>
       </c>
       <c r="F108" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.1330346443373509</v>
       </c>
       <c r="G108" s="15">
-        <f t="shared" si="10"/>
-        <v>5.1088954662551593</v>
+        <f t="shared" si="11"/>
+        <v>5.2556493133551694</v>
       </c>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.25">
@@ -8987,16 +8988,16 @@
         <v>4</v>
       </c>
       <c r="E109" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.9337488263195843</v>
       </c>
       <c r="F109" s="15">
-        <f t="shared" si="10"/>
-        <v>4.5697351276894462</v>
+        <f t="shared" si="11"/>
+        <v>4.5697351276894471</v>
       </c>
       <c r="G109" s="15">
-        <f t="shared" si="10"/>
-        <v>3.8016307441278037</v>
+        <f t="shared" si="11"/>
+        <v>3.9040097698203415</v>
       </c>
     </row>
     <row r="110" spans="3:7" x14ac:dyDescent="0.25">
@@ -9007,16 +9008,16 @@
         <v>5</v>
       </c>
       <c r="E110" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.3229663766048141</v>
       </c>
       <c r="F110" s="15">
-        <f t="shared" si="10"/>
-        <v>3.6317554177007039</v>
+        <f t="shared" si="11"/>
+        <v>3.6317554177007043</v>
       </c>
       <c r="G110" s="15">
-        <f t="shared" si="10"/>
-        <v>3.017271910851389</v>
+        <f t="shared" si="11"/>
+        <v>3.0930260436994446</v>
       </c>
     </row>
     <row r="111" spans="3:7" x14ac:dyDescent="0.25">
@@ -9035,7 +9036,7 @@
       </c>
       <c r="G111" s="15">
         <f>Engine_spec_d_life__h/Hours_in_a_year__h/G101</f>
-        <v>2.4943660220004467</v>
+        <v>2.5523702262855132</v>
       </c>
     </row>
     <row r="112" spans="3:7" x14ac:dyDescent="0.25">
@@ -9064,16 +9065,16 @@
         <v>0.5</v>
       </c>
       <c r="E114" s="24">
-        <f t="shared" ref="E114:G119" si="11">Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E86)</f>
-        <v>12.47270542201858</v>
+        <f t="shared" ref="E114:G119" si="12">Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/E86)</f>
+        <v>15.71560883174341</v>
       </c>
       <c r="F114" s="24">
-        <f t="shared" si="11"/>
-        <v>12.036142420092549</v>
+        <f t="shared" si="12"/>
+        <v>15.165539449316613</v>
       </c>
       <c r="G114" s="24">
-        <f t="shared" si="11"/>
-        <v>12.191989403175011</v>
+        <f t="shared" si="12"/>
+        <v>15.323226339665265</v>
       </c>
     </row>
     <row r="115" spans="3:7" x14ac:dyDescent="0.25">
@@ -9084,16 +9085,16 @@
         <v>1</v>
       </c>
       <c r="E115" s="24">
-        <f t="shared" si="11"/>
-        <v>6.9654634487951519</v>
+        <f t="shared" si="12"/>
+        <v>8.7764839454818908</v>
       </c>
       <c r="F115" s="24">
-        <f t="shared" si="11"/>
-        <v>6.4394383069927912</v>
+        <f t="shared" si="12"/>
+        <v>8.1136922668109168</v>
       </c>
       <c r="G115" s="24">
-        <f t="shared" si="11"/>
-        <v>6.6218680302958912</v>
+        <f t="shared" si="12"/>
+        <v>8.2990154268002563</v>
       </c>
     </row>
     <row r="116" spans="3:7" x14ac:dyDescent="0.25">
@@ -9104,16 +9105,16 @@
         <v>2</v>
       </c>
       <c r="E116" s="15">
-        <f t="shared" si="11"/>
-        <v>4.5665912103063349</v>
+        <f t="shared" si="12"/>
+        <v>5.7539049249859815</v>
       </c>
       <c r="F116" s="15">
-        <f t="shared" si="11"/>
-        <v>3.749950375209862</v>
+        <f t="shared" si="12"/>
+        <v>4.7249374727644256</v>
       </c>
       <c r="G116" s="15">
-        <f t="shared" si="11"/>
-        <v>4.0110362683161478</v>
+        <f t="shared" si="12"/>
+        <v>4.991917134927097</v>
       </c>
     </row>
     <row r="117" spans="3:7" x14ac:dyDescent="0.25">
@@ -9124,16 +9125,16 @@
         <v>3</v>
       </c>
       <c r="E117" s="15">
-        <f t="shared" si="11"/>
-        <v>4.4607710071888764</v>
+        <f t="shared" si="12"/>
+        <v>5.6205714690579844</v>
       </c>
       <c r="F117" s="15">
-        <f t="shared" si="11"/>
-        <v>3.0005610367155491</v>
+        <f t="shared" si="12"/>
+        <v>3.7807069062615923</v>
       </c>
       <c r="G117" s="15">
-        <f t="shared" si="11"/>
-        <v>3.4053903625434692</v>
+        <f t="shared" si="12"/>
+        <v>4.1961251038281713</v>
       </c>
     </row>
     <row r="118" spans="3:7" x14ac:dyDescent="0.25">
@@ -9144,16 +9145,16 @@
         <v>4</v>
       </c>
       <c r="E118" s="15">
-        <f t="shared" si="11"/>
-        <v>6.3697257227479769</v>
+        <f t="shared" si="12"/>
+        <v>8.0258544106624523</v>
       </c>
       <c r="F118" s="15">
-        <f t="shared" si="11"/>
-        <v>2.8231646837138276</v>
+        <f t="shared" si="12"/>
+        <v>3.5571875014794236</v>
       </c>
       <c r="G118" s="15">
-        <f t="shared" si="11"/>
-        <v>3.5366239207742294</v>
+        <f t="shared" si="12"/>
+        <v>4.2871141590662507</v>
       </c>
     </row>
     <row r="119" spans="3:7" x14ac:dyDescent="0.25">
@@ -9164,16 +9165,16 @@
         <v>5</v>
       </c>
       <c r="E119" s="15">
-        <f t="shared" si="11"/>
-        <v>65.860036641894098</v>
+        <f t="shared" si="12"/>
+        <v>82.983646168786564</v>
       </c>
       <c r="F119" s="15">
-        <f t="shared" si="11"/>
-        <v>3.0433247477309586</v>
+        <f t="shared" si="12"/>
+        <v>3.8345891821410083</v>
       </c>
       <c r="G119" s="15">
-        <f t="shared" si="11"/>
-        <v>4.6446259560631358</v>
+        <f t="shared" si="12"/>
+        <v>5.4380417748215653</v>
       </c>
     </row>
     <row r="120" spans="3:7" x14ac:dyDescent="0.25">
@@ -9188,11 +9189,11 @@
       </c>
       <c r="F120" s="15">
         <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/F92)</f>
-        <v>3.9143974372969867</v>
+        <v>4.9321407709942031</v>
       </c>
       <c r="G120" s="15">
         <f>Batt_Cycles_50__DOD__guesstimated/(Hours_in_a_year__h/G92)</f>
-        <v>11.119639174288887</v>
+        <v>11.248220551248643</v>
       </c>
     </row>
     <row r="122" spans="3:7" x14ac:dyDescent="0.25">
@@ -9214,16 +9215,16 @@
         <v>0.5</v>
       </c>
       <c r="E123" s="24">
-        <f t="shared" ref="E123:G128" si="12">(Engine_service_interval__h/E95)/24</f>
+        <f t="shared" ref="E123:G128" si="13">(Engine_service_interval__h/E95)/24</f>
         <v>443.67820583564179</v>
       </c>
       <c r="F123" s="24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>682.53220583564166</v>
       </c>
       <c r="G123" s="24">
-        <f t="shared" si="12"/>
-        <v>570.38896583564178</v>
+        <f t="shared" si="13"/>
+        <v>589.26403335894395</v>
       </c>
     </row>
     <row r="124" spans="3:7" x14ac:dyDescent="0.25">
@@ -9234,16 +9235,16 @@
         <v>1</v>
       </c>
       <c r="E124" s="24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>220.74261168975067</v>
       </c>
       <c r="F124" s="24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>340.16961168975064</v>
       </c>
       <c r="G124" s="24">
-        <f t="shared" si="12"/>
-        <v>284.0979916897507</v>
+        <f t="shared" si="13"/>
+        <v>293.25497332481672</v>
       </c>
     </row>
     <row r="125" spans="3:7" x14ac:dyDescent="0.25">
@@ -9254,16 +9255,16 @@
         <v>2</v>
       </c>
       <c r="E125" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>109.27481461680516</v>
       </c>
       <c r="F125" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>168.98831461680516</v>
       </c>
       <c r="G125" s="7">
-        <f t="shared" si="12"/>
-        <v>140.95250461680516</v>
+        <f t="shared" si="13"/>
+        <v>145.25044330775305</v>
       </c>
     </row>
     <row r="126" spans="3:7" x14ac:dyDescent="0.25">
@@ -9274,16 +9275,16 @@
         <v>3</v>
       </c>
       <c r="E126" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>72.118882259156663</v>
       </c>
       <c r="F126" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>111.92788225915666</v>
       </c>
       <c r="G126" s="7">
-        <f t="shared" si="12"/>
-        <v>93.237342259156662</v>
+        <f t="shared" si="13"/>
+        <v>95.91559996873184</v>
       </c>
     </row>
     <row r="127" spans="3:7" x14ac:dyDescent="0.25">
@@ -9294,16 +9295,16 @@
         <v>4</v>
       </c>
       <c r="E127" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>53.540916080332408</v>
       </c>
       <c r="F127" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>83.397666080332399</v>
       </c>
       <c r="G127" s="7">
-        <f t="shared" si="12"/>
-        <v>69.379761080332415</v>
+        <f t="shared" si="13"/>
+        <v>71.248178299221237</v>
       </c>
     </row>
     <row r="128" spans="3:7" x14ac:dyDescent="0.25">
@@ -9314,16 +9315,16 @@
         <v>5</v>
       </c>
       <c r="E128" s="7">
-        <f t="shared" si="12"/>
-        <v>42.39413637303786</v>
+        <f t="shared" si="13"/>
+        <v>42.394136373037853</v>
       </c>
       <c r="F128" s="7">
-        <f t="shared" si="12"/>
-        <v>66.279536373037843</v>
+        <f t="shared" si="13"/>
+        <v>66.279536373037857</v>
       </c>
       <c r="G128" s="7">
-        <f t="shared" si="12"/>
-        <v>55.065212373037845</v>
+        <f t="shared" si="13"/>
+        <v>56.447725297514857</v>
       </c>
     </row>
     <row r="129" spans="3:7" x14ac:dyDescent="0.25">
@@ -9342,7 +9343,7 @@
       </c>
       <c r="G129" s="7">
         <f>(Engine_service_interval__h/G101)/24</f>
-        <v>45.522179901508146</v>
+        <v>46.580756629710613</v>
       </c>
     </row>
   </sheetData>
@@ -9357,7 +9358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U136"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E7" workbookViewId="0">
       <selection activeCell="F13" sqref="F13:J31"/>
     </sheetView>
   </sheetViews>
@@ -12288,7 +12289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B28:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added LTO design tab to BMs Hygen System Design Calcs.xlsx. Some preliminary calculations for a HyGen based on Toshiba LTO battery modules.
</commit_message>
<xml_diff>
--- a/Control and Data Systems/BMs Hygen System Design Calcs.xlsx
+++ b/Control and Data Systems/BMs Hygen System Design Calcs.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="15315" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="15315" windowHeight="12075" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Beckett Battery Modules" sheetId="1" r:id="rId1"/>
     <sheet name="Hygen Use Models" sheetId="2" r:id="rId2"/>
     <sheet name="5 year life projections" sheetId="4" r:id="rId3"/>
     <sheet name="Boston Power Life" sheetId="5" r:id="rId4"/>
+    <sheet name="LTO comparison" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="AC_accessory_load__kW">'5 year life projections'!$E$50</definedName>
@@ -78,12 +79,11 @@
     <definedName name="Voltage_at_80">'Beckett Battery Modules'!$C$13</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="219">
   <si>
     <t>Boston Swing 5300</t>
   </si>
@@ -659,6 +659,90 @@
   </si>
   <si>
     <t>BK calculated this efficiency from our first 4kW Charge/Discharge cycle test.</t>
+  </si>
+  <si>
+    <t>Toshiba LTO Design</t>
+  </si>
+  <si>
+    <t>Voltage, nominal</t>
+  </si>
+  <si>
+    <t>Nominal capacity, Ah, 100% DOD</t>
+  </si>
+  <si>
+    <t>Dimensions, mm</t>
+  </si>
+  <si>
+    <t>Voltage, operating max</t>
+  </si>
+  <si>
+    <t>Voltage, operating min</t>
+  </si>
+  <si>
+    <t>Max charge rate, A</t>
+  </si>
+  <si>
+    <t>Cycle life, 80% DOD</t>
+  </si>
+  <si>
+    <t>Stack height, modules</t>
+  </si>
+  <si>
+    <t>Charge peak voltage</t>
+  </si>
+  <si>
+    <t>Discharge minimum voltage</t>
+  </si>
+  <si>
+    <t>Enatel minimum voltage range</t>
+  </si>
+  <si>
+    <t>Vicor minimum voltage range</t>
+  </si>
+  <si>
+    <t>Weight, kg</t>
+  </si>
+  <si>
+    <t>Nominal total energy/module,  Wh</t>
+  </si>
+  <si>
+    <t>Nominal total energy/stack, Wh</t>
+  </si>
+  <si>
+    <t>stack mass, kg</t>
+  </si>
+  <si>
+    <t>stack volume, m^3</t>
+  </si>
+  <si>
+    <t>Beckett
+8224S</t>
+  </si>
+  <si>
+    <t>Toshiba
+SCiB 2P12S</t>
+  </si>
+  <si>
+    <t>Est cycle life, 50% DOD</t>
+  </si>
+  <si>
+    <t>Cycle energy, Wh</t>
+  </si>
+  <si>
+    <t>Designed DoD, fraction</t>
+  </si>
+  <si>
+    <t>Lifetime energy delivered, kWh</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Toshiba
+SCiB 1P12S</t>
+  </si>
+  <si>
+    <t>Exists?</t>
   </si>
 </sst>
 </file>
@@ -668,7 +752,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -695,6 +779,13 @@
       <b/>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -751,7 +842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -884,6 +975,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,11 +1198,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121258368"/>
-        <c:axId val="121261440"/>
+        <c:axId val="187133952"/>
+        <c:axId val="187135872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121258368"/>
+        <c:axId val="187133952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,19 +1225,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121261440"/>
+        <c:crossAx val="187135872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121261440"/>
+        <c:axId val="187135872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -1169,14 +1260,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121258368"/>
+        <c:crossAx val="187133952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -1184,7 +1274,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1531,11 +1620,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="170325120"/>
-        <c:axId val="170327424"/>
+        <c:axId val="187925632"/>
+        <c:axId val="187927936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="170325120"/>
+        <c:axId val="187925632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1577,12 +1666,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170327424"/>
+        <c:crossAx val="187927936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170327424"/>
+        <c:axId val="187927936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1618,7 +1707,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170325120"/>
+        <c:crossAx val="187925632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -2054,11 +2143,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="171512576"/>
-        <c:axId val="171514112"/>
+        <c:axId val="187569280"/>
+        <c:axId val="187993472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="171512576"/>
+        <c:axId val="187569280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2069,13 +2158,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171514112"/>
+        <c:crossAx val="187993472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="171514112"/>
+        <c:axId val="187993472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2088,7 +2177,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171512576"/>
+        <c:crossAx val="187569280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2140,7 +2229,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2249,8 +2337,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="190689280"/>
-        <c:axId val="190691200"/>
+        <c:axId val="187163008"/>
+        <c:axId val="187164928"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2342,11 +2430,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169027840"/>
-        <c:axId val="169025920"/>
+        <c:axId val="182982912"/>
+        <c:axId val="182980992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="190689280"/>
+        <c:axId val="187163008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2369,19 +2457,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190691200"/>
+        <c:crossAx val="187164928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="190691200"/>
+        <c:axId val="187164928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2404,19 +2491,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190689280"/>
+        <c:crossAx val="187163008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169025920"/>
+        <c:axId val="182980992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="270"/>
@@ -2440,20 +2526,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169027840"/>
+        <c:crossAx val="182982912"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169027840"/>
+        <c:axId val="182982912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2463,7 +2548,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169025920"/>
+        <c:crossAx val="182980992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2476,7 +2561,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2605,8 +2689,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169043072"/>
-        <c:axId val="169044992"/>
+        <c:axId val="183022720"/>
+        <c:axId val="183024640"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2729,11 +2813,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169053184"/>
-        <c:axId val="169051264"/>
+        <c:axId val="183032832"/>
+        <c:axId val="183030912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169043072"/>
+        <c:axId val="183022720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -2763,13 +2847,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169044992"/>
+        <c:crossAx val="183024640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169044992"/>
+        <c:axId val="183024640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2798,12 +2882,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169043072"/>
+        <c:crossAx val="183022720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169051264"/>
+        <c:axId val="183030912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="540"/>
@@ -2833,13 +2917,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169053184"/>
+        <c:crossAx val="183032832"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169053184"/>
+        <c:axId val="183032832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2849,7 +2933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169051264"/>
+        <c:crossAx val="183030912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3028,11 +3112,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169152512"/>
-        <c:axId val="169154432"/>
+        <c:axId val="187170816"/>
+        <c:axId val="187172736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169152512"/>
+        <c:axId val="187170816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -3062,13 +3146,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169154432"/>
+        <c:crossAx val="187172736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169154432"/>
+        <c:axId val="187172736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3097,7 +3181,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169152512"/>
+        <c:crossAx val="187170816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3786,11 +3870,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169245696"/>
-        <c:axId val="169248256"/>
+        <c:axId val="186104832"/>
+        <c:axId val="186107392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169245696"/>
+        <c:axId val="186104832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3832,12 +3916,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169248256"/>
+        <c:crossAx val="186107392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169248256"/>
+        <c:axId val="186107392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -3873,7 +3957,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169245696"/>
+        <c:crossAx val="186104832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -4034,8 +4118,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169267584"/>
-        <c:axId val="169269504"/>
+        <c:axId val="186161024"/>
+        <c:axId val="186167296"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -4127,11 +4211,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169273600"/>
-        <c:axId val="169271680"/>
+        <c:axId val="186183680"/>
+        <c:axId val="186169216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169267584"/>
+        <c:axId val="186161024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4160,12 +4244,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169269504"/>
+        <c:crossAx val="186167296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169269504"/>
+        <c:axId val="186167296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4194,12 +4278,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169267584"/>
+        <c:crossAx val="186161024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169271680"/>
+        <c:axId val="186169216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="270"/>
@@ -4229,13 +4313,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169273600"/>
+        <c:crossAx val="186183680"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169273600"/>
+        <c:axId val="186183680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4245,7 +4329,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169271680"/>
+        <c:crossAx val="186169216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4386,8 +4470,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169583744"/>
-        <c:axId val="169585664"/>
+        <c:axId val="186198656"/>
+        <c:axId val="186200832"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -4510,11 +4594,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169597952"/>
-        <c:axId val="169596032"/>
+        <c:axId val="186221312"/>
+        <c:axId val="186202752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169583744"/>
+        <c:axId val="186198656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -4544,13 +4628,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169585664"/>
+        <c:crossAx val="186200832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169585664"/>
+        <c:axId val="186200832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4579,12 +4663,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169583744"/>
+        <c:crossAx val="186198656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169596032"/>
+        <c:axId val="186202752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="540"/>
@@ -4614,13 +4698,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169597952"/>
+        <c:crossAx val="186221312"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169597952"/>
+        <c:axId val="186221312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4630,7 +4714,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169596032"/>
+        <c:crossAx val="186202752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4809,11 +4893,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169794560"/>
-        <c:axId val="169800832"/>
+        <c:axId val="186242176"/>
+        <c:axId val="186244096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169794560"/>
+        <c:axId val="186242176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -4843,13 +4927,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169800832"/>
+        <c:crossAx val="186244096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169800832"/>
+        <c:axId val="186244096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4878,7 +4962,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169794560"/>
+        <c:crossAx val="186242176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5308,11 +5392,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="170274176"/>
-        <c:axId val="170284928"/>
+        <c:axId val="186293632"/>
+        <c:axId val="186304384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="170274176"/>
+        <c:axId val="186293632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5354,12 +5438,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170284928"/>
+        <c:crossAx val="186304384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170284928"/>
+        <c:axId val="186304384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -5395,7 +5479,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170274176"/>
+        <c:crossAx val="186293632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -7307,7 +7391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
@@ -12519,4 +12603,423 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="54">
+        <v>42643</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="56" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E4" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5">
+        <v>24</v>
+      </c>
+      <c r="F5">
+        <v>27.6</v>
+      </c>
+      <c r="I5">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6">
+        <v>28.7</v>
+      </c>
+      <c r="F6">
+        <v>32.4</v>
+      </c>
+      <c r="I6">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7">
+        <v>21</v>
+      </c>
+      <c r="F7">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8">
+        <v>42.4</v>
+      </c>
+      <c r="F8">
+        <v>40</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>195</v>
+      </c>
+      <c r="E9">
+        <v>600</v>
+      </c>
+      <c r="F9">
+        <v>359</v>
+      </c>
+      <c r="I9">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>195</v>
+      </c>
+      <c r="E10">
+        <v>210</v>
+      </c>
+      <c r="F10">
+        <v>187</v>
+      </c>
+      <c r="I10">
+        <f>F10/2</f>
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E11">
+        <v>56</v>
+      </c>
+      <c r="F11">
+        <v>123</v>
+      </c>
+      <c r="I11">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>205</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>14</v>
+      </c>
+      <c r="I12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E13">
+        <v>21.2</v>
+      </c>
+      <c r="F13">
+        <v>120</v>
+      </c>
+      <c r="I13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>199</v>
+      </c>
+      <c r="E14">
+        <v>3000</v>
+      </c>
+      <c r="F14">
+        <v>15000</v>
+      </c>
+      <c r="I14">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17">
+        <v>11</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E18">
+        <v>308</v>
+      </c>
+      <c r="F18">
+        <f>F17*F6</f>
+        <v>324</v>
+      </c>
+      <c r="I18">
+        <f>I17*I6</f>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19">
+        <v>262</v>
+      </c>
+      <c r="F19">
+        <f>F17*F7</f>
+        <v>180</v>
+      </c>
+      <c r="I19">
+        <f>I17*I7</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>203</v>
+      </c>
+      <c r="E21">
+        <v>200</v>
+      </c>
+      <c r="F21">
+        <v>360</v>
+      </c>
+      <c r="I21">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>204</v>
+      </c>
+      <c r="E22">
+        <v>180</v>
+      </c>
+      <c r="F22">
+        <v>375</v>
+      </c>
+      <c r="I22">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>206</v>
+      </c>
+      <c r="E24">
+        <f>E8*E5</f>
+        <v>1017.5999999999999</v>
+      </c>
+      <c r="F24">
+        <f>F8*F5</f>
+        <v>1104</v>
+      </c>
+      <c r="I24">
+        <f>I8*I5</f>
+        <v>552</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>207</v>
+      </c>
+      <c r="E25">
+        <f>E17*E24</f>
+        <v>11193.599999999999</v>
+      </c>
+      <c r="F25">
+        <f>F17*F24</f>
+        <v>11040</v>
+      </c>
+      <c r="I25">
+        <f>I17*I24</f>
+        <v>5520</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>214</v>
+      </c>
+      <c r="E26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F26">
+        <v>0.8</v>
+      </c>
+      <c r="I26">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>213</v>
+      </c>
+      <c r="E27">
+        <f>E26*E25</f>
+        <v>6156.48</v>
+      </c>
+      <c r="F27">
+        <f>F26*F25</f>
+        <v>8832</v>
+      </c>
+      <c r="I27">
+        <f>I26*I25</f>
+        <v>4416</v>
+      </c>
+      <c r="J27" s="3">
+        <f>I27/E27</f>
+        <v>0.71729299859660067</v>
+      </c>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>215</v>
+      </c>
+      <c r="E28">
+        <f>E27*E15*0.9/1000</f>
+        <v>55408.319999999992</v>
+      </c>
+      <c r="F28">
+        <f>F27*F14*0.9/1000</f>
+        <v>119232</v>
+      </c>
+      <c r="G28" s="3">
+        <f>F28/E28</f>
+        <v>2.1518789957898021</v>
+      </c>
+      <c r="I28">
+        <f>I27*I14*0.9/1000</f>
+        <v>59616</v>
+      </c>
+      <c r="J28" s="3">
+        <f>I28/E28</f>
+        <v>1.0759394978949011</v>
+      </c>
+    </row>
+    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>208</v>
+      </c>
+      <c r="E30">
+        <f>E17*E12</f>
+        <v>88</v>
+      </c>
+      <c r="F30">
+        <f>F17*F12</f>
+        <v>140</v>
+      </c>
+      <c r="G30" s="3">
+        <f>F30/E30</f>
+        <v>1.5909090909090908</v>
+      </c>
+      <c r="I30">
+        <f>I17*I12</f>
+        <v>70</v>
+      </c>
+      <c r="J30" s="3">
+        <f>I30/E30</f>
+        <v>0.79545454545454541</v>
+      </c>
+    </row>
+    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>209</v>
+      </c>
+      <c r="E31">
+        <f>E17*E9*E10*E11/(1000^3)</f>
+        <v>7.7616000000000004E-2</v>
+      </c>
+      <c r="F31">
+        <f>F17*F9*F10*F11/(1000^3)</f>
+        <v>8.2573590000000002E-2</v>
+      </c>
+      <c r="G31" s="3">
+        <f>F31/E31</f>
+        <v>1.063873299319728</v>
+      </c>
+      <c r="I31">
+        <f>I17*I9*I10*I11/(1000^3)</f>
+        <v>4.1286795000000001E-2</v>
+      </c>
+      <c r="J31" s="3">
+        <f>I31/E31</f>
+        <v>0.53193664965986398</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Minor tweaks to LTO tab.  This is the version I sent to Kurt on 10/4/2016.
</commit_message>
<xml_diff>
--- a/Control and Data Systems/BMs Hygen System Design Calcs.xlsx
+++ b/Control and Data Systems/BMs Hygen System Design Calcs.xlsx
@@ -742,7 +742,7 @@
 SCiB 1P12S</t>
   </si>
   <si>
-    <t>Exists?</t>
+    <t>Does Toshiba offer this module?</t>
   </si>
 </sst>
 </file>
@@ -975,7 +975,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,11 +1200,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="187133952"/>
-        <c:axId val="187135872"/>
+        <c:axId val="167997824"/>
+        <c:axId val="167999744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="187133952"/>
+        <c:axId val="167997824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,12 +1233,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187135872"/>
+        <c:crossAx val="167999744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="187135872"/>
+        <c:axId val="167999744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -1266,7 +1268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187133952"/>
+        <c:crossAx val="167997824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -1620,11 +1622,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="187925632"/>
-        <c:axId val="187927936"/>
+        <c:axId val="169581952"/>
+        <c:axId val="169588608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="187925632"/>
+        <c:axId val="169581952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1666,12 +1668,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187927936"/>
+        <c:crossAx val="169588608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="187927936"/>
+        <c:axId val="169588608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1707,7 +1709,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187925632"/>
+        <c:crossAx val="169581952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -2143,11 +2145,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="187569280"/>
-        <c:axId val="187993472"/>
+        <c:axId val="171899904"/>
+        <c:axId val="171516672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="187569280"/>
+        <c:axId val="171899904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,13 +2160,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187993472"/>
+        <c:crossAx val="171516672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="187993472"/>
+        <c:axId val="171516672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2177,13 +2179,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187569280"/>
+        <c:crossAx val="171899904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2337,8 +2340,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="187163008"/>
-        <c:axId val="187164928"/>
+        <c:axId val="168137472"/>
+        <c:axId val="168139392"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2430,11 +2433,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="182982912"/>
-        <c:axId val="182980992"/>
+        <c:axId val="168147584"/>
+        <c:axId val="168145664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="187163008"/>
+        <c:axId val="168137472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2463,12 +2466,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187164928"/>
+        <c:crossAx val="168139392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="187164928"/>
+        <c:axId val="168139392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,12 +2500,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187163008"/>
+        <c:crossAx val="168137472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="182980992"/>
+        <c:axId val="168145664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="270"/>
@@ -2532,13 +2535,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182982912"/>
+        <c:crossAx val="168147584"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="182982912"/>
+        <c:axId val="168147584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2548,7 +2551,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182980992"/>
+        <c:crossAx val="168145664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2689,8 +2692,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="183022720"/>
-        <c:axId val="183024640"/>
+        <c:axId val="171206144"/>
+        <c:axId val="171208064"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2813,11 +2816,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="183032832"/>
-        <c:axId val="183030912"/>
+        <c:axId val="171216256"/>
+        <c:axId val="171214336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="183022720"/>
+        <c:axId val="171206144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -2847,13 +2850,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183024640"/>
+        <c:crossAx val="171208064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="183024640"/>
+        <c:axId val="171208064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2882,12 +2885,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183022720"/>
+        <c:crossAx val="171206144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="183030912"/>
+        <c:axId val="171214336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="540"/>
@@ -2917,13 +2920,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183032832"/>
+        <c:crossAx val="171216256"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="183032832"/>
+        <c:axId val="171216256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2933,7 +2936,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183030912"/>
+        <c:crossAx val="171214336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3112,11 +3115,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="187170816"/>
-        <c:axId val="187172736"/>
+        <c:axId val="169419136"/>
+        <c:axId val="169421056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="187170816"/>
+        <c:axId val="169419136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -3146,13 +3149,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187172736"/>
+        <c:crossAx val="169421056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="187172736"/>
+        <c:axId val="169421056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3181,7 +3184,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187170816"/>
+        <c:crossAx val="169419136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3870,11 +3873,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186104832"/>
-        <c:axId val="186107392"/>
+        <c:axId val="169137664"/>
+        <c:axId val="169476096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186104832"/>
+        <c:axId val="169137664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3916,12 +3919,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186107392"/>
+        <c:crossAx val="169476096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186107392"/>
+        <c:axId val="169476096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -3957,7 +3960,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186104832"/>
+        <c:crossAx val="169137664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -4118,8 +4121,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186161024"/>
-        <c:axId val="186167296"/>
+        <c:axId val="169515264"/>
+        <c:axId val="169521536"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -4211,11 +4214,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186183680"/>
-        <c:axId val="186169216"/>
+        <c:axId val="169533824"/>
+        <c:axId val="169523456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186161024"/>
+        <c:axId val="169515264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4244,12 +4247,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186167296"/>
+        <c:crossAx val="169521536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186167296"/>
+        <c:axId val="169521536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4278,12 +4281,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186161024"/>
+        <c:crossAx val="169515264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186169216"/>
+        <c:axId val="169523456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="270"/>
@@ -4313,13 +4316,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186183680"/>
+        <c:crossAx val="169533824"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186183680"/>
+        <c:axId val="169533824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4329,7 +4332,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186169216"/>
+        <c:crossAx val="169523456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4470,8 +4473,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186198656"/>
-        <c:axId val="186200832"/>
+        <c:axId val="169290752"/>
+        <c:axId val="169292928"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -4594,11 +4597,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186221312"/>
-        <c:axId val="186202752"/>
+        <c:axId val="169309312"/>
+        <c:axId val="169294848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186198656"/>
+        <c:axId val="169290752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -4628,13 +4631,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186200832"/>
+        <c:crossAx val="169292928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186200832"/>
+        <c:axId val="169292928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4663,12 +4666,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186198656"/>
+        <c:crossAx val="169290752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186202752"/>
+        <c:axId val="169294848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="540"/>
@@ -4698,13 +4701,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186221312"/>
+        <c:crossAx val="169309312"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186221312"/>
+        <c:axId val="169309312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4714,7 +4717,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186202752"/>
+        <c:crossAx val="169294848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4893,11 +4896,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186242176"/>
-        <c:axId val="186244096"/>
+        <c:axId val="169330176"/>
+        <c:axId val="169332096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186242176"/>
+        <c:axId val="169330176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -4927,13 +4930,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186244096"/>
+        <c:crossAx val="169332096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186244096"/>
+        <c:axId val="169332096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4962,7 +4965,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186242176"/>
+        <c:crossAx val="169330176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5392,11 +5395,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="186293632"/>
-        <c:axId val="186304384"/>
+        <c:axId val="169252736"/>
+        <c:axId val="169267584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186293632"/>
+        <c:axId val="169252736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5438,12 +5441,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186304384"/>
+        <c:crossAx val="169267584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186304384"/>
+        <c:axId val="169267584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -5479,7 +5482,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186293632"/>
+        <c:crossAx val="169252736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -12607,414 +12610,413 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J31"/>
+  <dimension ref="B1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" customWidth="1"/>
-    <col min="5" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="3" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="54">
         <v>42643</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I3" s="56" t="s">
+    <row r="3" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G3" s="56" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="E4" s="27" t="s">
+    <row r="4" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="D4" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="G4" s="27" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>193</v>
       </c>
-      <c r="E5">
+      <c r="C5">
         <v>24</v>
       </c>
-      <c r="F5">
+      <c r="D5">
         <v>27.6</v>
       </c>
-      <c r="I5">
+      <c r="G5">
         <v>27.6</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>196</v>
       </c>
-      <c r="E6">
+      <c r="C6">
         <v>28.7</v>
       </c>
-      <c r="F6">
+      <c r="D6">
         <v>32.4</v>
       </c>
-      <c r="I6">
+      <c r="G6">
         <v>32.4</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>197</v>
       </c>
-      <c r="E7">
+      <c r="C7">
         <v>21</v>
       </c>
-      <c r="F7">
+      <c r="D7">
         <v>18</v>
       </c>
-      <c r="I7">
+      <c r="G7">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>194</v>
       </c>
-      <c r="E8">
+      <c r="C8">
         <v>42.4</v>
       </c>
-      <c r="F8">
+      <c r="D8">
         <v>40</v>
       </c>
-      <c r="I8">
+      <c r="G8">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>195</v>
       </c>
-      <c r="E9">
+      <c r="C9">
         <v>600</v>
       </c>
-      <c r="F9">
+      <c r="D9">
         <v>359</v>
       </c>
-      <c r="I9">
+      <c r="G9">
         <v>359</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>195</v>
       </c>
-      <c r="E10">
+      <c r="C10">
         <v>210</v>
       </c>
-      <c r="F10">
+      <c r="D10">
         <v>187</v>
       </c>
-      <c r="I10">
-        <f>F10/2</f>
+      <c r="G10">
+        <f>D10/2</f>
         <v>93.5</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>195</v>
       </c>
-      <c r="E11">
+      <c r="C11">
         <v>56</v>
       </c>
-      <c r="F11">
+      <c r="D11">
         <v>123</v>
       </c>
-      <c r="I11">
+      <c r="G11">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>205</v>
       </c>
-      <c r="E12">
+      <c r="C12">
         <v>8</v>
       </c>
-      <c r="F12">
+      <c r="D12">
         <v>14</v>
       </c>
-      <c r="I12">
+      <c r="G12">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>198</v>
       </c>
-      <c r="E13">
+      <c r="C13">
         <v>21.2</v>
       </c>
-      <c r="F13">
+      <c r="D13">
         <v>120</v>
       </c>
-      <c r="I13">
+      <c r="G13">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>199</v>
       </c>
-      <c r="E14">
+      <c r="C14">
         <v>3000</v>
       </c>
-      <c r="F14">
+      <c r="D14">
         <v>15000</v>
       </c>
-      <c r="I14">
+      <c r="G14">
         <v>15000</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>212</v>
       </c>
-      <c r="E15">
+      <c r="C15">
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>200</v>
       </c>
-      <c r="E17">
+      <c r="C17">
         <v>11</v>
       </c>
-      <c r="F17">
+      <c r="D17">
         <v>10</v>
       </c>
-      <c r="I17">
+      <c r="G17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>201</v>
       </c>
-      <c r="E18">
+      <c r="C18">
         <v>308</v>
       </c>
-      <c r="F18">
-        <f>F17*F6</f>
+      <c r="D18">
+        <f>D17*D6</f>
         <v>324</v>
       </c>
-      <c r="I18">
-        <f>I17*I6</f>
+      <c r="G18">
+        <f>G17*G6</f>
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>202</v>
       </c>
-      <c r="E19">
+      <c r="C19">
         <v>262</v>
       </c>
-      <c r="F19">
-        <f>F17*F7</f>
+      <c r="D19">
+        <f>D17*D7</f>
         <v>180</v>
       </c>
-      <c r="I19">
-        <f>I17*I7</f>
+      <c r="G19">
+        <f>G17*G7</f>
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>203</v>
       </c>
-      <c r="E21">
+      <c r="C21">
         <v>200</v>
       </c>
-      <c r="F21">
+      <c r="D21">
         <v>360</v>
       </c>
-      <c r="I21">
+      <c r="G21">
         <v>360</v>
       </c>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>204</v>
       </c>
-      <c r="E22">
+      <c r="C22">
         <v>180</v>
       </c>
-      <c r="F22">
+      <c r="D22">
         <v>375</v>
       </c>
-      <c r="I22">
+      <c r="G22">
         <v>375</v>
       </c>
     </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>206</v>
       </c>
-      <c r="E24">
-        <f>E8*E5</f>
+      <c r="C24">
+        <f>C8*C5</f>
         <v>1017.5999999999999</v>
       </c>
-      <c r="F24">
-        <f>F8*F5</f>
+      <c r="D24">
+        <f>D8*D5</f>
         <v>1104</v>
       </c>
-      <c r="I24">
-        <f>I8*I5</f>
+      <c r="G24">
+        <f>G8*G5</f>
         <v>552</v>
       </c>
     </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>207</v>
       </c>
-      <c r="E25">
-        <f>E17*E24</f>
+      <c r="C25">
+        <f>C17*C24</f>
         <v>11193.599999999999</v>
       </c>
-      <c r="F25">
-        <f>F17*F24</f>
+      <c r="D25">
+        <f>D17*D24</f>
         <v>11040</v>
       </c>
-      <c r="I25">
-        <f>I17*I24</f>
+      <c r="G25">
+        <f>G17*G24</f>
         <v>5520</v>
       </c>
     </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>214</v>
       </c>
-      <c r="E26">
+      <c r="C26">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F26">
+      <c r="D26">
         <v>0.8</v>
       </c>
-      <c r="I26">
+      <c r="G26">
         <v>0.8</v>
       </c>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>213</v>
       </c>
-      <c r="E27">
-        <f>E26*E25</f>
+      <c r="C27">
+        <f>C26*C25</f>
         <v>6156.48</v>
       </c>
-      <c r="F27">
-        <f>F26*F25</f>
+      <c r="D27">
+        <f>D26*D25</f>
         <v>8832</v>
       </c>
-      <c r="I27">
-        <f>I26*I25</f>
+      <c r="G27">
+        <f>G26*G25</f>
         <v>4416</v>
       </c>
-      <c r="J27" s="3">
-        <f>I27/E27</f>
+      <c r="H27" s="3">
+        <f>G27/C27</f>
         <v>0.71729299859660067</v>
       </c>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>215</v>
       </c>
-      <c r="E28">
-        <f>E27*E15*0.9/1000</f>
+      <c r="C28">
+        <f>C27*C15*0.9/1000</f>
         <v>55408.319999999992</v>
       </c>
-      <c r="F28">
-        <f>F27*F14*0.9/1000</f>
+      <c r="D28">
+        <f>D27*D14*0.9/1000</f>
         <v>119232</v>
       </c>
-      <c r="G28" s="3">
-        <f>F28/E28</f>
+      <c r="E28" s="3">
+        <f>D28/C28</f>
         <v>2.1518789957898021</v>
       </c>
-      <c r="I28">
-        <f>I27*I14*0.9/1000</f>
+      <c r="G28">
+        <f>G27*G14*0.9/1000</f>
         <v>59616</v>
       </c>
-      <c r="J28" s="3">
-        <f>I28/E28</f>
+      <c r="H28" s="3">
+        <f>G28/C28</f>
         <v>1.0759394978949011</v>
       </c>
     </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>208</v>
       </c>
-      <c r="E30">
-        <f>E17*E12</f>
+      <c r="C30">
+        <f>C17*C12</f>
         <v>88</v>
       </c>
-      <c r="F30">
-        <f>F17*F12</f>
+      <c r="D30">
+        <f>D17*D12</f>
         <v>140</v>
       </c>
-      <c r="G30" s="3">
-        <f>F30/E30</f>
+      <c r="E30" s="3">
+        <f>D30/C30</f>
         <v>1.5909090909090908</v>
       </c>
-      <c r="I30">
-        <f>I17*I12</f>
+      <c r="G30">
+        <f>G17*G12</f>
         <v>70</v>
       </c>
-      <c r="J30" s="3">
-        <f>I30/E30</f>
+      <c r="H30" s="3">
+        <f>G30/C30</f>
         <v>0.79545454545454541</v>
       </c>
     </row>
-    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>209</v>
       </c>
-      <c r="E31">
-        <f>E17*E9*E10*E11/(1000^3)</f>
+      <c r="C31">
+        <f>C17*C9*C10*C11/(1000^3)</f>
         <v>7.7616000000000004E-2</v>
       </c>
-      <c r="F31">
-        <f>F17*F9*F10*F11/(1000^3)</f>
+      <c r="D31">
+        <f>D17*D9*D10*D11/(1000^3)</f>
         <v>8.2573590000000002E-2</v>
       </c>
-      <c r="G31" s="3">
-        <f>F31/E31</f>
+      <c r="E31" s="3">
+        <f>D31/C31</f>
         <v>1.063873299319728</v>
       </c>
-      <c r="I31">
-        <f>I17*I9*I10*I11/(1000^3)</f>
+      <c r="G31">
+        <f>G17*G9*G10*G11/(1000^3)</f>
         <v>4.1286795000000001E-2</v>
       </c>
-      <c r="J31" s="3">
-        <f>I31/E31</f>
+      <c r="H31" s="3">
+        <f>G31/C31</f>
         <v>0.53193664965986398</v>
       </c>
     </row>

</xml_diff>